<commit_message>
tree measurements for height
</commit_message>
<xml_diff>
--- a/data/treeMeasurements/TreeMeasurements.xlsx
+++ b/data/treeMeasurements/TreeMeasurements.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christophe_rouleau-desrochers/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christophe_rouleau-desrochers/github/fuelinex/data/treeMeasurements/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F635B282-C81B-4F47-953A-FAB6E0305C64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18821697-81D2-C745-9106-EF454B255385}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17200" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="1" r:id="rId1"/>
@@ -21,12 +21,11 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">data!$A$1:$E$631</definedName>
   </definedNames>
   <calcPr calcId="0"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4636" uniqueCount="1437">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4654" uniqueCount="1442">
   <si>
     <t>Metadata for Phenological Monitoring - FUELINEX 2024</t>
   </si>
@@ -4337,6 +4336,21 @@
   </si>
   <si>
     <t>apical shoot died, new lateral shoot measured, lateral shoot where the tag is</t>
+  </si>
+  <si>
+    <t>apical meristem died</t>
+  </si>
+  <si>
+    <t>mark from 2024 buried, therefore new mark, measurement from last year is 39.4</t>
+  </si>
+  <si>
+    <t>apical shoot snapped off</t>
+  </si>
+  <si>
+    <t>no (trunk 2)</t>
+  </si>
+  <si>
+    <t>apical and lateral meristems are dead, lateral shoot measured only has living lateral buds</t>
   </si>
 </sst>
 </file>
@@ -4346,11 +4360,18 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -4414,7 +4435,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4443,6 +4464,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FFE7E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -4489,52 +4516,58 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6456,9 +6489,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:R820"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A575" zoomScale="150" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="I1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="O586" sqref="O586"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="O530" sqref="O530"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6917,6 +6950,9 @@
         <v>14</v>
       </c>
       <c r="K12" s="17"/>
+      <c r="N12" s="14">
+        <v>56.4</v>
+      </c>
     </row>
     <row r="13" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="14" t="s">
@@ -6948,7 +6984,9 @@
       <c r="K13" s="18"/>
       <c r="L13" s="14"/>
       <c r="M13" s="14"/>
-      <c r="N13" s="14"/>
+      <c r="N13" s="19">
+        <v>47</v>
+      </c>
       <c r="O13" s="14"/>
       <c r="P13" s="14"/>
       <c r="Q13" s="14"/>
@@ -6982,6 +7020,9 @@
         <v>14</v>
       </c>
       <c r="K14" s="17"/>
+      <c r="N14" s="20">
+        <v>48</v>
+      </c>
     </row>
     <row r="15" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
@@ -7013,7 +7054,9 @@
       <c r="K15" s="18"/>
       <c r="L15" s="14"/>
       <c r="M15" s="14"/>
-      <c r="N15" s="14"/>
+      <c r="N15">
+        <v>47.9</v>
+      </c>
       <c r="O15" s="14"/>
       <c r="P15" s="14"/>
       <c r="Q15" s="14"/>
@@ -7047,6 +7090,9 @@
         <v>14</v>
       </c>
       <c r="K16" s="17"/>
+      <c r="N16" s="20">
+        <v>52</v>
+      </c>
     </row>
     <row r="17" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="14" t="s">
@@ -7428,7 +7474,9 @@
       <c r="K27" s="18"/>
       <c r="L27" s="14"/>
       <c r="M27" s="14"/>
-      <c r="N27" s="14"/>
+      <c r="N27" s="14">
+        <v>39.4</v>
+      </c>
       <c r="O27" s="14"/>
       <c r="P27" s="14"/>
       <c r="Q27" s="14"/>
@@ -7462,6 +7510,9 @@
         <v>14</v>
       </c>
       <c r="K28" s="17"/>
+      <c r="N28" s="19">
+        <v>72</v>
+      </c>
     </row>
     <row r="29" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="14" t="s">
@@ -7493,11 +7544,15 @@
       <c r="K29" s="18"/>
       <c r="L29" s="14"/>
       <c r="M29" s="14"/>
-      <c r="N29" s="14"/>
+      <c r="N29" s="14">
+        <v>66.400000000000006</v>
+      </c>
       <c r="O29" s="14"/>
       <c r="P29" s="14"/>
       <c r="Q29" s="14"/>
-      <c r="R29" s="14"/>
+      <c r="R29" s="14" t="s">
+        <v>1437</v>
+      </c>
     </row>
     <row r="30" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
@@ -7527,6 +7582,9 @@
         <v>14</v>
       </c>
       <c r="K30" s="17"/>
+      <c r="N30">
+        <v>50.6</v>
+      </c>
     </row>
     <row r="31" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="14" t="s">
@@ -7558,7 +7616,9 @@
       <c r="K31" s="18"/>
       <c r="L31" s="14"/>
       <c r="M31" s="14"/>
-      <c r="N31" s="14"/>
+      <c r="N31" s="14">
+        <v>56.5</v>
+      </c>
       <c r="O31" s="14"/>
       <c r="P31" s="14"/>
       <c r="Q31" s="14"/>
@@ -7942,6 +8002,9 @@
         <v>14</v>
       </c>
       <c r="K42" s="17"/>
+      <c r="N42">
+        <v>51.4</v>
+      </c>
     </row>
     <row r="43" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="14" t="s">
@@ -7973,7 +8036,9 @@
       <c r="K43" s="18"/>
       <c r="L43" s="14"/>
       <c r="M43" s="14"/>
-      <c r="N43" s="14"/>
+      <c r="N43" s="14">
+        <v>27.7</v>
+      </c>
       <c r="O43" s="14"/>
       <c r="P43" s="14"/>
       <c r="Q43" s="14"/>
@@ -8007,6 +8072,9 @@
         <v>14</v>
       </c>
       <c r="K44" s="17"/>
+      <c r="N44">
+        <v>67.099999999999994</v>
+      </c>
     </row>
     <row r="45" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="14" t="s">
@@ -8038,7 +8106,9 @@
       <c r="K45" s="18"/>
       <c r="L45" s="14"/>
       <c r="M45" s="14"/>
-      <c r="N45" s="14"/>
+      <c r="N45" s="14">
+        <v>36.4</v>
+      </c>
       <c r="O45" s="14"/>
       <c r="P45" s="14"/>
       <c r="Q45" s="14"/>
@@ -8072,6 +8142,9 @@
         <v>14</v>
       </c>
       <c r="K46" s="17"/>
+      <c r="N46">
+        <v>46.1</v>
+      </c>
     </row>
     <row r="47" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="14" t="s">
@@ -8453,7 +8526,9 @@
       <c r="K57" s="18"/>
       <c r="L57" s="14"/>
       <c r="M57" s="14"/>
-      <c r="N57" s="14"/>
+      <c r="N57" s="40">
+        <v>49.9</v>
+      </c>
       <c r="O57" s="14"/>
       <c r="P57" s="14"/>
       <c r="Q57" s="14"/>
@@ -8487,6 +8562,9 @@
         <v>14</v>
       </c>
       <c r="K58" s="17"/>
+      <c r="N58" s="41">
+        <v>50</v>
+      </c>
     </row>
     <row r="59" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="14" t="s">
@@ -8518,7 +8596,9 @@
       <c r="K59" s="18"/>
       <c r="L59" s="14"/>
       <c r="M59" s="14"/>
-      <c r="N59" s="14"/>
+      <c r="N59" s="40">
+        <v>52.5</v>
+      </c>
       <c r="O59" s="14"/>
       <c r="P59" s="14"/>
       <c r="Q59" s="14"/>
@@ -8552,6 +8632,9 @@
         <v>14</v>
       </c>
       <c r="K60" s="17"/>
+      <c r="N60" s="40">
+        <v>56.6</v>
+      </c>
     </row>
     <row r="61" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="14" t="s">
@@ -8583,7 +8666,9 @@
       <c r="K61" s="18"/>
       <c r="L61" s="14"/>
       <c r="M61" s="14"/>
-      <c r="N61" s="14"/>
+      <c r="N61" s="40">
+        <v>43.4</v>
+      </c>
       <c r="O61" s="14"/>
       <c r="P61" s="14"/>
       <c r="Q61" s="14"/>
@@ -8967,6 +9052,9 @@
         <v>14</v>
       </c>
       <c r="K72" s="17"/>
+      <c r="N72">
+        <v>59.5</v>
+      </c>
     </row>
     <row r="73" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="14" t="s">
@@ -8998,7 +9086,9 @@
       <c r="K73" s="18"/>
       <c r="L73" s="14"/>
       <c r="M73" s="14"/>
-      <c r="N73" s="14"/>
+      <c r="N73" s="14">
+        <v>46.5</v>
+      </c>
       <c r="O73" s="14"/>
       <c r="P73" s="14"/>
       <c r="Q73" s="14"/>
@@ -9032,6 +9122,9 @@
         <v>14</v>
       </c>
       <c r="K74" s="17"/>
+      <c r="N74">
+        <v>50.9</v>
+      </c>
     </row>
     <row r="75" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="14" t="s">
@@ -9063,7 +9156,9 @@
       <c r="K75" s="18"/>
       <c r="L75" s="14"/>
       <c r="M75" s="14"/>
-      <c r="N75" s="14"/>
+      <c r="N75" s="14">
+        <v>51.5</v>
+      </c>
       <c r="O75" s="14"/>
       <c r="P75" s="14"/>
       <c r="Q75" s="14"/>
@@ -9097,6 +9192,12 @@
         <v>14</v>
       </c>
       <c r="K76" s="17"/>
+      <c r="N76">
+        <v>59.6</v>
+      </c>
+      <c r="R76" s="39" t="s">
+        <v>1438</v>
+      </c>
     </row>
     <row r="77" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="14" t="s">
@@ -9478,7 +9579,9 @@
       <c r="K87" s="18"/>
       <c r="L87" s="14"/>
       <c r="M87" s="14"/>
-      <c r="N87" s="14"/>
+      <c r="N87" s="14">
+        <v>42.5</v>
+      </c>
       <c r="O87" s="14"/>
       <c r="P87" s="14"/>
       <c r="Q87" s="14"/>
@@ -9512,6 +9615,9 @@
         <v>14</v>
       </c>
       <c r="K88" s="17"/>
+      <c r="N88">
+        <v>66.5</v>
+      </c>
     </row>
     <row r="89" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="14" t="s">
@@ -9543,7 +9649,9 @@
       <c r="K89" s="18"/>
       <c r="L89" s="14"/>
       <c r="M89" s="14"/>
-      <c r="N89" s="14"/>
+      <c r="N89" s="14">
+        <v>55.9</v>
+      </c>
       <c r="O89" s="14"/>
       <c r="P89" s="14"/>
       <c r="Q89" s="14"/>
@@ -9577,6 +9685,9 @@
         <v>14</v>
       </c>
       <c r="K90" s="17"/>
+      <c r="N90">
+        <v>43.6</v>
+      </c>
     </row>
     <row r="91" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="14" t="s">
@@ -9608,7 +9719,9 @@
       <c r="K91" s="18"/>
       <c r="L91" s="14"/>
       <c r="M91" s="14"/>
-      <c r="N91" s="14"/>
+      <c r="N91" s="14">
+        <v>71.5</v>
+      </c>
       <c r="O91" s="14"/>
       <c r="P91" s="14"/>
       <c r="Q91" s="14"/>
@@ -13281,6 +13394,9 @@
         <v>414</v>
       </c>
       <c r="K192" s="17"/>
+      <c r="N192">
+        <v>31.8</v>
+      </c>
     </row>
     <row r="193" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A193" s="14" t="s">
@@ -13312,7 +13428,9 @@
       <c r="K193" s="18"/>
       <c r="L193" s="14"/>
       <c r="M193" s="14"/>
-      <c r="N193" s="14"/>
+      <c r="N193" s="14">
+        <v>22.7</v>
+      </c>
       <c r="O193" s="14"/>
       <c r="P193" s="14"/>
       <c r="Q193" s="14"/>
@@ -13346,6 +13464,9 @@
         <v>414</v>
       </c>
       <c r="K194" s="17"/>
+      <c r="N194">
+        <v>29.5</v>
+      </c>
     </row>
     <row r="195" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A195" s="14" t="s">
@@ -13377,7 +13498,9 @@
       <c r="K195" s="18"/>
       <c r="L195" s="14"/>
       <c r="M195" s="14"/>
-      <c r="N195" s="14"/>
+      <c r="N195" s="20">
+        <v>13</v>
+      </c>
       <c r="O195" s="14"/>
       <c r="P195" s="14"/>
       <c r="Q195" s="14"/>
@@ -13411,6 +13534,9 @@
         <v>414</v>
       </c>
       <c r="K196" s="17"/>
+      <c r="N196">
+        <v>42.9</v>
+      </c>
     </row>
     <row r="197" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A197" s="14" t="s">
@@ -13792,7 +13918,9 @@
       <c r="K207" s="18"/>
       <c r="L207" s="14"/>
       <c r="M207" s="14"/>
-      <c r="N207" s="14"/>
+      <c r="N207" s="14">
+        <v>17.8</v>
+      </c>
       <c r="O207" s="14"/>
       <c r="P207" s="14"/>
       <c r="Q207" s="14"/>
@@ -13826,6 +13954,9 @@
         <v>414</v>
       </c>
       <c r="K208" s="17"/>
+      <c r="N208">
+        <v>32.5</v>
+      </c>
     </row>
     <row r="209" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A209" s="14" t="s">
@@ -13857,7 +13988,9 @@
       <c r="K209" s="18"/>
       <c r="L209" s="14"/>
       <c r="M209" s="14"/>
-      <c r="N209" s="14"/>
+      <c r="N209" s="14">
+        <v>23.9</v>
+      </c>
       <c r="O209" s="14"/>
       <c r="P209" s="14"/>
       <c r="Q209" s="14"/>
@@ -13891,6 +14024,9 @@
         <v>414</v>
       </c>
       <c r="K210" s="17"/>
+      <c r="N210" s="19">
+        <v>41</v>
+      </c>
     </row>
     <row r="211" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A211" s="14" t="s">
@@ -13922,7 +14058,9 @@
       <c r="K211" s="18"/>
       <c r="L211" s="14"/>
       <c r="M211" s="14"/>
-      <c r="N211" s="14"/>
+      <c r="N211" s="14">
+        <v>31.7</v>
+      </c>
       <c r="O211" s="14"/>
       <c r="P211" s="14"/>
       <c r="Q211" s="14"/>
@@ -14306,6 +14444,9 @@
         <v>414</v>
       </c>
       <c r="K222" s="17"/>
+      <c r="N222">
+        <v>30.4</v>
+      </c>
     </row>
     <row r="223" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A223" s="14" t="s">
@@ -14337,7 +14478,9 @@
       <c r="K223" s="18"/>
       <c r="L223" s="14"/>
       <c r="M223" s="14"/>
-      <c r="N223" s="14"/>
+      <c r="N223" s="14">
+        <v>31.2</v>
+      </c>
       <c r="O223" s="14"/>
       <c r="P223" s="14"/>
       <c r="Q223" s="14"/>
@@ -14371,6 +14514,9 @@
         <v>414</v>
       </c>
       <c r="K224" s="17"/>
+      <c r="N224">
+        <v>29.3</v>
+      </c>
     </row>
     <row r="225" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A225" s="14" t="s">
@@ -14402,7 +14548,9 @@
       <c r="K225" s="18"/>
       <c r="L225" s="14"/>
       <c r="M225" s="14"/>
-      <c r="N225" s="14"/>
+      <c r="N225" s="14">
+        <v>25.4</v>
+      </c>
       <c r="O225" s="14"/>
       <c r="P225" s="14"/>
       <c r="Q225" s="14"/>
@@ -14436,6 +14584,9 @@
         <v>414</v>
       </c>
       <c r="K226" s="17"/>
+      <c r="N226">
+        <v>20.8</v>
+      </c>
     </row>
     <row r="227" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A227" s="14" t="s">
@@ -14817,7 +14968,9 @@
       <c r="K237" s="18"/>
       <c r="L237" s="14"/>
       <c r="M237" s="14"/>
-      <c r="N237" s="14"/>
+      <c r="N237" s="20">
+        <v>25</v>
+      </c>
       <c r="O237" s="14"/>
       <c r="P237" s="14"/>
       <c r="Q237" s="14"/>
@@ -14851,6 +15004,9 @@
         <v>414</v>
       </c>
       <c r="K238" s="17"/>
+      <c r="N238">
+        <v>37.9</v>
+      </c>
     </row>
     <row r="239" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A239" s="14" t="s">
@@ -14882,7 +15038,9 @@
       <c r="K239" s="18"/>
       <c r="L239" s="14"/>
       <c r="M239" s="14"/>
-      <c r="N239" s="14"/>
+      <c r="N239" s="14">
+        <v>38.200000000000003</v>
+      </c>
       <c r="O239" s="14"/>
       <c r="P239" s="14"/>
       <c r="Q239" s="14"/>
@@ -14916,6 +15074,9 @@
         <v>414</v>
       </c>
       <c r="K240" s="17"/>
+      <c r="N240">
+        <v>27.9</v>
+      </c>
     </row>
     <row r="241" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A241" s="14" t="s">
@@ -14947,7 +15108,9 @@
       <c r="K241" s="18"/>
       <c r="L241" s="14"/>
       <c r="M241" s="14"/>
-      <c r="N241" s="14"/>
+      <c r="N241" s="14">
+        <v>32.700000000000003</v>
+      </c>
       <c r="O241" s="14"/>
       <c r="P241" s="14"/>
       <c r="Q241" s="14"/>
@@ -15333,6 +15496,9 @@
         <v>414</v>
       </c>
       <c r="K252" s="17"/>
+      <c r="N252">
+        <v>23.7</v>
+      </c>
     </row>
     <row r="253" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A253" s="14" t="s">
@@ -15364,7 +15530,9 @@
       <c r="K253" s="18"/>
       <c r="L253" s="14"/>
       <c r="M253" s="14"/>
-      <c r="N253" s="14"/>
+      <c r="N253" s="14">
+        <v>36.4</v>
+      </c>
       <c r="O253" s="14"/>
       <c r="P253" s="14"/>
       <c r="Q253" s="14"/>
@@ -15398,6 +15566,9 @@
         <v>414</v>
       </c>
       <c r="K254" s="17"/>
+      <c r="N254">
+        <v>29.5</v>
+      </c>
     </row>
     <row r="255" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A255" s="14" t="s">
@@ -15429,7 +15600,9 @@
       <c r="K255" s="18"/>
       <c r="L255" s="14"/>
       <c r="M255" s="14"/>
-      <c r="N255" s="14"/>
+      <c r="N255" s="14">
+        <v>28.2</v>
+      </c>
       <c r="O255" s="14"/>
       <c r="P255" s="14"/>
       <c r="Q255" s="14"/>
@@ -15463,6 +15636,9 @@
         <v>414</v>
       </c>
       <c r="K256" s="17"/>
+      <c r="N256" s="37">
+        <v>25</v>
+      </c>
     </row>
     <row r="257" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A257" s="14" t="s">
@@ -15844,7 +16020,9 @@
       <c r="K267" s="18"/>
       <c r="L267" s="14"/>
       <c r="M267" s="14"/>
-      <c r="N267" s="14"/>
+      <c r="N267" s="14">
+        <v>31.8</v>
+      </c>
       <c r="O267" s="14"/>
       <c r="P267" s="14"/>
       <c r="Q267" s="14"/>
@@ -15878,6 +16056,9 @@
         <v>414</v>
       </c>
       <c r="K268" s="17"/>
+      <c r="N268" s="19">
+        <v>30</v>
+      </c>
     </row>
     <row r="269" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A269" s="14" t="s">
@@ -15909,7 +16090,9 @@
       <c r="K269" s="18"/>
       <c r="L269" s="14"/>
       <c r="M269" s="14"/>
-      <c r="N269" s="14"/>
+      <c r="N269" s="14">
+        <v>25.6</v>
+      </c>
       <c r="O269" s="14"/>
       <c r="P269" s="14"/>
       <c r="Q269" s="14"/>
@@ -15943,6 +16126,9 @@
         <v>414</v>
       </c>
       <c r="K270" s="17"/>
+      <c r="N270">
+        <v>33.4</v>
+      </c>
     </row>
     <row r="271" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A271" s="14" t="s">
@@ -15974,7 +16160,9 @@
       <c r="K271" s="18"/>
       <c r="L271" s="14"/>
       <c r="M271" s="14"/>
-      <c r="N271" s="14"/>
+      <c r="N271" s="14">
+        <v>17.100000000000001</v>
+      </c>
       <c r="O271" s="14"/>
       <c r="P271" s="14"/>
       <c r="Q271" s="14"/>
@@ -16366,6 +16554,12 @@
         <v>325</v>
       </c>
       <c r="K282" s="17"/>
+      <c r="Q282" s="38" t="s">
+        <v>1424</v>
+      </c>
+      <c r="R282" s="34" t="s">
+        <v>1434</v>
+      </c>
     </row>
     <row r="283" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A283" s="14" t="s">
@@ -16397,11 +16591,15 @@
       <c r="K283" s="18"/>
       <c r="L283" s="14"/>
       <c r="M283" s="14"/>
-      <c r="N283" s="14"/>
+      <c r="N283" s="14" t="s">
+        <v>1396</v>
+      </c>
       <c r="O283" s="14"/>
       <c r="P283" s="14"/>
       <c r="Q283" s="14"/>
-      <c r="R283" s="14"/>
+      <c r="R283" s="14" t="s">
+        <v>1401</v>
+      </c>
     </row>
     <row r="284" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A284" s="4" t="s">
@@ -16431,6 +16629,9 @@
         <v>325</v>
       </c>
       <c r="K284" s="17"/>
+      <c r="N284">
+        <v>39.299999999999997</v>
+      </c>
     </row>
     <row r="285" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A285" s="14" t="s">
@@ -16462,7 +16663,9 @@
       <c r="K285" s="18"/>
       <c r="L285" s="14"/>
       <c r="M285" s="14"/>
-      <c r="N285" s="14"/>
+      <c r="N285" s="14">
+        <v>32.5</v>
+      </c>
       <c r="O285" s="14"/>
       <c r="P285" s="14"/>
       <c r="Q285" s="14"/>
@@ -16496,6 +16699,9 @@
         <v>325</v>
       </c>
       <c r="K286" s="17"/>
+      <c r="N286">
+        <v>63.2</v>
+      </c>
     </row>
     <row r="287" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A287" s="14" t="s">
@@ -16883,7 +17089,9 @@
       <c r="K297" s="18"/>
       <c r="L297" s="14"/>
       <c r="M297" s="14"/>
-      <c r="N297" s="14"/>
+      <c r="N297" s="14">
+        <v>65.5</v>
+      </c>
       <c r="O297" s="14"/>
       <c r="P297" s="14"/>
       <c r="Q297" s="14"/>
@@ -16917,6 +17125,9 @@
         <v>325</v>
       </c>
       <c r="K298" s="17"/>
+      <c r="N298">
+        <v>63.9</v>
+      </c>
     </row>
     <row r="299" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A299" s="14" t="s">
@@ -16948,7 +17159,9 @@
       <c r="K299" s="18"/>
       <c r="L299" s="14"/>
       <c r="M299" s="14"/>
-      <c r="N299" s="14"/>
+      <c r="N299" s="14">
+        <v>37.6</v>
+      </c>
       <c r="O299" s="14"/>
       <c r="P299" s="14"/>
       <c r="Q299" s="14"/>
@@ -16982,6 +17195,9 @@
         <v>325</v>
       </c>
       <c r="K300" s="17"/>
+      <c r="N300">
+        <v>39.299999999999997</v>
+      </c>
     </row>
     <row r="301" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A301" s="14" t="s">
@@ -17013,11 +17229,17 @@
       <c r="K301" s="18"/>
       <c r="L301" s="14"/>
       <c r="M301" s="14"/>
-      <c r="N301" s="14"/>
+      <c r="N301" s="14">
+        <v>38.4</v>
+      </c>
       <c r="O301" s="14"/>
       <c r="P301" s="14"/>
-      <c r="Q301" s="14"/>
-      <c r="R301" s="14"/>
+      <c r="Q301" s="14" t="s">
+        <v>1424</v>
+      </c>
+      <c r="R301" s="14" t="s">
+        <v>1441</v>
+      </c>
     </row>
     <row r="302" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A302" s="4" t="s">
@@ -17397,6 +17619,9 @@
         <v>325</v>
       </c>
       <c r="K312" s="17"/>
+      <c r="N312">
+        <v>47.2</v>
+      </c>
     </row>
     <row r="313" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A313" s="14" t="s">
@@ -17428,7 +17653,9 @@
       <c r="K313" s="18"/>
       <c r="L313" s="14"/>
       <c r="M313" s="14"/>
-      <c r="N313" s="14"/>
+      <c r="N313" s="14">
+        <v>60.9</v>
+      </c>
       <c r="O313" s="14"/>
       <c r="P313" s="14"/>
       <c r="Q313" s="14"/>
@@ -17462,6 +17689,9 @@
         <v>325</v>
       </c>
       <c r="K314" s="17"/>
+      <c r="N314">
+        <v>50.9</v>
+      </c>
     </row>
     <row r="315" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A315" s="14" t="s">
@@ -17493,7 +17723,9 @@
       <c r="K315" s="18"/>
       <c r="L315" s="14"/>
       <c r="M315" s="14"/>
-      <c r="N315" s="14"/>
+      <c r="N315" s="14">
+        <v>57.4</v>
+      </c>
       <c r="O315" s="14"/>
       <c r="P315" s="14"/>
       <c r="Q315" s="14"/>
@@ -17527,6 +17759,9 @@
         <v>325</v>
       </c>
       <c r="K316" s="17"/>
+      <c r="N316">
+        <v>64.599999999999994</v>
+      </c>
     </row>
     <row r="317" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A317" s="14" t="s">
@@ -17908,7 +18143,9 @@
       <c r="K327" s="18"/>
       <c r="L327" s="14"/>
       <c r="M327" s="14"/>
-      <c r="N327" s="14"/>
+      <c r="N327" s="14">
+        <v>21.5</v>
+      </c>
       <c r="O327" s="14"/>
       <c r="P327" s="14"/>
       <c r="Q327" s="14"/>
@@ -17942,6 +18179,12 @@
         <v>325</v>
       </c>
       <c r="K328" s="17"/>
+      <c r="N328">
+        <v>28.9</v>
+      </c>
+      <c r="R328" s="38" t="s">
+        <v>1426</v>
+      </c>
     </row>
     <row r="329" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A329" s="14" t="s">
@@ -17973,7 +18216,9 @@
       <c r="K329" s="18"/>
       <c r="L329" s="14"/>
       <c r="M329" s="14"/>
-      <c r="N329" s="14"/>
+      <c r="N329" s="14">
+        <v>56.2</v>
+      </c>
       <c r="O329" s="14"/>
       <c r="P329" s="14"/>
       <c r="Q329" s="14"/>
@@ -18007,6 +18252,9 @@
         <v>325</v>
       </c>
       <c r="K330" s="17"/>
+      <c r="N330">
+        <v>32.200000000000003</v>
+      </c>
     </row>
     <row r="331" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A331" s="14" t="s">
@@ -18038,7 +18286,9 @@
       <c r="K331" s="18"/>
       <c r="L331" s="14"/>
       <c r="M331" s="14"/>
-      <c r="N331" s="14"/>
+      <c r="N331" s="14">
+        <v>43.3</v>
+      </c>
       <c r="O331" s="14"/>
       <c r="P331" s="14"/>
       <c r="Q331" s="14"/>
@@ -18422,6 +18672,9 @@
         <v>325</v>
       </c>
       <c r="K342" s="17"/>
+      <c r="N342">
+        <v>44.4</v>
+      </c>
     </row>
     <row r="343" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A343" s="14" t="s">
@@ -18453,7 +18706,9 @@
       <c r="K343" s="18"/>
       <c r="L343" s="14"/>
       <c r="M343" s="14"/>
-      <c r="N343" s="14"/>
+      <c r="N343" s="14">
+        <v>59.6</v>
+      </c>
       <c r="O343" s="14"/>
       <c r="P343" s="14"/>
       <c r="Q343" s="14"/>
@@ -18487,6 +18742,9 @@
         <v>325</v>
       </c>
       <c r="K344" s="17"/>
+      <c r="N344">
+        <v>36.5</v>
+      </c>
     </row>
     <row r="345" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A345" s="14" t="s">
@@ -18518,11 +18776,13 @@
       <c r="K345" s="18"/>
       <c r="L345" s="14"/>
       <c r="M345" s="14"/>
-      <c r="N345" s="14"/>
+      <c r="N345" s="14">
+        <v>55.2</v>
+      </c>
       <c r="O345" s="14"/>
       <c r="P345" s="14"/>
       <c r="Q345" s="14"/>
-      <c r="R345" s="14"/>
+      <c r="R345" s="42"/>
     </row>
     <row r="346" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A346" s="4" t="s">
@@ -18552,6 +18812,12 @@
         <v>325</v>
       </c>
       <c r="K346" s="17"/>
+      <c r="Q346" s="38" t="s">
+        <v>1424</v>
+      </c>
+      <c r="R346" s="34" t="s">
+        <v>1434</v>
+      </c>
     </row>
     <row r="347" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A347" s="14" t="s">
@@ -18936,7 +19202,9 @@
       <c r="K357" s="18"/>
       <c r="L357" s="14"/>
       <c r="M357" s="14"/>
-      <c r="N357" s="14"/>
+      <c r="N357" s="14">
+        <v>31.5</v>
+      </c>
       <c r="O357" s="14"/>
       <c r="P357" s="14"/>
       <c r="Q357" s="14"/>
@@ -18970,6 +19238,9 @@
         <v>325</v>
       </c>
       <c r="K358" s="17"/>
+      <c r="N358">
+        <v>37.4</v>
+      </c>
     </row>
     <row r="359" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A359" s="14" t="s">
@@ -19001,7 +19272,9 @@
       <c r="K359" s="18"/>
       <c r="L359" s="14"/>
       <c r="M359" s="14"/>
-      <c r="N359" s="14"/>
+      <c r="N359" s="14">
+        <v>40.5</v>
+      </c>
       <c r="O359" s="14"/>
       <c r="P359" s="14"/>
       <c r="Q359" s="14"/>
@@ -19035,6 +19308,9 @@
         <v>325</v>
       </c>
       <c r="K360" s="17"/>
+      <c r="N360" s="19">
+        <v>62</v>
+      </c>
     </row>
     <row r="361" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A361" s="14" t="s">
@@ -19066,7 +19342,9 @@
       <c r="K361" s="18"/>
       <c r="L361" s="14"/>
       <c r="M361" s="14"/>
-      <c r="N361" s="14"/>
+      <c r="N361" s="14">
+        <v>60.4</v>
+      </c>
       <c r="O361" s="14"/>
       <c r="P361" s="14"/>
       <c r="Q361" s="14"/>
@@ -22357,6 +22635,9 @@
         <v>325</v>
       </c>
       <c r="K452" s="17"/>
+      <c r="N452">
+        <v>27.2</v>
+      </c>
     </row>
     <row r="453" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A453" s="14" t="s">
@@ -22388,7 +22669,9 @@
       <c r="K453" s="18"/>
       <c r="L453" s="14"/>
       <c r="M453" s="14"/>
-      <c r="N453" s="14"/>
+      <c r="N453" s="14">
+        <v>27.8</v>
+      </c>
       <c r="O453" s="14"/>
       <c r="P453" s="14"/>
       <c r="Q453" s="14"/>
@@ -22422,6 +22705,9 @@
         <v>325</v>
       </c>
       <c r="K454" s="17"/>
+      <c r="N454">
+        <v>31.1</v>
+      </c>
     </row>
     <row r="455" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A455" s="14" t="s">
@@ -22453,7 +22739,9 @@
       <c r="K455" s="18"/>
       <c r="L455" s="14"/>
       <c r="M455" s="14"/>
-      <c r="N455" s="14"/>
+      <c r="N455" s="14">
+        <v>39.1</v>
+      </c>
       <c r="O455" s="14"/>
       <c r="P455" s="14"/>
       <c r="Q455" s="14"/>
@@ -22487,6 +22775,9 @@
         <v>325</v>
       </c>
       <c r="K456" s="17"/>
+      <c r="N456">
+        <v>23.3</v>
+      </c>
     </row>
     <row r="457" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A457" s="14" t="s">
@@ -22694,6 +22985,15 @@
         <v>325</v>
       </c>
       <c r="K462" s="17"/>
+      <c r="N462" s="19">
+        <v>24</v>
+      </c>
+      <c r="Q462" s="38" t="s">
+        <v>1424</v>
+      </c>
+      <c r="R462" s="38" t="s">
+        <v>1433</v>
+      </c>
     </row>
     <row r="463" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A463" s="14" t="s">
@@ -22725,7 +23025,9 @@
       <c r="K463" s="18"/>
       <c r="L463" s="14"/>
       <c r="M463" s="14"/>
-      <c r="N463" s="14"/>
+      <c r="N463" s="20">
+        <v>43</v>
+      </c>
       <c r="O463" s="14"/>
       <c r="P463" s="14"/>
       <c r="Q463" s="14"/>
@@ -22759,6 +23061,9 @@
         <v>325</v>
       </c>
       <c r="K464" s="17"/>
+      <c r="N464">
+        <v>48.6</v>
+      </c>
     </row>
     <row r="465" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A465" s="14" t="s">
@@ -22790,7 +23095,9 @@
       <c r="K465" s="18"/>
       <c r="L465" s="14"/>
       <c r="M465" s="14"/>
-      <c r="N465" s="14"/>
+      <c r="N465" s="14">
+        <v>21.9</v>
+      </c>
       <c r="O465" s="14"/>
       <c r="P465" s="14"/>
       <c r="Q465" s="14"/>
@@ -22824,6 +23131,9 @@
         <v>325</v>
       </c>
       <c r="K466" s="17"/>
+      <c r="N466">
+        <v>33.9</v>
+      </c>
     </row>
     <row r="467" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A467" s="14" t="s">
@@ -22855,7 +23165,9 @@
       <c r="K467" s="18"/>
       <c r="L467" s="14"/>
       <c r="M467" s="14"/>
-      <c r="N467" s="14"/>
+      <c r="N467" s="14">
+        <v>28.9</v>
+      </c>
       <c r="O467" s="14"/>
       <c r="P467" s="14"/>
       <c r="Q467" s="14"/>
@@ -22889,6 +23201,9 @@
         <v>325</v>
       </c>
       <c r="K468" s="17"/>
+      <c r="N468" s="19">
+        <v>32</v>
+      </c>
     </row>
     <row r="469" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A469" s="14" t="s">
@@ -22920,7 +23235,9 @@
       <c r="K469" s="18"/>
       <c r="L469" s="14"/>
       <c r="M469" s="14"/>
-      <c r="N469" s="14"/>
+      <c r="N469" s="14">
+        <v>25.1</v>
+      </c>
       <c r="O469" s="14"/>
       <c r="P469" s="14"/>
       <c r="Q469" s="14"/>
@@ -22954,6 +23271,9 @@
         <v>325</v>
       </c>
       <c r="K470" s="17"/>
+      <c r="N470">
+        <v>19.8</v>
+      </c>
     </row>
     <row r="471" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A471" s="14" t="s">
@@ -22985,7 +23305,9 @@
       <c r="K471" s="18"/>
       <c r="L471" s="14"/>
       <c r="M471" s="14"/>
-      <c r="N471" s="14"/>
+      <c r="N471" s="14">
+        <v>26.7</v>
+      </c>
       <c r="O471" s="14"/>
       <c r="P471" s="14"/>
       <c r="Q471" s="14"/>
@@ -23193,7 +23515,9 @@
       <c r="K477" s="18"/>
       <c r="L477" s="14"/>
       <c r="M477" s="14"/>
-      <c r="N477" s="14"/>
+      <c r="N477" s="14">
+        <v>24.6</v>
+      </c>
       <c r="O477" s="14"/>
       <c r="P477" s="14"/>
       <c r="Q477" s="14"/>
@@ -23227,6 +23551,9 @@
         <v>325</v>
       </c>
       <c r="K478" s="17"/>
+      <c r="N478">
+        <v>27.9</v>
+      </c>
     </row>
     <row r="479" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A479" s="14" t="s">
@@ -23258,7 +23585,9 @@
       <c r="K479" s="18"/>
       <c r="L479" s="14"/>
       <c r="M479" s="14"/>
-      <c r="N479" s="14"/>
+      <c r="N479" s="14">
+        <v>33.4</v>
+      </c>
       <c r="O479" s="14"/>
       <c r="P479" s="14"/>
       <c r="Q479" s="14"/>
@@ -23292,6 +23621,9 @@
         <v>325</v>
       </c>
       <c r="K480" s="17"/>
+      <c r="N480">
+        <v>28.4</v>
+      </c>
     </row>
     <row r="481" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A481" s="14" t="s">
@@ -23323,7 +23655,9 @@
       <c r="K481" s="18"/>
       <c r="L481" s="14"/>
       <c r="M481" s="14"/>
-      <c r="N481" s="14"/>
+      <c r="N481" s="14">
+        <v>27.1</v>
+      </c>
       <c r="O481" s="14"/>
       <c r="P481" s="14"/>
       <c r="Q481" s="14"/>
@@ -23357,6 +23691,9 @@
         <v>325</v>
       </c>
       <c r="K482" s="17"/>
+      <c r="N482">
+        <v>34.299999999999997</v>
+      </c>
     </row>
     <row r="483" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A483" s="14" t="s">
@@ -23388,7 +23725,9 @@
       <c r="K483" s="18"/>
       <c r="L483" s="14"/>
       <c r="M483" s="14"/>
-      <c r="N483" s="14"/>
+      <c r="N483" s="14">
+        <v>37.200000000000003</v>
+      </c>
       <c r="O483" s="14"/>
       <c r="P483" s="14"/>
       <c r="Q483" s="14"/>
@@ -23422,6 +23761,9 @@
         <v>325</v>
       </c>
       <c r="K484" s="17"/>
+      <c r="N484">
+        <v>25.4</v>
+      </c>
     </row>
     <row r="485" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A485" s="14" t="s">
@@ -23453,7 +23795,9 @@
       <c r="K485" s="18"/>
       <c r="L485" s="14"/>
       <c r="M485" s="14"/>
-      <c r="N485" s="14"/>
+      <c r="N485" s="14">
+        <v>34.5</v>
+      </c>
       <c r="O485" s="14"/>
       <c r="P485" s="14"/>
       <c r="Q485" s="14"/>
@@ -23487,6 +23831,9 @@
         <v>325</v>
       </c>
       <c r="K486" s="17"/>
+      <c r="N486">
+        <v>23.1</v>
+      </c>
     </row>
     <row r="487" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A487" s="14" t="s">
@@ -23694,6 +24041,9 @@
         <v>325</v>
       </c>
       <c r="K492" s="17"/>
+      <c r="N492">
+        <v>21.6</v>
+      </c>
     </row>
     <row r="493" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A493" s="14" t="s">
@@ -23725,7 +24075,9 @@
       <c r="K493" s="18"/>
       <c r="L493" s="14"/>
       <c r="M493" s="14"/>
-      <c r="N493" s="14"/>
+      <c r="N493" s="20">
+        <v>35</v>
+      </c>
       <c r="O493" s="14"/>
       <c r="P493" s="14"/>
       <c r="Q493" s="14"/>
@@ -23759,6 +24111,12 @@
         <v>325</v>
       </c>
       <c r="K494" s="17"/>
+      <c r="N494">
+        <v>24.9</v>
+      </c>
+      <c r="R494" s="38" t="s">
+        <v>1439</v>
+      </c>
     </row>
     <row r="495" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A495" s="14" t="s">
@@ -23790,11 +24148,15 @@
       <c r="K495" s="18"/>
       <c r="L495" s="14"/>
       <c r="M495" s="14"/>
-      <c r="N495" s="14"/>
+      <c r="N495" s="14" t="s">
+        <v>1396</v>
+      </c>
       <c r="O495" s="14"/>
       <c r="P495" s="14"/>
       <c r="Q495" s="14"/>
-      <c r="R495" s="14"/>
+      <c r="R495" s="14" t="s">
+        <v>1401</v>
+      </c>
     </row>
     <row r="496" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A496" s="4" t="s">
@@ -23824,6 +24186,9 @@
         <v>325</v>
       </c>
       <c r="K496" s="17"/>
+      <c r="N496">
+        <v>30.9</v>
+      </c>
     </row>
     <row r="497" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A497" s="14" t="s">
@@ -23855,7 +24220,9 @@
       <c r="K497" s="18"/>
       <c r="L497" s="14"/>
       <c r="M497" s="14"/>
-      <c r="N497" s="14"/>
+      <c r="N497" s="14">
+        <v>30.1</v>
+      </c>
       <c r="O497" s="14"/>
       <c r="P497" s="14"/>
       <c r="Q497" s="14"/>
@@ -23889,6 +24256,9 @@
         <v>325</v>
       </c>
       <c r="K498" s="17"/>
+      <c r="N498">
+        <v>37.799999999999997</v>
+      </c>
     </row>
     <row r="499" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A499" s="14" t="s">
@@ -23920,7 +24290,9 @@
       <c r="K499" s="18"/>
       <c r="L499" s="14"/>
       <c r="M499" s="14"/>
-      <c r="N499" s="14"/>
+      <c r="N499" s="20">
+        <v>29</v>
+      </c>
       <c r="O499" s="14"/>
       <c r="P499" s="14"/>
       <c r="Q499" s="14"/>
@@ -23954,6 +24326,9 @@
         <v>325</v>
       </c>
       <c r="K500" s="17"/>
+      <c r="N500">
+        <v>39.299999999999997</v>
+      </c>
     </row>
     <row r="501" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A501" s="14" t="s">
@@ -23985,7 +24360,9 @@
       <c r="K501" s="18"/>
       <c r="L501" s="14"/>
       <c r="M501" s="14"/>
-      <c r="N501" s="14"/>
+      <c r="N501" s="14">
+        <v>31.1</v>
+      </c>
       <c r="O501" s="14"/>
       <c r="P501" s="14"/>
       <c r="Q501" s="14"/>
@@ -24200,7 +24577,9 @@
       <c r="K507" s="18"/>
       <c r="L507" s="14"/>
       <c r="M507" s="14"/>
-      <c r="N507" s="14"/>
+      <c r="N507" s="14">
+        <v>33.799999999999997</v>
+      </c>
       <c r="O507" s="14"/>
       <c r="P507" s="14"/>
       <c r="Q507" s="14"/>
@@ -24234,6 +24613,9 @@
         <v>325</v>
       </c>
       <c r="K508" s="17"/>
+      <c r="N508">
+        <v>25.3</v>
+      </c>
     </row>
     <row r="509" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A509" s="14" t="s">
@@ -24265,7 +24647,9 @@
       <c r="K509" s="18"/>
       <c r="L509" s="14"/>
       <c r="M509" s="14"/>
-      <c r="N509" s="14"/>
+      <c r="N509" s="14">
+        <v>34.1</v>
+      </c>
       <c r="O509" s="14"/>
       <c r="P509" s="14"/>
       <c r="Q509" s="14"/>
@@ -24303,6 +24687,18 @@
         <v>325</v>
       </c>
       <c r="K510" s="17"/>
+      <c r="N510">
+        <v>18.899999999999999</v>
+      </c>
+      <c r="O510">
+        <v>21.5</v>
+      </c>
+      <c r="Q510" s="38" t="s">
+        <v>1440</v>
+      </c>
+      <c r="R510" s="38" t="s">
+        <v>1433</v>
+      </c>
     </row>
     <row r="511" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A511" s="14" t="s">
@@ -24334,7 +24730,9 @@
       <c r="K511" s="18"/>
       <c r="L511" s="14"/>
       <c r="M511" s="14"/>
-      <c r="N511" s="14"/>
+      <c r="N511" s="14">
+        <v>26.6</v>
+      </c>
       <c r="O511" s="14"/>
       <c r="P511" s="14"/>
       <c r="Q511" s="14"/>
@@ -24368,6 +24766,9 @@
         <v>325</v>
       </c>
       <c r="K512" s="17"/>
+      <c r="N512">
+        <v>23.7</v>
+      </c>
     </row>
     <row r="513" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A513" s="14" t="s">
@@ -24399,7 +24800,9 @@
       <c r="K513" s="18"/>
       <c r="L513" s="14"/>
       <c r="M513" s="14"/>
-      <c r="N513" s="14"/>
+      <c r="N513" s="14">
+        <v>31.2</v>
+      </c>
       <c r="O513" s="14"/>
       <c r="P513" s="14"/>
       <c r="Q513" s="14"/>
@@ -24433,6 +24836,9 @@
         <v>325</v>
       </c>
       <c r="K514" s="17"/>
+      <c r="N514">
+        <v>37.4</v>
+      </c>
     </row>
     <row r="515" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A515" s="14" t="s">
@@ -24464,7 +24870,9 @@
       <c r="K515" s="18"/>
       <c r="L515" s="14"/>
       <c r="M515" s="14"/>
-      <c r="N515" s="14"/>
+      <c r="N515" s="14">
+        <v>28.4</v>
+      </c>
       <c r="O515" s="14"/>
       <c r="P515" s="14"/>
       <c r="Q515" s="14"/>
@@ -24498,6 +24906,9 @@
         <v>325</v>
       </c>
       <c r="K516" s="17"/>
+      <c r="N516">
+        <v>31.8</v>
+      </c>
     </row>
     <row r="517" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A517" s="14" t="s">
@@ -24718,6 +25129,9 @@
         <v>325</v>
       </c>
       <c r="K522" s="17"/>
+      <c r="N522">
+        <v>24.8</v>
+      </c>
     </row>
     <row r="523" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A523" s="14" t="s">
@@ -24749,7 +25163,9 @@
       <c r="K523" s="18"/>
       <c r="L523" s="14"/>
       <c r="M523" s="14"/>
-      <c r="N523" s="14"/>
+      <c r="N523" s="14">
+        <v>26.9</v>
+      </c>
       <c r="O523" s="14"/>
       <c r="P523" s="14"/>
       <c r="Q523" s="14"/>
@@ -24783,6 +25199,9 @@
         <v>325</v>
       </c>
       <c r="K524" s="17"/>
+      <c r="N524">
+        <v>26.4</v>
+      </c>
     </row>
     <row r="525" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A525" s="14" t="s">
@@ -24814,7 +25233,9 @@
       <c r="K525" s="18"/>
       <c r="L525" s="14"/>
       <c r="M525" s="14"/>
-      <c r="N525" s="14"/>
+      <c r="N525" s="14">
+        <v>38.1</v>
+      </c>
       <c r="O525" s="14"/>
       <c r="P525" s="14"/>
       <c r="Q525" s="14"/>
@@ -24850,6 +25271,9 @@
       <c r="K526" s="4" t="s">
         <v>1249</v>
       </c>
+      <c r="N526">
+        <v>41.6</v>
+      </c>
       <c r="R526" s="26"/>
     </row>
     <row r="527" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -24882,7 +25306,9 @@
       <c r="K527" s="18"/>
       <c r="L527" s="14"/>
       <c r="M527" s="14"/>
-      <c r="N527" s="14"/>
+      <c r="N527" s="14">
+        <v>34.799999999999997</v>
+      </c>
       <c r="O527" s="14"/>
       <c r="P527" s="14"/>
       <c r="Q527" s="14"/>
@@ -24916,6 +25342,9 @@
         <v>325</v>
       </c>
       <c r="K528" s="17"/>
+      <c r="N528">
+        <v>22.6</v>
+      </c>
     </row>
     <row r="529" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A529" s="14" t="s">
@@ -24947,7 +25376,9 @@
       <c r="K529" s="18"/>
       <c r="L529" s="14"/>
       <c r="M529" s="14"/>
-      <c r="N529" s="14"/>
+      <c r="N529" s="14">
+        <v>27.9</v>
+      </c>
       <c r="O529" s="14"/>
       <c r="P529" s="14"/>
       <c r="Q529" s="14"/>
@@ -24981,6 +25412,9 @@
         <v>325</v>
       </c>
       <c r="K530" s="17"/>
+      <c r="N530">
+        <v>26.7</v>
+      </c>
     </row>
     <row r="531" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A531" s="14" t="s">
@@ -25012,7 +25446,9 @@
       <c r="K531" s="18"/>
       <c r="L531" s="14"/>
       <c r="M531" s="14"/>
-      <c r="N531" s="14"/>
+      <c r="N531" s="14">
+        <v>28.4</v>
+      </c>
       <c r="O531" s="14"/>
       <c r="P531" s="14"/>
       <c r="Q531" s="14"/>
@@ -25220,7 +25656,9 @@
       <c r="K537" s="18"/>
       <c r="L537" s="14"/>
       <c r="M537" s="14"/>
-      <c r="N537" s="14"/>
+      <c r="N537" s="14">
+        <v>26.7</v>
+      </c>
       <c r="O537" s="14"/>
       <c r="P537" s="14"/>
       <c r="Q537" s="14"/>
@@ -25254,6 +25692,9 @@
         <v>325</v>
       </c>
       <c r="K538" s="17"/>
+      <c r="N538">
+        <v>32.1</v>
+      </c>
     </row>
     <row r="539" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A539" s="14" t="s">
@@ -25285,7 +25726,9 @@
       <c r="K539" s="18"/>
       <c r="L539" s="14"/>
       <c r="M539" s="14"/>
-      <c r="N539" s="14"/>
+      <c r="N539" s="14">
+        <v>29.2</v>
+      </c>
       <c r="O539" s="14"/>
       <c r="P539" s="14"/>
       <c r="Q539" s="14"/>
@@ -25319,6 +25762,9 @@
         <v>325</v>
       </c>
       <c r="K540" s="17"/>
+      <c r="N540">
+        <v>32.200000000000003</v>
+      </c>
     </row>
     <row r="541" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A541" s="14" t="s">
@@ -25350,7 +25796,9 @@
       <c r="K541" s="18"/>
       <c r="L541" s="14"/>
       <c r="M541" s="14"/>
-      <c r="N541" s="14"/>
+      <c r="N541" s="14">
+        <v>25.9</v>
+      </c>
       <c r="O541" s="14"/>
       <c r="P541" s="14"/>
       <c r="Q541" s="14"/>
@@ -30088,7 +30536,7 @@
       <c r="K820" s="17"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="9" type="noConversion"/>
+  <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
small change in comment for measurements
</commit_message>
<xml_diff>
--- a/data/treeMeasurements/TreeMeasurements.xlsx
+++ b/data/treeMeasurements/TreeMeasurements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christophe_rouleau-desrochers/github/fuelinex/data/treeMeasurements/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B90B2FE8-163E-4E49-BFF4-5F240C22A5BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E205C32-30D5-A94E-A403-1528F1DFA5A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4732" uniqueCount="1453">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4733" uniqueCount="1454">
   <si>
     <t>tree_ID</t>
   </si>
@@ -4395,6 +4395,9 @@
   </si>
   <si>
     <t>middle of the crown is dead; the rest is not doing great</t>
+  </si>
+  <si>
+    <t>apical shoot dead, lateral shoot measured</t>
   </si>
 </sst>
 </file>
@@ -4404,11 +4407,18 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -4577,47 +4587,48 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="17" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="14" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="15" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -5500,7 +5511,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="167" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Y210" sqref="Y210"/>
+      <selection pane="topRight" activeCell="V402" sqref="V402"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5510,27 +5521,27 @@
     <col min="3" max="3" width="11.6640625" customWidth="1"/>
     <col min="4" max="4" width="8.1640625" customWidth="1"/>
     <col min="5" max="5" width="7.1640625" customWidth="1"/>
-    <col min="6" max="6" width="19" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="22.83203125" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="16.5" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="10.6640625" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="7.83203125" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="16.33203125" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="19.6640625" style="18" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="17.33203125" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="19" customWidth="1"/>
+    <col min="7" max="7" width="22.83203125" customWidth="1"/>
+    <col min="8" max="8" width="16.5" customWidth="1"/>
+    <col min="9" max="9" width="10.6640625" customWidth="1"/>
+    <col min="10" max="10" width="7.83203125" customWidth="1"/>
+    <col min="11" max="11" width="16.33203125" customWidth="1"/>
+    <col min="12" max="12" width="19.6640625" style="18" customWidth="1"/>
+    <col min="13" max="13" width="17.33203125" customWidth="1"/>
     <col min="14" max="14" width="16.6640625" customWidth="1"/>
-    <col min="15" max="15" width="27.5" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="14" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="21" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="24.1640625" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="15.33203125" customWidth="1"/>
-    <col min="20" max="20" width="20" hidden="1" customWidth="1"/>
-    <col min="21" max="21" width="22.6640625" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="27.5" customWidth="1"/>
+    <col min="16" max="16" width="14" customWidth="1"/>
+    <col min="17" max="17" width="21" customWidth="1"/>
+    <col min="18" max="18" width="24.1640625" customWidth="1"/>
+    <col min="19" max="19" width="29" customWidth="1"/>
+    <col min="20" max="20" width="20" customWidth="1"/>
+    <col min="21" max="21" width="8.83203125" customWidth="1"/>
     <col min="22" max="22" width="18.5" customWidth="1"/>
-    <col min="23" max="23" width="19.5" hidden="1" customWidth="1"/>
-    <col min="24" max="24" width="23.1640625" hidden="1" customWidth="1"/>
+    <col min="23" max="23" width="19.5" customWidth="1"/>
+    <col min="24" max="24" width="23.1640625" customWidth="1"/>
     <col min="25" max="25" width="26.1640625" customWidth="1"/>
-    <col min="26" max="26" width="17.83203125" hidden="1" customWidth="1"/>
+    <col min="26" max="26" width="17.83203125" customWidth="1"/>
     <col min="27" max="27" width="25.83203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -24527,7 +24538,7 @@
       </c>
       <c r="Y392" s="30"/>
       <c r="Z392" s="30"/>
-      <c r="AA392" s="30"/>
+      <c r="AA392" s="15"/>
     </row>
     <row r="393" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A393" s="3" t="s">
@@ -25082,7 +25093,9 @@
         <v>1407</v>
       </c>
       <c r="Z402" s="17"/>
-      <c r="AA402" s="17"/>
+      <c r="AA402" s="43" t="s">
+        <v>1453</v>
+      </c>
     </row>
     <row r="403" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A403" s="3" t="s">
@@ -38160,7 +38173,7 @@
       <c r="K820" s="6"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="18" type="noConversion"/>
+  <phoneticPr fontId="19" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
done with first draft of proposal
</commit_message>
<xml_diff>
--- a/data/treeMeasurements/TreeMeasurements.xlsx
+++ b/data/treeMeasurements/TreeMeasurements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christophe_rouleau-desrochers/github/fuelinex/data/treeMeasurements/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51FBA737-67BB-4349-B289-A4507622F358}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{893BCE22-9A84-374E-8CDE-2C9FBBC1DAD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4738" uniqueCount="1455">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4750" uniqueCount="1462">
   <si>
     <t>tree_ID</t>
   </si>
@@ -4401,6 +4401,27 @@
   </si>
   <si>
     <t>trunk 2 is smaller than previous year because its dead</t>
+  </si>
+  <si>
+    <t>there are 2 trunks; might have missed measurement last year</t>
+  </si>
+  <si>
+    <t>main trunk might be dead but still took measurement</t>
+  </si>
+  <si>
+    <t>top of tree is dead; highest lateral shoot measured</t>
+  </si>
+  <si>
+    <t>previous year's measurement was probably wrong; double checked and shoot is intact</t>
+  </si>
+  <si>
+    <t>yes (trunk 2)</t>
+  </si>
+  <si>
+    <t>second trunk previous year measurement is wrong; it grew 2cm in 2025</t>
+  </si>
+  <si>
+    <t>apical shoot died; lateral shoot measured</t>
   </si>
 </sst>
 </file>
@@ -4410,11 +4431,18 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -4597,47 +4625,48 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="17" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="19" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="18" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="16" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="17" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -5289,7 +5318,7 @@
   <autoFilter ref="A1:AA631" xr:uid="{3F288811-81FB-F847-9587-99D03002EDFF}">
     <filterColumn colId="1">
       <filters>
-        <filter val="2"/>
+        <filter val="3"/>
       </filters>
     </filterColumn>
     <filterColumn colId="3">
@@ -5531,9 +5560,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AA820"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="167" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="U99" sqref="U99"/>
+    <sheetView tabSelected="1" topLeftCell="A117" zoomScale="167" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="N1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="W163" sqref="W163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5549,20 +5578,20 @@
     <col min="9" max="9" width="0.33203125" customWidth="1"/>
     <col min="10" max="10" width="20.83203125" customWidth="1"/>
     <col min="11" max="11" width="18.1640625" customWidth="1"/>
-    <col min="12" max="12" width="22.5" style="18" customWidth="1"/>
-    <col min="13" max="13" width="22.83203125" customWidth="1"/>
-    <col min="14" max="14" width="0.6640625" customWidth="1"/>
-    <col min="15" max="15" width="0.1640625" customWidth="1"/>
+    <col min="12" max="12" width="4.6640625" style="18" customWidth="1"/>
+    <col min="13" max="13" width="2.6640625" customWidth="1"/>
+    <col min="14" max="14" width="18.1640625" customWidth="1"/>
+    <col min="15" max="15" width="20.83203125" customWidth="1"/>
     <col min="16" max="16" width="21.33203125" customWidth="1"/>
     <col min="17" max="17" width="10.33203125" hidden="1" customWidth="1"/>
     <col min="18" max="18" width="19.83203125" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="20.5" customWidth="1"/>
-    <col min="20" max="20" width="15.6640625" customWidth="1"/>
-    <col min="21" max="21" width="25.5" customWidth="1"/>
-    <col min="22" max="22" width="10.83203125" customWidth="1"/>
+    <col min="19" max="19" width="17.1640625" customWidth="1"/>
+    <col min="20" max="20" width="15.6640625" hidden="1" customWidth="1"/>
+    <col min="21" max="21" width="0.5" customWidth="1"/>
+    <col min="22" max="22" width="12.5" customWidth="1"/>
     <col min="23" max="23" width="19.83203125" customWidth="1"/>
     <col min="24" max="24" width="23.1640625" customWidth="1"/>
-    <col min="25" max="25" width="26.1640625" customWidth="1"/>
+    <col min="25" max="25" width="22.5" customWidth="1"/>
     <col min="26" max="26" width="17.83203125" customWidth="1"/>
     <col min="27" max="27" width="25.83203125" customWidth="1"/>
   </cols>
@@ -10378,6 +10407,9 @@
       <c r="T92">
         <v>9.57</v>
       </c>
+      <c r="V92">
+        <v>65.7</v>
+      </c>
     </row>
     <row r="93" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="3" t="s">
@@ -10425,7 +10457,9 @@
         <v>9.0299999999999994</v>
       </c>
       <c r="U93" s="3"/>
-      <c r="V93" s="3"/>
+      <c r="V93" s="3">
+        <v>93.3</v>
+      </c>
       <c r="W93" s="3"/>
       <c r="X93" s="3"/>
       <c r="Y93" s="3"/>
@@ -10472,6 +10506,9 @@
       <c r="T94">
         <v>8.52</v>
       </c>
+      <c r="V94">
+        <v>69.5</v>
+      </c>
     </row>
     <row r="95" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="3" t="s">
@@ -10529,12 +10566,18 @@
       <c r="U95" s="3">
         <v>11.15</v>
       </c>
-      <c r="V95" s="3"/>
-      <c r="W95" s="3"/>
+      <c r="V95" s="3">
+        <v>103.3</v>
+      </c>
+      <c r="W95" s="3">
+        <v>110</v>
+      </c>
       <c r="X95" s="3"/>
       <c r="Y95" s="3"/>
       <c r="Z95" s="3"/>
-      <c r="AA95" s="3"/>
+      <c r="AA95" s="3" t="s">
+        <v>1456</v>
+      </c>
     </row>
     <row r="96" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
@@ -10576,8 +10619,11 @@
       <c r="T96">
         <v>8.65</v>
       </c>
-    </row>
-    <row r="97" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V96">
+        <v>72.900000000000006</v>
+      </c>
+    </row>
+    <row r="97" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="3" t="s">
         <v>416</v>
       </c>
@@ -10623,14 +10669,16 @@
         <v>10.93</v>
       </c>
       <c r="U97" s="3"/>
-      <c r="V97" s="3"/>
+      <c r="V97" s="3">
+        <v>98.6</v>
+      </c>
       <c r="W97" s="3"/>
       <c r="X97" s="3"/>
       <c r="Y97" s="3"/>
       <c r="Z97" s="3"/>
       <c r="AA97" s="3"/>
     </row>
-    <row r="98" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
         <v>419</v>
       </c>
@@ -10670,8 +10718,11 @@
       <c r="T98">
         <v>9.7200000000000006</v>
       </c>
-    </row>
-    <row r="99" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V98">
+        <v>106.9</v>
+      </c>
+    </row>
+    <row r="99" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="3" t="s">
         <v>422</v>
       </c>
@@ -10717,14 +10768,16 @@
         <v>13.89</v>
       </c>
       <c r="U99" s="3"/>
-      <c r="V99" s="3"/>
+      <c r="V99" s="3">
+        <v>114.3</v>
+      </c>
       <c r="W99" s="3"/>
       <c r="X99" s="3"/>
       <c r="Y99" s="3"/>
       <c r="Z99" s="3"/>
       <c r="AA99" s="3"/>
     </row>
-    <row r="100" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
         <v>425</v>
       </c>
@@ -10764,8 +10817,17 @@
       <c r="T100">
         <v>10.23</v>
       </c>
-    </row>
-    <row r="101" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V100">
+        <v>98.6</v>
+      </c>
+      <c r="Y100" s="45" t="s">
+        <v>1427</v>
+      </c>
+      <c r="AA100" s="45" t="s">
+        <v>1458</v>
+      </c>
+    </row>
+    <row r="101" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="3" t="s">
         <v>428</v>
       </c>
@@ -10811,14 +10873,16 @@
         <v>9.2899999999999991</v>
       </c>
       <c r="U101" s="3"/>
-      <c r="V101" s="3"/>
+      <c r="V101" s="3">
+        <v>128.6</v>
+      </c>
       <c r="W101" s="3"/>
       <c r="X101" s="3"/>
       <c r="Y101" s="3"/>
       <c r="Z101" s="3"/>
       <c r="AA101" s="3"/>
     </row>
-    <row r="102" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
         <v>431</v>
       </c>
@@ -10865,8 +10929,26 @@
       <c r="P102">
         <v>57</v>
       </c>
-    </row>
-    <row r="103" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="T102">
+        <v>7.77</v>
+      </c>
+      <c r="U102">
+        <v>6.41</v>
+      </c>
+      <c r="V102">
+        <v>69.5</v>
+      </c>
+      <c r="W102">
+        <v>60.6</v>
+      </c>
+      <c r="Y102" s="45" t="s">
+        <v>1427</v>
+      </c>
+      <c r="AA102" s="45" t="s">
+        <v>1461</v>
+      </c>
+    </row>
+    <row r="103" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="3" t="s">
         <v>436</v>
       </c>
@@ -10908,16 +10990,20 @@
       <c r="Q103" s="3"/>
       <c r="R103" s="3"/>
       <c r="S103" s="3"/>
-      <c r="T103" s="3"/>
+      <c r="T103" s="3">
+        <v>9.61</v>
+      </c>
       <c r="U103" s="3"/>
-      <c r="V103" s="3"/>
+      <c r="V103" s="3">
+        <v>95.7</v>
+      </c>
       <c r="W103" s="3"/>
       <c r="X103" s="3"/>
       <c r="Y103" s="3"/>
       <c r="Z103" s="3"/>
       <c r="AA103" s="3"/>
     </row>
-    <row r="104" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
         <v>439</v>
       </c>
@@ -10954,8 +11040,14 @@
       <c r="P104">
         <v>57</v>
       </c>
-    </row>
-    <row r="105" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="T104">
+        <v>11.12</v>
+      </c>
+      <c r="V104">
+        <v>120.3</v>
+      </c>
+    </row>
+    <row r="105" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="3" t="s">
         <v>442</v>
       </c>
@@ -11005,16 +11097,24 @@
       <c r="Q105" s="3"/>
       <c r="R105" s="3"/>
       <c r="S105" s="3"/>
-      <c r="T105" s="3"/>
-      <c r="U105" s="3"/>
-      <c r="V105" s="3"/>
-      <c r="W105" s="3"/>
+      <c r="T105" s="3">
+        <v>6.27</v>
+      </c>
+      <c r="U105" s="3">
+        <v>6.3</v>
+      </c>
+      <c r="V105" s="3">
+        <v>63.3</v>
+      </c>
+      <c r="W105" s="3">
+        <v>63.5</v>
+      </c>
       <c r="X105" s="3"/>
       <c r="Y105" s="3"/>
       <c r="Z105" s="3"/>
       <c r="AA105" s="3"/>
     </row>
-    <row r="106" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
         <v>446</v>
       </c>
@@ -11060,6 +11160,18 @@
       </c>
       <c r="P106">
         <v>57</v>
+      </c>
+      <c r="T106">
+        <v>8.58</v>
+      </c>
+      <c r="U106">
+        <v>5.75</v>
+      </c>
+      <c r="V106">
+        <v>82.8</v>
+      </c>
+      <c r="W106">
+        <v>46</v>
       </c>
     </row>
     <row r="107" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -11108,7 +11220,9 @@
         <v>12.17</v>
       </c>
       <c r="U107" s="3"/>
-      <c r="V107" s="3"/>
+      <c r="V107" s="3">
+        <v>120.8</v>
+      </c>
       <c r="W107" s="3"/>
       <c r="X107" s="3"/>
       <c r="Y107" s="3"/>
@@ -11155,6 +11269,9 @@
       <c r="T108">
         <v>7.95</v>
       </c>
+      <c r="V108">
+        <v>74.400000000000006</v>
+      </c>
     </row>
     <row r="109" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="3" t="s">
@@ -11202,7 +11319,9 @@
         <v>11.08</v>
       </c>
       <c r="U109" s="3"/>
-      <c r="V109" s="3"/>
+      <c r="V109" s="3">
+        <v>99</v>
+      </c>
       <c r="W109" s="3"/>
       <c r="X109" s="3"/>
       <c r="Y109" s="3"/>
@@ -11262,6 +11381,18 @@
       <c r="U110">
         <v>8.85</v>
       </c>
+      <c r="V110">
+        <v>58.5</v>
+      </c>
+      <c r="W110">
+        <v>76.599999999999994</v>
+      </c>
+      <c r="Y110" s="45" t="s">
+        <v>1427</v>
+      </c>
+      <c r="AA110" s="45" t="s">
+        <v>1419</v>
+      </c>
     </row>
     <row r="111" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="3" t="s">
@@ -11309,14 +11440,16 @@
         <v>9.09</v>
       </c>
       <c r="U111" s="3"/>
-      <c r="V111" s="3"/>
+      <c r="V111" s="3">
+        <v>57.6</v>
+      </c>
       <c r="W111" s="3"/>
       <c r="X111" s="3"/>
       <c r="Y111" s="3"/>
       <c r="Z111" s="3"/>
       <c r="AA111" s="3"/>
     </row>
-    <row r="112" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
         <v>461</v>
       </c>
@@ -11356,8 +11489,11 @@
       <c r="T112">
         <v>10.77</v>
       </c>
-    </row>
-    <row r="113" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V112">
+        <v>126.9</v>
+      </c>
+    </row>
+    <row r="113" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="3" t="s">
         <v>463</v>
       </c>
@@ -11403,14 +11539,16 @@
         <v>13.08</v>
       </c>
       <c r="U113" s="3"/>
-      <c r="V113" s="3"/>
+      <c r="V113" s="3">
+        <v>105.3</v>
+      </c>
       <c r="W113" s="3"/>
       <c r="X113" s="3"/>
       <c r="Y113" s="3"/>
       <c r="Z113" s="3"/>
       <c r="AA113" s="3"/>
     </row>
-    <row r="114" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
         <v>466</v>
       </c>
@@ -11450,8 +11588,11 @@
       <c r="T114">
         <v>8.5299999999999994</v>
       </c>
-    </row>
-    <row r="115" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V114">
+        <v>97.1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="3" t="s">
         <v>469</v>
       </c>
@@ -11497,14 +11638,16 @@
         <v>9.0299999999999994</v>
       </c>
       <c r="U115" s="3"/>
-      <c r="V115" s="3"/>
+      <c r="V115" s="3">
+        <v>85</v>
+      </c>
       <c r="W115" s="3"/>
       <c r="X115" s="3"/>
       <c r="Y115" s="3"/>
       <c r="Z115" s="3"/>
       <c r="AA115" s="3"/>
     </row>
-    <row r="116" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
         <v>471</v>
       </c>
@@ -11544,8 +11687,11 @@
       <c r="T116">
         <v>12.25</v>
       </c>
-    </row>
-    <row r="117" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V116">
+        <v>122.9</v>
+      </c>
+    </row>
+    <row r="117" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="3" t="s">
         <v>473</v>
       </c>
@@ -11587,16 +11733,20 @@
       <c r="Q117" s="3"/>
       <c r="R117" s="3"/>
       <c r="S117" s="3"/>
-      <c r="T117" s="3"/>
+      <c r="T117" s="3">
+        <v>8.1300000000000008</v>
+      </c>
       <c r="U117" s="3"/>
-      <c r="V117" s="3"/>
+      <c r="V117" s="3">
+        <v>68.8</v>
+      </c>
       <c r="W117" s="3"/>
       <c r="X117" s="3"/>
       <c r="Y117" s="3"/>
       <c r="Z117" s="3"/>
       <c r="AA117" s="3"/>
     </row>
-    <row r="118" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
         <v>476</v>
       </c>
@@ -11633,8 +11783,14 @@
       <c r="P118">
         <v>57</v>
       </c>
-    </row>
-    <row r="119" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="T118">
+        <v>9.98</v>
+      </c>
+      <c r="V118">
+        <v>64.2</v>
+      </c>
+    </row>
+    <row r="119" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="3" t="s">
         <v>478</v>
       </c>
@@ -11682,16 +11838,26 @@
       <c r="Q119" s="3"/>
       <c r="R119" s="3"/>
       <c r="S119" s="3"/>
-      <c r="T119" s="3"/>
-      <c r="U119" s="3"/>
-      <c r="V119" s="3"/>
-      <c r="W119" s="3"/>
+      <c r="T119" s="3">
+        <v>9.68</v>
+      </c>
+      <c r="U119" s="3">
+        <v>5.05</v>
+      </c>
+      <c r="V119" s="3">
+        <v>87.6</v>
+      </c>
+      <c r="W119" s="3">
+        <v>58.9</v>
+      </c>
       <c r="X119" s="3"/>
       <c r="Y119" s="3"/>
       <c r="Z119" s="3"/>
-      <c r="AA119" s="3"/>
-    </row>
-    <row r="120" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AA119" s="3" t="s">
+        <v>1455</v>
+      </c>
+    </row>
+    <row r="120" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
         <v>481</v>
       </c>
@@ -11728,8 +11894,14 @@
       <c r="P120">
         <v>57</v>
       </c>
-    </row>
-    <row r="121" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="T120">
+        <v>12.37</v>
+      </c>
+      <c r="V120">
+        <v>102.5</v>
+      </c>
+    </row>
+    <row r="121" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="3" t="s">
         <v>483</v>
       </c>
@@ -11771,9 +11943,13 @@
       <c r="Q121" s="3"/>
       <c r="R121" s="3"/>
       <c r="S121" s="3"/>
-      <c r="T121" s="3"/>
+      <c r="T121" s="3">
+        <v>9.1999999999999993</v>
+      </c>
       <c r="U121" s="3"/>
-      <c r="V121" s="3"/>
+      <c r="V121" s="3">
+        <v>87.4</v>
+      </c>
       <c r="W121" s="3"/>
       <c r="X121" s="3"/>
       <c r="Y121" s="3"/>
@@ -11820,6 +11996,9 @@
       <c r="T122">
         <v>8.2899999999999991</v>
       </c>
+      <c r="V122">
+        <v>62.4</v>
+      </c>
     </row>
     <row r="123" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" s="3" t="s">
@@ -11867,7 +12046,9 @@
         <v>8.52</v>
       </c>
       <c r="U123" s="3"/>
-      <c r="V123" s="3"/>
+      <c r="V123" s="3">
+        <v>68.3</v>
+      </c>
       <c r="W123" s="3"/>
       <c r="X123" s="3"/>
       <c r="Y123" s="3"/>
@@ -11914,6 +12095,9 @@
       <c r="T124">
         <v>8.66</v>
       </c>
+      <c r="V124">
+        <v>91.1</v>
+      </c>
     </row>
     <row r="125" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125" s="3" t="s">
@@ -11961,7 +12145,9 @@
         <v>10.49</v>
       </c>
       <c r="U125" s="3"/>
-      <c r="V125" s="3"/>
+      <c r="V125" s="3">
+        <v>109.1</v>
+      </c>
       <c r="W125" s="3"/>
       <c r="X125" s="3"/>
       <c r="Y125" s="3"/>
@@ -12015,8 +12201,14 @@
       <c r="T126">
         <v>7.37</v>
       </c>
-    </row>
-    <row r="127" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V126">
+        <v>87.3</v>
+      </c>
+      <c r="W126">
+        <v>51.1</v>
+      </c>
+    </row>
+    <row r="127" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" s="3" t="s">
         <v>498</v>
       </c>
@@ -12062,14 +12254,16 @@
         <v>12.18</v>
       </c>
       <c r="U127" s="3"/>
-      <c r="V127" s="3"/>
+      <c r="V127" s="3">
+        <v>75</v>
+      </c>
       <c r="W127" s="3"/>
       <c r="X127" s="3"/>
       <c r="Y127" s="3"/>
       <c r="Z127" s="3"/>
       <c r="AA127" s="3"/>
     </row>
-    <row r="128" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
         <v>501</v>
       </c>
@@ -12109,8 +12303,11 @@
       <c r="T128">
         <v>10.93</v>
       </c>
-    </row>
-    <row r="129" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V128">
+        <v>81.400000000000006</v>
+      </c>
+    </row>
+    <row r="129" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A129" s="3" t="s">
         <v>504</v>
       </c>
@@ -12156,14 +12353,16 @@
         <v>9.91</v>
       </c>
       <c r="U129" s="3"/>
-      <c r="V129" s="3"/>
+      <c r="V129" s="3">
+        <v>90.8</v>
+      </c>
       <c r="W129" s="3"/>
       <c r="X129" s="3"/>
       <c r="Y129" s="3"/>
       <c r="Z129" s="3"/>
       <c r="AA129" s="3"/>
     </row>
-    <row r="130" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
         <v>507</v>
       </c>
@@ -12203,8 +12402,11 @@
       <c r="T130">
         <v>13.66</v>
       </c>
-    </row>
-    <row r="131" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V130">
+        <v>110.1</v>
+      </c>
+    </row>
+    <row r="131" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131" s="3" t="s">
         <v>510</v>
       </c>
@@ -12250,14 +12452,16 @@
         <v>9.4700000000000006</v>
       </c>
       <c r="U131" s="3"/>
-      <c r="V131" s="3"/>
+      <c r="V131" s="3">
+        <v>86</v>
+      </c>
       <c r="W131" s="3"/>
       <c r="X131" s="3"/>
       <c r="Y131" s="3"/>
       <c r="Z131" s="3"/>
       <c r="AA131" s="3"/>
     </row>
-    <row r="132" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
         <v>513</v>
       </c>
@@ -12304,8 +12508,20 @@
       <c r="P132">
         <v>57</v>
       </c>
-    </row>
-    <row r="133" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="T132">
+        <v>9.5500000000000007</v>
+      </c>
+      <c r="U132">
+        <v>6.52</v>
+      </c>
+      <c r="V132">
+        <v>86.9</v>
+      </c>
+      <c r="W132">
+        <v>66.099999999999994</v>
+      </c>
+    </row>
+    <row r="133" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A133" s="3" t="s">
         <v>516</v>
       </c>
@@ -12355,16 +12571,24 @@
       <c r="Q133" s="3"/>
       <c r="R133" s="3"/>
       <c r="S133" s="3"/>
-      <c r="T133" s="3"/>
-      <c r="U133" s="3"/>
-      <c r="V133" s="3"/>
-      <c r="W133" s="3"/>
+      <c r="T133" s="3">
+        <v>9.51</v>
+      </c>
+      <c r="U133" s="3">
+        <v>5.44</v>
+      </c>
+      <c r="V133" s="3">
+        <v>91.7</v>
+      </c>
+      <c r="W133" s="3">
+        <v>62.3</v>
+      </c>
       <c r="X133" s="3"/>
       <c r="Y133" s="3"/>
       <c r="Z133" s="3"/>
       <c r="AA133" s="3"/>
     </row>
-    <row r="134" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
         <v>520</v>
       </c>
@@ -12401,8 +12625,14 @@
       <c r="P134">
         <v>57</v>
       </c>
-    </row>
-    <row r="135" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="T134">
+        <v>9.26</v>
+      </c>
+      <c r="V134">
+        <v>78.099999999999994</v>
+      </c>
+    </row>
+    <row r="135" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A135" s="3" t="s">
         <v>522</v>
       </c>
@@ -12444,16 +12674,20 @@
       <c r="Q135" s="3"/>
       <c r="R135" s="3"/>
       <c r="S135" s="3"/>
-      <c r="T135" s="3"/>
+      <c r="T135" s="3">
+        <v>9.1999999999999993</v>
+      </c>
       <c r="U135" s="3"/>
-      <c r="V135" s="3"/>
+      <c r="V135" s="3">
+        <v>74.2</v>
+      </c>
       <c r="W135" s="3"/>
       <c r="X135" s="3"/>
       <c r="Y135" s="3"/>
       <c r="Z135" s="3"/>
       <c r="AA135" s="3"/>
     </row>
-    <row r="136" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
         <v>524</v>
       </c>
@@ -12502,6 +12736,12 @@
       </c>
       <c r="S136" s="17" t="s">
         <v>1411</v>
+      </c>
+      <c r="T136">
+        <v>7.16</v>
+      </c>
+      <c r="V136">
+        <v>72.8</v>
       </c>
     </row>
     <row r="137" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -12550,7 +12790,9 @@
         <v>9.81</v>
       </c>
       <c r="U137" s="3"/>
-      <c r="V137" s="3"/>
+      <c r="V137" s="3">
+        <v>83.6</v>
+      </c>
       <c r="W137" s="3"/>
       <c r="X137" s="3"/>
       <c r="Y137" s="3"/>
@@ -12610,6 +12852,12 @@
       <c r="U138">
         <v>6.45</v>
       </c>
+      <c r="V138">
+        <v>64.2</v>
+      </c>
+      <c r="W138">
+        <v>63.9</v>
+      </c>
     </row>
     <row r="139" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A139" s="3" t="s">
@@ -12657,7 +12905,9 @@
         <v>10.24</v>
       </c>
       <c r="U139" s="3"/>
-      <c r="V139" s="3"/>
+      <c r="V139" s="3">
+        <v>88.2</v>
+      </c>
       <c r="W139" s="3"/>
       <c r="X139" s="3"/>
       <c r="Y139" s="3"/>
@@ -12717,6 +12967,12 @@
       <c r="U140">
         <v>5.33</v>
       </c>
+      <c r="V140">
+        <v>107.1</v>
+      </c>
+      <c r="W140">
+        <v>64.2</v>
+      </c>
     </row>
     <row r="141" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A141" s="3" t="s">
@@ -12764,14 +13020,16 @@
         <v>12.72</v>
       </c>
       <c r="U141" s="3"/>
-      <c r="V141" s="3"/>
+      <c r="V141" s="3">
+        <v>108.9</v>
+      </c>
       <c r="W141" s="3"/>
       <c r="X141" s="3"/>
       <c r="Y141" s="3"/>
       <c r="Z141" s="3"/>
       <c r="AA141" s="3"/>
     </row>
-    <row r="142" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A142" s="1" t="s">
         <v>544</v>
       </c>
@@ -12811,8 +13069,11 @@
       <c r="T142">
         <v>9.42</v>
       </c>
-    </row>
-    <row r="143" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V142">
+        <v>69.7</v>
+      </c>
+    </row>
+    <row r="143" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A143" s="3" t="s">
         <v>547</v>
       </c>
@@ -12858,14 +13119,16 @@
         <v>9.2100000000000009</v>
       </c>
       <c r="U143" s="3"/>
-      <c r="V143" s="3"/>
+      <c r="V143" s="3">
+        <v>91.4</v>
+      </c>
       <c r="W143" s="3"/>
       <c r="X143" s="3"/>
       <c r="Y143" s="3"/>
       <c r="Z143" s="3"/>
       <c r="AA143" s="3"/>
     </row>
-    <row r="144" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A144" s="1" t="s">
         <v>550</v>
       </c>
@@ -12905,8 +13168,11 @@
       <c r="T144">
         <v>12.78</v>
       </c>
-    </row>
-    <row r="145" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V144">
+        <v>132.4</v>
+      </c>
+    </row>
+    <row r="145" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A145" s="3" t="s">
         <v>553</v>
       </c>
@@ -12962,14 +13228,18 @@
       <c r="U145" s="3">
         <v>3.52</v>
       </c>
-      <c r="V145" s="3"/>
-      <c r="W145" s="3"/>
+      <c r="V145" s="3">
+        <v>159.19999999999999</v>
+      </c>
+      <c r="W145" s="3">
+        <v>38.9</v>
+      </c>
       <c r="X145" s="3"/>
       <c r="Y145" s="3"/>
       <c r="Z145" s="3"/>
       <c r="AA145" s="3"/>
     </row>
-    <row r="146" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
         <v>558</v>
       </c>
@@ -13009,8 +13279,11 @@
       <c r="T146">
         <v>11.55</v>
       </c>
-    </row>
-    <row r="147" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V146">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="147" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A147" s="3" t="s">
         <v>561</v>
       </c>
@@ -13052,16 +13325,20 @@
       <c r="Q147" s="3"/>
       <c r="R147" s="3"/>
       <c r="S147" s="3"/>
-      <c r="T147" s="3"/>
+      <c r="T147" s="3">
+        <v>12.81</v>
+      </c>
       <c r="U147" s="3"/>
-      <c r="V147" s="3"/>
+      <c r="V147" s="3">
+        <v>151.1</v>
+      </c>
       <c r="W147" s="3"/>
       <c r="X147" s="3"/>
       <c r="Y147" s="3"/>
       <c r="Z147" s="3"/>
       <c r="AA147" s="3"/>
     </row>
-    <row r="148" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A148" s="1" t="s">
         <v>564</v>
       </c>
@@ -13098,8 +13375,14 @@
       <c r="P148">
         <v>57</v>
       </c>
-    </row>
-    <row r="149" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="T148">
+        <v>7.46</v>
+      </c>
+      <c r="V148">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="149" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A149" s="3" t="s">
         <v>566</v>
       </c>
@@ -13141,16 +13424,20 @@
       <c r="Q149" s="3"/>
       <c r="R149" s="3"/>
       <c r="S149" s="3"/>
-      <c r="T149" s="3"/>
+      <c r="T149" s="3">
+        <v>12.04</v>
+      </c>
       <c r="U149" s="3"/>
-      <c r="V149" s="3"/>
+      <c r="V149" s="3">
+        <v>129</v>
+      </c>
       <c r="W149" s="3"/>
       <c r="X149" s="3"/>
       <c r="Y149" s="3"/>
       <c r="Z149" s="3"/>
       <c r="AA149" s="3"/>
     </row>
-    <row r="150" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
         <v>569</v>
       </c>
@@ -13197,11 +13484,23 @@
       <c r="P150">
         <v>57</v>
       </c>
-      <c r="S150" s="36" t="s">
+      <c r="S150" s="45" t="s">
         <v>1431</v>
       </c>
-    </row>
-    <row r="151" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="T150">
+        <v>7.22</v>
+      </c>
+      <c r="U150">
+        <v>9.24</v>
+      </c>
+      <c r="V150">
+        <v>109.6</v>
+      </c>
+      <c r="W150">
+        <v>127.9</v>
+      </c>
+    </row>
+    <row r="151" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A151" s="3" t="s">
         <v>574</v>
       </c>
@@ -13243,9 +13542,13 @@
       <c r="Q151" s="3"/>
       <c r="R151" s="3"/>
       <c r="S151" s="3"/>
-      <c r="T151" s="3"/>
+      <c r="T151" s="3">
+        <v>10.050000000000001</v>
+      </c>
       <c r="U151" s="3"/>
-      <c r="V151" s="3"/>
+      <c r="V151" s="3">
+        <v>77.3</v>
+      </c>
       <c r="W151" s="3"/>
       <c r="X151" s="3"/>
       <c r="Y151" s="3"/>
@@ -13292,6 +13595,9 @@
       <c r="T152">
         <v>12.49</v>
       </c>
+      <c r="V152">
+        <v>107.7</v>
+      </c>
     </row>
     <row r="153" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A153" s="3" t="s">
@@ -13339,7 +13645,9 @@
         <v>9.89</v>
       </c>
       <c r="U153" s="3"/>
-      <c r="V153" s="3"/>
+      <c r="V153" s="3">
+        <v>120</v>
+      </c>
       <c r="W153" s="3"/>
       <c r="X153" s="3"/>
       <c r="Y153" s="3"/>
@@ -13386,6 +13694,9 @@
       <c r="T154">
         <v>10.02</v>
       </c>
+      <c r="V154">
+        <v>68.8</v>
+      </c>
     </row>
     <row r="155" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A155" s="3" t="s">
@@ -13443,8 +13754,12 @@
       <c r="U155" s="3" t="s">
         <v>1386</v>
       </c>
-      <c r="V155" s="3"/>
-      <c r="W155" s="3"/>
+      <c r="V155" s="3">
+        <v>91</v>
+      </c>
+      <c r="W155" s="3">
+        <v>46.9</v>
+      </c>
       <c r="X155" s="3"/>
       <c r="Y155" s="3"/>
       <c r="Z155" s="3"/>
@@ -13492,8 +13807,11 @@
       <c r="T156">
         <v>15.19</v>
       </c>
-    </row>
-    <row r="157" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V156">
+        <v>139.5</v>
+      </c>
+    </row>
+    <row r="157" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A157" s="3" t="s">
         <v>593</v>
       </c>
@@ -13539,14 +13857,16 @@
         <v>13.04</v>
       </c>
       <c r="U157" s="3"/>
-      <c r="V157" s="3"/>
+      <c r="V157" s="3">
+        <v>93.3</v>
+      </c>
       <c r="W157" s="3"/>
       <c r="X157" s="3"/>
       <c r="Y157" s="3"/>
       <c r="Z157" s="3"/>
       <c r="AA157" s="3"/>
     </row>
-    <row r="158" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A158" s="1" t="s">
         <v>596</v>
       </c>
@@ -13586,8 +13906,17 @@
       <c r="T158">
         <v>11.3</v>
       </c>
-    </row>
-    <row r="159" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V158">
+        <v>38.1</v>
+      </c>
+      <c r="Y158" s="45" t="s">
+        <v>1427</v>
+      </c>
+      <c r="AA158" s="45" t="s">
+        <v>1457</v>
+      </c>
+    </row>
+    <row r="159" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A159" s="3" t="s">
         <v>599</v>
       </c>
@@ -13633,14 +13962,16 @@
         <v>10.29</v>
       </c>
       <c r="U159" s="3"/>
-      <c r="V159" s="3"/>
+      <c r="V159" s="3">
+        <v>109.1</v>
+      </c>
       <c r="W159" s="3"/>
       <c r="X159" s="3"/>
       <c r="Y159" s="3"/>
       <c r="Z159" s="3"/>
       <c r="AA159" s="3"/>
     </row>
-    <row r="160" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A160" s="1" t="s">
         <v>602</v>
       </c>
@@ -13680,8 +14011,11 @@
       <c r="T160">
         <v>13.62</v>
       </c>
-    </row>
-    <row r="161" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V160">
+        <v>141.9</v>
+      </c>
+    </row>
+    <row r="161" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A161" s="3" t="s">
         <v>605</v>
       </c>
@@ -13727,14 +14061,16 @@
         <v>8.89</v>
       </c>
       <c r="U161" s="3"/>
-      <c r="V161" s="3"/>
+      <c r="V161" s="3">
+        <v>46.2</v>
+      </c>
       <c r="W161" s="3"/>
       <c r="X161" s="3"/>
       <c r="Y161" s="3"/>
       <c r="Z161" s="3"/>
       <c r="AA161" s="3"/>
     </row>
-    <row r="162" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A162" s="1" t="s">
         <v>607</v>
       </c>
@@ -13771,8 +14107,14 @@
       <c r="P162">
         <v>57</v>
       </c>
-    </row>
-    <row r="163" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="T162">
+        <v>11.96</v>
+      </c>
+      <c r="V162">
+        <v>114.9</v>
+      </c>
+    </row>
+    <row r="163" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A163" s="3" t="s">
         <v>610</v>
       </c>
@@ -13822,16 +14164,28 @@
       <c r="Q163" s="3"/>
       <c r="R163" s="3"/>
       <c r="S163" s="3"/>
-      <c r="T163" s="3"/>
-      <c r="U163" s="3"/>
-      <c r="V163" s="3"/>
-      <c r="W163" s="3"/>
+      <c r="T163" s="3">
+        <v>7.6</v>
+      </c>
+      <c r="U163" s="3">
+        <v>4.6399999999999997</v>
+      </c>
+      <c r="V163" s="3">
+        <v>76.2</v>
+      </c>
+      <c r="W163" s="3">
+        <v>53.7</v>
+      </c>
       <c r="X163" s="3"/>
-      <c r="Y163" s="3"/>
+      <c r="Y163" s="3" t="s">
+        <v>1459</v>
+      </c>
       <c r="Z163" s="3"/>
-      <c r="AA163" s="3"/>
-    </row>
-    <row r="164" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AA163" s="3" t="s">
+        <v>1460</v>
+      </c>
+    </row>
+    <row r="164" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A164" s="1" t="s">
         <v>614</v>
       </c>
@@ -13878,8 +14232,20 @@
       <c r="P164">
         <v>57</v>
       </c>
-    </row>
-    <row r="165" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="T164">
+        <v>8.43</v>
+      </c>
+      <c r="U164">
+        <v>6.49</v>
+      </c>
+      <c r="V164">
+        <v>68.900000000000006</v>
+      </c>
+      <c r="W164">
+        <v>62.1</v>
+      </c>
+    </row>
+    <row r="165" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A165" s="3" t="s">
         <v>617</v>
       </c>
@@ -13921,16 +14287,20 @@
       <c r="Q165" s="3"/>
       <c r="R165" s="3"/>
       <c r="S165" s="3"/>
-      <c r="T165" s="3"/>
+      <c r="T165" s="3">
+        <v>7.3</v>
+      </c>
       <c r="U165" s="3"/>
-      <c r="V165" s="3"/>
+      <c r="V165" s="3">
+        <v>73.3</v>
+      </c>
       <c r="W165" s="3"/>
       <c r="X165" s="3"/>
       <c r="Y165" s="3"/>
       <c r="Z165" s="3"/>
       <c r="AA165" s="3"/>
     </row>
-    <row r="166" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A166" s="1" t="s">
         <v>620</v>
       </c>
@@ -13966,6 +14336,12 @@
       </c>
       <c r="P166">
         <v>57</v>
+      </c>
+      <c r="T166">
+        <v>9.0299999999999994</v>
+      </c>
+      <c r="V166">
+        <v>55.1</v>
       </c>
     </row>
     <row r="167" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -14024,8 +14400,12 @@
       <c r="U167" s="3">
         <v>6.33</v>
       </c>
-      <c r="V167" s="3"/>
-      <c r="W167" s="3"/>
+      <c r="V167" s="3">
+        <v>108.4</v>
+      </c>
+      <c r="W167" s="3">
+        <v>51.8</v>
+      </c>
       <c r="X167" s="3"/>
       <c r="Y167" s="3"/>
       <c r="Z167" s="3"/>
@@ -14070,6 +14450,9 @@
       </c>
       <c r="T168">
         <v>7.73</v>
+      </c>
+      <c r="V168">
+        <v>63.5</v>
       </c>
     </row>
     <row r="169" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -14128,8 +14511,12 @@
       <c r="U169" s="3">
         <v>7.86</v>
       </c>
-      <c r="V169" s="3"/>
-      <c r="W169" s="3"/>
+      <c r="V169" s="3">
+        <v>130.1</v>
+      </c>
+      <c r="W169" s="3">
+        <v>97.4</v>
+      </c>
       <c r="X169" s="3"/>
       <c r="Y169" s="3"/>
       <c r="Z169" s="3"/>
@@ -14174,6 +14561,9 @@
       </c>
       <c r="T170">
         <v>9.15</v>
+      </c>
+      <c r="V170">
+        <v>84.5</v>
       </c>
     </row>
     <row r="171" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -14222,14 +14612,16 @@
         <v>11.27</v>
       </c>
       <c r="U171" s="3"/>
-      <c r="V171" s="3"/>
+      <c r="V171" s="3">
+        <v>78.599999999999994</v>
+      </c>
       <c r="W171" s="3"/>
       <c r="X171" s="3"/>
       <c r="Y171" s="3"/>
       <c r="Z171" s="3"/>
       <c r="AA171" s="3"/>
     </row>
-    <row r="172" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A172" s="1" t="s">
         <v>637</v>
       </c>
@@ -14282,8 +14674,14 @@
       <c r="U172">
         <v>6.34</v>
       </c>
-    </row>
-    <row r="173" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V172">
+        <v>55.4</v>
+      </c>
+      <c r="W172">
+        <v>61.4</v>
+      </c>
+    </row>
+    <row r="173" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A173" s="3" t="s">
         <v>640</v>
       </c>
@@ -14329,14 +14727,16 @@
         <v>9.32</v>
       </c>
       <c r="U173" s="3"/>
-      <c r="V173" s="3"/>
+      <c r="V173" s="3">
+        <v>124.9</v>
+      </c>
       <c r="W173" s="3"/>
       <c r="X173" s="3"/>
       <c r="Y173" s="3"/>
       <c r="Z173" s="3"/>
       <c r="AA173" s="3"/>
     </row>
-    <row r="174" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A174" s="1" t="s">
         <v>643</v>
       </c>
@@ -14389,8 +14789,14 @@
       <c r="U174">
         <v>5.0199999999999996</v>
       </c>
-    </row>
-    <row r="175" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V174">
+        <v>60.2</v>
+      </c>
+      <c r="W174">
+        <v>56.7</v>
+      </c>
+    </row>
+    <row r="175" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A175" s="3" t="s">
         <v>647</v>
       </c>
@@ -14436,14 +14842,16 @@
         <v>13.14</v>
       </c>
       <c r="U175" s="3"/>
-      <c r="V175" s="3"/>
+      <c r="V175" s="3">
+        <v>104.3</v>
+      </c>
       <c r="W175" s="3"/>
       <c r="X175" s="3"/>
       <c r="Y175" s="3"/>
       <c r="Z175" s="3"/>
       <c r="AA175" s="3"/>
     </row>
-    <row r="176" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A176" s="1" t="s">
         <v>650</v>
       </c>
@@ -14483,8 +14891,11 @@
       <c r="T176">
         <v>11.13</v>
       </c>
-    </row>
-    <row r="177" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V176">
+        <v>97.4</v>
+      </c>
+    </row>
+    <row r="177" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A177" s="3" t="s">
         <v>653</v>
       </c>
@@ -14526,16 +14937,20 @@
       <c r="Q177" s="3"/>
       <c r="R177" s="3"/>
       <c r="S177" s="3"/>
-      <c r="T177" s="3"/>
+      <c r="T177" s="3">
+        <v>7.21</v>
+      </c>
       <c r="U177" s="3"/>
-      <c r="V177" s="3"/>
+      <c r="V177" s="3">
+        <v>96.8</v>
+      </c>
       <c r="W177" s="3"/>
       <c r="X177" s="3"/>
       <c r="Y177" s="3"/>
       <c r="Z177" s="3"/>
       <c r="AA177" s="3"/>
     </row>
-    <row r="178" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A178" s="1" t="s">
         <v>656</v>
       </c>
@@ -14572,8 +14987,14 @@
       <c r="P178">
         <v>57</v>
       </c>
-    </row>
-    <row r="179" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="T178">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="V178">
+        <v>75.900000000000006</v>
+      </c>
+    </row>
+    <row r="179" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A179" s="3" t="s">
         <v>659</v>
       </c>
@@ -14615,16 +15036,20 @@
       <c r="Q179" s="3"/>
       <c r="R179" s="3"/>
       <c r="S179" s="3"/>
-      <c r="T179" s="3"/>
+      <c r="T179" s="3">
+        <v>11.69</v>
+      </c>
       <c r="U179" s="3"/>
-      <c r="V179" s="3"/>
+      <c r="V179" s="3">
+        <v>98.7</v>
+      </c>
       <c r="W179" s="3"/>
       <c r="X179" s="3"/>
       <c r="Y179" s="3"/>
       <c r="Z179" s="3"/>
       <c r="AA179" s="3"/>
     </row>
-    <row r="180" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A180" s="1" t="s">
         <v>662</v>
       </c>
@@ -14661,8 +15086,14 @@
       <c r="P180">
         <v>57</v>
       </c>
-    </row>
-    <row r="181" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="T180">
+        <v>8.51</v>
+      </c>
+      <c r="V180">
+        <v>83.1</v>
+      </c>
+    </row>
+    <row r="181" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A181" s="3" t="s">
         <v>664</v>
       </c>
@@ -14704,9 +15135,13 @@
       <c r="Q181" s="3"/>
       <c r="R181" s="3"/>
       <c r="S181" s="3"/>
-      <c r="T181" s="3"/>
+      <c r="T181" s="3">
+        <v>6.82</v>
+      </c>
       <c r="U181" s="3"/>
-      <c r="V181" s="3"/>
+      <c r="V181" s="3">
+        <v>78.7</v>
+      </c>
       <c r="W181" s="3"/>
       <c r="X181" s="3"/>
       <c r="Y181" s="3"/>
@@ -38901,7 +39336,7 @@
       <c r="K820" s="6"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="20" type="noConversion"/>
+  <phoneticPr fontId="21" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
measured height segi b1, b2 and b3, and poba b1 and b2
</commit_message>
<xml_diff>
--- a/data/treeMeasurements/TreeMeasurements.xlsx
+++ b/data/treeMeasurements/TreeMeasurements.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christophe_rouleau-desrochers/github/fuelinex/data/treeMeasurements/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{893BCE22-9A84-374E-8CDE-2C9FBBC1DAD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7C7BA4B-2DA5-1B4C-8837-B4E69E3A0E03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4750" uniqueCount="1462">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4752" uniqueCount="1462">
   <si>
     <t>tree_ID</t>
   </si>
@@ -4431,11 +4431,18 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -4625,47 +4632,48 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="17" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="18" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="17" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="20" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="19" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="17" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="18" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -5318,12 +5326,12 @@
   <autoFilter ref="A1:AA631" xr:uid="{3F288811-81FB-F847-9587-99D03002EDFF}">
     <filterColumn colId="1">
       <filters>
-        <filter val="3"/>
+        <filter val="2"/>
       </filters>
     </filterColumn>
     <filterColumn colId="3">
       <filters>
-        <filter val="betula"/>
+        <filter val="populus"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -5560,9 +5568,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AA820"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A117" zoomScale="167" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="N1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="W163" sqref="W163"/>
+    <sheetView tabSelected="1" topLeftCell="A311" zoomScale="167" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="K1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="V292" sqref="V292"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5577,17 +5585,17 @@
     <col min="8" max="8" width="0.83203125" customWidth="1"/>
     <col min="9" max="9" width="0.33203125" customWidth="1"/>
     <col min="10" max="10" width="20.83203125" customWidth="1"/>
-    <col min="11" max="11" width="18.1640625" customWidth="1"/>
-    <col min="12" max="12" width="4.6640625" style="18" customWidth="1"/>
+    <col min="11" max="11" width="17.5" customWidth="1"/>
+    <col min="12" max="12" width="20.5" style="18" hidden="1" customWidth="1"/>
     <col min="13" max="13" width="2.6640625" customWidth="1"/>
-    <col min="14" max="14" width="18.1640625" customWidth="1"/>
-    <col min="15" max="15" width="20.83203125" customWidth="1"/>
-    <col min="16" max="16" width="21.33203125" customWidth="1"/>
+    <col min="14" max="14" width="18.5" customWidth="1"/>
+    <col min="15" max="15" width="21.83203125" customWidth="1"/>
+    <col min="16" max="16" width="0.5" hidden="1" customWidth="1"/>
     <col min="17" max="17" width="10.33203125" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="19.83203125" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="0.1640625" hidden="1" customWidth="1"/>
     <col min="19" max="19" width="17.1640625" customWidth="1"/>
-    <col min="20" max="20" width="15.6640625" hidden="1" customWidth="1"/>
-    <col min="21" max="21" width="0.5" customWidth="1"/>
+    <col min="20" max="20" width="0.33203125" customWidth="1"/>
+    <col min="21" max="21" width="1.33203125" customWidth="1"/>
     <col min="22" max="22" width="12.5" customWidth="1"/>
     <col min="23" max="23" width="19.83203125" customWidth="1"/>
     <col min="24" max="24" width="23.1640625" customWidth="1"/>
@@ -10882,7 +10890,7 @@
       <c r="Z101" s="3"/>
       <c r="AA101" s="3"/>
     </row>
-    <row r="102" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
         <v>431</v>
       </c>
@@ -10948,7 +10956,7 @@
         <v>1461</v>
       </c>
     </row>
-    <row r="103" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="3" t="s">
         <v>436</v>
       </c>
@@ -11003,7 +11011,7 @@
       <c r="Z103" s="3"/>
       <c r="AA103" s="3"/>
     </row>
-    <row r="104" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
         <v>439</v>
       </c>
@@ -11047,7 +11055,7 @@
         <v>120.3</v>
       </c>
     </row>
-    <row r="105" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="3" t="s">
         <v>442</v>
       </c>
@@ -11114,7 +11122,7 @@
       <c r="Z105" s="3"/>
       <c r="AA105" s="3"/>
     </row>
-    <row r="106" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
         <v>446</v>
       </c>
@@ -11691,7 +11699,7 @@
         <v>122.9</v>
       </c>
     </row>
-    <row r="117" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="3" t="s">
         <v>473</v>
       </c>
@@ -11746,7 +11754,7 @@
       <c r="Z117" s="3"/>
       <c r="AA117" s="3"/>
     </row>
-    <row r="118" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
         <v>476</v>
       </c>
@@ -11790,7 +11798,7 @@
         <v>64.2</v>
       </c>
     </row>
-    <row r="119" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="3" t="s">
         <v>478</v>
       </c>
@@ -11857,7 +11865,7 @@
         <v>1455</v>
       </c>
     </row>
-    <row r="120" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
         <v>481</v>
       </c>
@@ -11901,7 +11909,7 @@
         <v>102.5</v>
       </c>
     </row>
-    <row r="121" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="3" t="s">
         <v>483</v>
       </c>
@@ -12461,7 +12469,7 @@
       <c r="Z131" s="3"/>
       <c r="AA131" s="3"/>
     </row>
-    <row r="132" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
         <v>513</v>
       </c>
@@ -12521,7 +12529,7 @@
         <v>66.099999999999994</v>
       </c>
     </row>
-    <row r="133" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A133" s="3" t="s">
         <v>516</v>
       </c>
@@ -12588,7 +12596,7 @@
       <c r="Z133" s="3"/>
       <c r="AA133" s="3"/>
     </row>
-    <row r="134" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
         <v>520</v>
       </c>
@@ -12632,7 +12640,7 @@
         <v>78.099999999999994</v>
       </c>
     </row>
-    <row r="135" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A135" s="3" t="s">
         <v>522</v>
       </c>
@@ -12687,7 +12695,7 @@
       <c r="Z135" s="3"/>
       <c r="AA135" s="3"/>
     </row>
-    <row r="136" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
         <v>524</v>
       </c>
@@ -13283,7 +13291,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="147" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A147" s="3" t="s">
         <v>561</v>
       </c>
@@ -13338,7 +13346,7 @@
       <c r="Z147" s="3"/>
       <c r="AA147" s="3"/>
     </row>
-    <row r="148" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A148" s="1" t="s">
         <v>564</v>
       </c>
@@ -13382,7 +13390,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="149" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A149" s="3" t="s">
         <v>566</v>
       </c>
@@ -13437,7 +13445,7 @@
       <c r="Z149" s="3"/>
       <c r="AA149" s="3"/>
     </row>
-    <row r="150" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
         <v>569</v>
       </c>
@@ -13500,7 +13508,7 @@
         <v>127.9</v>
       </c>
     </row>
-    <row r="151" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A151" s="3" t="s">
         <v>574</v>
       </c>
@@ -14070,7 +14078,7 @@
       <c r="Z161" s="3"/>
       <c r="AA161" s="3"/>
     </row>
-    <row r="162" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A162" s="1" t="s">
         <v>607</v>
       </c>
@@ -14114,7 +14122,7 @@
         <v>114.9</v>
       </c>
     </row>
-    <row r="163" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A163" s="3" t="s">
         <v>610</v>
       </c>
@@ -14185,7 +14193,7 @@
         <v>1460</v>
       </c>
     </row>
-    <row r="164" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A164" s="1" t="s">
         <v>614</v>
       </c>
@@ -14245,7 +14253,7 @@
         <v>62.1</v>
       </c>
     </row>
-    <row r="165" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A165" s="3" t="s">
         <v>617</v>
       </c>
@@ -14300,7 +14308,7 @@
       <c r="Z165" s="3"/>
       <c r="AA165" s="3"/>
     </row>
-    <row r="166" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A166" s="1" t="s">
         <v>620</v>
       </c>
@@ -14895,7 +14903,7 @@
         <v>97.4</v>
       </c>
     </row>
-    <row r="177" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A177" s="3" t="s">
         <v>653</v>
       </c>
@@ -14950,7 +14958,7 @@
       <c r="Z177" s="3"/>
       <c r="AA177" s="3"/>
     </row>
-    <row r="178" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A178" s="1" t="s">
         <v>656</v>
       </c>
@@ -14994,7 +15002,7 @@
         <v>75.900000000000006</v>
       </c>
     </row>
-    <row r="179" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A179" s="3" t="s">
         <v>659</v>
       </c>
@@ -15049,7 +15057,7 @@
       <c r="Z179" s="3"/>
       <c r="AA179" s="3"/>
     </row>
-    <row r="180" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A180" s="1" t="s">
         <v>662</v>
       </c>
@@ -15093,7 +15101,7 @@
         <v>83.1</v>
       </c>
     </row>
-    <row r="181" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A181" s="3" t="s">
         <v>664</v>
       </c>
@@ -19886,6 +19894,9 @@
       <c r="S272" s="11" t="s">
         <v>1387</v>
       </c>
+      <c r="V272">
+        <v>72.2</v>
+      </c>
     </row>
     <row r="273" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A273" s="3" t="s">
@@ -19931,7 +19942,9 @@
       <c r="S273" s="3"/>
       <c r="T273" s="3"/>
       <c r="U273" s="3"/>
-      <c r="V273" s="3"/>
+      <c r="V273" s="3">
+        <v>88.9</v>
+      </c>
       <c r="W273" s="3"/>
       <c r="X273" s="3"/>
       <c r="Y273" s="3"/>
@@ -19975,6 +19988,9 @@
       <c r="P274">
         <v>37</v>
       </c>
+      <c r="V274">
+        <v>70.2</v>
+      </c>
     </row>
     <row r="275" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A275" s="3" t="s">
@@ -20022,7 +20038,9 @@
       </c>
       <c r="T275" s="3"/>
       <c r="U275" s="3"/>
-      <c r="V275" s="3"/>
+      <c r="V275" s="3">
+        <v>82.9</v>
+      </c>
       <c r="W275" s="3"/>
       <c r="X275" s="3"/>
       <c r="Y275" s="3"/>
@@ -20069,8 +20087,11 @@
       <c r="S276" s="11" t="s">
         <v>1387</v>
       </c>
-    </row>
-    <row r="277" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V276">
+        <v>71.7</v>
+      </c>
+    </row>
+    <row r="277" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A277" s="3" t="s">
         <v>850</v>
       </c>
@@ -20114,14 +20135,16 @@
       <c r="S277" s="3"/>
       <c r="T277" s="3"/>
       <c r="U277" s="3"/>
-      <c r="V277" s="3"/>
+      <c r="V277" s="3" t="s">
+        <v>1386</v>
+      </c>
       <c r="W277" s="3"/>
       <c r="X277" s="3"/>
       <c r="Y277" s="3"/>
       <c r="Z277" s="3"/>
       <c r="AA277" s="3"/>
     </row>
-    <row r="278" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A278" s="1" t="s">
         <v>853</v>
       </c>
@@ -20158,8 +20181,11 @@
       <c r="P278">
         <v>37</v>
       </c>
-    </row>
-    <row r="279" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V278" s="46" t="s">
+        <v>1386</v>
+      </c>
+    </row>
+    <row r="279" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A279" s="3" t="s">
         <v>854</v>
       </c>
@@ -20209,14 +20235,16 @@
       </c>
       <c r="T279" s="3"/>
       <c r="U279" s="3"/>
-      <c r="V279" s="3"/>
+      <c r="V279" s="3">
+        <v>94.2</v>
+      </c>
       <c r="W279" s="3"/>
       <c r="X279" s="3"/>
       <c r="Y279" s="3"/>
       <c r="Z279" s="3"/>
       <c r="AA279" s="3"/>
     </row>
-    <row r="280" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A280" s="1" t="s">
         <v>855</v>
       </c>
@@ -20253,8 +20281,11 @@
       <c r="P280">
         <v>37</v>
       </c>
-    </row>
-    <row r="281" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V280">
+        <v>80.400000000000006</v>
+      </c>
+    </row>
+    <row r="281" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A281" s="3" t="s">
         <v>856</v>
       </c>
@@ -20298,7 +20329,9 @@
       <c r="S281" s="3"/>
       <c r="T281" s="3"/>
       <c r="U281" s="3"/>
-      <c r="V281" s="3"/>
+      <c r="V281" s="3">
+        <v>97.9</v>
+      </c>
       <c r="W281" s="3"/>
       <c r="X281" s="3"/>
       <c r="Y281" s="3"/>
@@ -20584,7 +20617,9 @@
       <c r="S287" s="3"/>
       <c r="T287" s="3"/>
       <c r="U287" s="3"/>
-      <c r="V287" s="3"/>
+      <c r="V287" s="3">
+        <v>101.6</v>
+      </c>
       <c r="W287" s="3"/>
       <c r="X287" s="3"/>
       <c r="Y287" s="3"/>
@@ -20628,6 +20663,9 @@
       <c r="P288">
         <v>37</v>
       </c>
+      <c r="V288">
+        <v>66.5</v>
+      </c>
     </row>
     <row r="289" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A289" s="3" t="s">
@@ -20673,7 +20711,9 @@
       <c r="S289" s="3"/>
       <c r="T289" s="3"/>
       <c r="U289" s="3"/>
-      <c r="V289" s="3"/>
+      <c r="V289" s="3">
+        <v>90.5</v>
+      </c>
       <c r="W289" s="3"/>
       <c r="X289" s="3"/>
       <c r="Y289" s="3"/>
@@ -20717,6 +20757,9 @@
       <c r="P290">
         <v>37</v>
       </c>
+      <c r="V290">
+        <v>83.6</v>
+      </c>
     </row>
     <row r="291" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A291" s="3" t="s">
@@ -20768,14 +20811,16 @@
       </c>
       <c r="T291" s="3"/>
       <c r="U291" s="3"/>
-      <c r="V291" s="3"/>
+      <c r="V291" s="3">
+        <v>80.7</v>
+      </c>
       <c r="W291" s="3"/>
       <c r="X291" s="3"/>
       <c r="Y291" s="3"/>
       <c r="Z291" s="3"/>
       <c r="AA291" s="3"/>
     </row>
-    <row r="292" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A292" s="1" t="s">
         <v>874</v>
       </c>
@@ -20816,7 +20861,7 @@
         <v>1391</v>
       </c>
     </row>
-    <row r="293" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A293" s="3" t="s">
         <v>875</v>
       </c>
@@ -20860,14 +20905,16 @@
       <c r="S293" s="3"/>
       <c r="T293" s="3"/>
       <c r="U293" s="3"/>
-      <c r="V293" s="3"/>
+      <c r="V293" s="3">
+        <v>101.7</v>
+      </c>
       <c r="W293" s="3"/>
       <c r="X293" s="3"/>
       <c r="Y293" s="3"/>
       <c r="Z293" s="3"/>
       <c r="AA293" s="3"/>
     </row>
-    <row r="294" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A294" s="1" t="s">
         <v>878</v>
       </c>
@@ -20908,7 +20955,7 @@
         <v>1391</v>
       </c>
     </row>
-    <row r="295" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A295" s="3" t="s">
         <v>880</v>
       </c>
@@ -20952,14 +20999,16 @@
       <c r="S295" s="3"/>
       <c r="T295" s="3"/>
       <c r="U295" s="3"/>
-      <c r="V295" s="3"/>
+      <c r="V295" s="3">
+        <v>122.5</v>
+      </c>
       <c r="W295" s="3"/>
       <c r="X295" s="3"/>
       <c r="Y295" s="3"/>
       <c r="Z295" s="3"/>
       <c r="AA295" s="3"/>
     </row>
-    <row r="296" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A296" s="1" t="s">
         <v>882</v>
       </c>
@@ -20995,6 +21044,9 @@
       </c>
       <c r="P296">
         <v>37</v>
+      </c>
+      <c r="V296">
+        <v>114.9</v>
       </c>
     </row>
     <row r="297" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -21267,6 +21319,9 @@
       <c r="P302">
         <v>37</v>
       </c>
+      <c r="V302">
+        <v>51.5</v>
+      </c>
     </row>
     <row r="303" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A303" s="3" t="s">
@@ -21312,7 +21367,9 @@
       <c r="S303" s="3"/>
       <c r="T303" s="3"/>
       <c r="U303" s="3"/>
-      <c r="V303" s="3"/>
+      <c r="V303" s="3">
+        <v>87.6</v>
+      </c>
       <c r="W303" s="3"/>
       <c r="X303" s="3"/>
       <c r="Y303" s="3"/>
@@ -21356,6 +21413,9 @@
       <c r="P304">
         <v>37</v>
       </c>
+      <c r="V304">
+        <v>78.099999999999994</v>
+      </c>
     </row>
     <row r="305" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A305" s="3" t="s">
@@ -21401,7 +21461,9 @@
       <c r="S305" s="3"/>
       <c r="T305" s="3"/>
       <c r="U305" s="3"/>
-      <c r="V305" s="3"/>
+      <c r="V305" s="3">
+        <v>82.3</v>
+      </c>
       <c r="W305" s="3"/>
       <c r="X305" s="3"/>
       <c r="Y305" s="3"/>
@@ -21445,8 +21507,11 @@
       <c r="P306">
         <v>37</v>
       </c>
-    </row>
-    <row r="307" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V306">
+        <v>90.7</v>
+      </c>
+    </row>
+    <row r="307" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A307" s="3" t="s">
         <v>899</v>
       </c>
@@ -21490,14 +21555,16 @@
       <c r="S307" s="3"/>
       <c r="T307" s="3"/>
       <c r="U307" s="3"/>
-      <c r="V307" s="3"/>
+      <c r="V307" s="3">
+        <v>88.2</v>
+      </c>
       <c r="W307" s="3"/>
       <c r="X307" s="3"/>
       <c r="Y307" s="3"/>
       <c r="Z307" s="3"/>
       <c r="AA307" s="3"/>
     </row>
-    <row r="308" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A308" s="1" t="s">
         <v>901</v>
       </c>
@@ -21534,8 +21601,11 @@
       <c r="P308">
         <v>37</v>
       </c>
-    </row>
-    <row r="309" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V308">
+        <v>70.2</v>
+      </c>
+    </row>
+    <row r="309" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A309" s="3" t="s">
         <v>902</v>
       </c>
@@ -21579,14 +21649,16 @@
       <c r="S309" s="3"/>
       <c r="T309" s="3"/>
       <c r="U309" s="3"/>
-      <c r="V309" s="3"/>
+      <c r="V309" s="3">
+        <v>63.5</v>
+      </c>
       <c r="W309" s="3"/>
       <c r="X309" s="3"/>
       <c r="Y309" s="3"/>
       <c r="Z309" s="3"/>
       <c r="AA309" s="3"/>
     </row>
-    <row r="310" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="310" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A310" s="1" t="s">
         <v>903</v>
       </c>
@@ -21623,8 +21695,11 @@
       <c r="P310">
         <v>37</v>
       </c>
-    </row>
-    <row r="311" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V310">
+        <v>85.4</v>
+      </c>
+    </row>
+    <row r="311" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A311" s="3" t="s">
         <v>904</v>
       </c>
@@ -21668,7 +21743,9 @@
       <c r="S311" s="3"/>
       <c r="T311" s="3"/>
       <c r="U311" s="3"/>
-      <c r="V311" s="3"/>
+      <c r="V311" s="3">
+        <v>106.9</v>
+      </c>
       <c r="W311" s="3"/>
       <c r="X311" s="3"/>
       <c r="Y311" s="3"/>
@@ -21935,7 +22012,9 @@
       <c r="S317" s="3"/>
       <c r="T317" s="3"/>
       <c r="U317" s="3"/>
-      <c r="V317" s="3"/>
+      <c r="V317" s="3">
+        <v>97.5</v>
+      </c>
       <c r="W317" s="3"/>
       <c r="X317" s="3"/>
       <c r="Y317" s="3"/>
@@ -21979,6 +22058,9 @@
       <c r="P318">
         <v>37</v>
       </c>
+      <c r="V318">
+        <v>86.6</v>
+      </c>
     </row>
     <row r="319" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A319" s="3" t="s">
@@ -22024,7 +22106,9 @@
       <c r="S319" s="3"/>
       <c r="T319" s="3"/>
       <c r="U319" s="3"/>
-      <c r="V319" s="3"/>
+      <c r="V319" s="3">
+        <v>62</v>
+      </c>
       <c r="W319" s="3"/>
       <c r="X319" s="3"/>
       <c r="Y319" s="3"/>
@@ -22077,7 +22161,9 @@
       <c r="S320" s="12"/>
       <c r="T320" s="30"/>
       <c r="U320" s="30"/>
-      <c r="V320" s="30"/>
+      <c r="V320" s="30">
+        <v>61.9</v>
+      </c>
       <c r="W320" s="30"/>
       <c r="X320" s="30"/>
       <c r="Y320" s="30"/>
@@ -22128,14 +22214,16 @@
       <c r="S321" s="3"/>
       <c r="T321" s="3"/>
       <c r="U321" s="3"/>
-      <c r="V321" s="3"/>
+      <c r="V321" s="3">
+        <v>83.8</v>
+      </c>
       <c r="W321" s="3"/>
       <c r="X321" s="3"/>
       <c r="Y321" s="3"/>
       <c r="Z321" s="3"/>
       <c r="AA321" s="3"/>
     </row>
-    <row r="322" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A322" s="1" t="s">
         <v>922</v>
       </c>
@@ -22172,8 +22260,11 @@
       <c r="P322">
         <v>37</v>
       </c>
-    </row>
-    <row r="323" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V322">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="323" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A323" s="3" t="s">
         <v>923</v>
       </c>
@@ -22217,14 +22308,16 @@
       <c r="S323" s="3"/>
       <c r="T323" s="3"/>
       <c r="U323" s="3"/>
-      <c r="V323" s="3"/>
+      <c r="V323" s="3">
+        <v>76.900000000000006</v>
+      </c>
       <c r="W323" s="3"/>
       <c r="X323" s="3"/>
       <c r="Y323" s="3"/>
       <c r="Z323" s="3"/>
       <c r="AA323" s="3"/>
     </row>
-    <row r="324" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="324" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A324" s="1" t="s">
         <v>924</v>
       </c>
@@ -22261,8 +22354,11 @@
       <c r="P324">
         <v>37</v>
       </c>
-    </row>
-    <row r="325" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V324">
+        <v>58.8</v>
+      </c>
+    </row>
+    <row r="325" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A325" s="3" t="s">
         <v>925</v>
       </c>
@@ -22306,14 +22402,16 @@
       <c r="S325" s="3"/>
       <c r="T325" s="3"/>
       <c r="U325" s="3"/>
-      <c r="V325" s="3"/>
+      <c r="V325" s="3">
+        <v>102.3</v>
+      </c>
       <c r="W325" s="3"/>
       <c r="X325" s="3"/>
       <c r="Y325" s="3"/>
       <c r="Z325" s="3"/>
       <c r="AA325" s="3"/>
     </row>
-    <row r="326" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="326" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A326" s="1" t="s">
         <v>926</v>
       </c>
@@ -22349,6 +22447,9 @@
       </c>
       <c r="P326">
         <v>37</v>
+      </c>
+      <c r="V326">
+        <v>91</v>
       </c>
     </row>
     <row r="327" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -22629,7 +22730,9 @@
       <c r="S332" s="12"/>
       <c r="T332" s="30"/>
       <c r="U332" s="30"/>
-      <c r="V332" s="30"/>
+      <c r="V332" s="30">
+        <v>85.2</v>
+      </c>
       <c r="W332" s="30"/>
       <c r="X332" s="30"/>
       <c r="Y332" s="30"/>
@@ -22684,7 +22787,9 @@
       <c r="S333" s="12"/>
       <c r="T333" s="30"/>
       <c r="U333" s="30"/>
-      <c r="V333" s="30"/>
+      <c r="V333" s="30">
+        <v>99.6</v>
+      </c>
       <c r="W333" s="30"/>
       <c r="X333" s="30"/>
       <c r="Y333" s="30"/>
@@ -22737,7 +22842,9 @@
       <c r="S334" s="12"/>
       <c r="T334" s="30"/>
       <c r="U334" s="30"/>
-      <c r="V334" s="30"/>
+      <c r="V334" s="30">
+        <v>95.4</v>
+      </c>
       <c r="W334" s="30"/>
       <c r="X334" s="30"/>
       <c r="Y334" s="30"/>
@@ -22788,7 +22895,9 @@
       <c r="S335" s="3"/>
       <c r="T335" s="3"/>
       <c r="U335" s="3"/>
-      <c r="V335" s="3"/>
+      <c r="V335" s="3">
+        <v>74.400000000000006</v>
+      </c>
       <c r="W335" s="3"/>
       <c r="X335" s="3"/>
       <c r="Y335" s="3"/>
@@ -22832,8 +22941,11 @@
       <c r="P336">
         <v>37</v>
       </c>
-    </row>
-    <row r="337" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V336">
+        <v>87.7</v>
+      </c>
+    </row>
+    <row r="337" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A337" s="3" t="s">
         <v>941</v>
       </c>
@@ -22883,14 +22995,16 @@
       </c>
       <c r="T337" s="30"/>
       <c r="U337" s="30"/>
-      <c r="V337" s="30"/>
+      <c r="V337" s="30">
+        <v>94.5</v>
+      </c>
       <c r="W337" s="30"/>
       <c r="X337" s="30"/>
       <c r="Y337" s="30"/>
       <c r="Z337" s="30"/>
       <c r="AA337" s="30"/>
     </row>
-    <row r="338" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="338" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A338" s="1" t="s">
         <v>943</v>
       </c>
@@ -22927,8 +23041,11 @@
       <c r="P338">
         <v>37</v>
       </c>
-    </row>
-    <row r="339" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V338">
+        <v>71.7</v>
+      </c>
+    </row>
+    <row r="339" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A339" s="3" t="s">
         <v>945</v>
       </c>
@@ -22976,14 +23093,16 @@
       <c r="S339" s="12"/>
       <c r="T339" s="30"/>
       <c r="U339" s="30"/>
-      <c r="V339" s="30"/>
+      <c r="V339" s="30">
+        <v>63.9</v>
+      </c>
       <c r="W339" s="30"/>
       <c r="X339" s="30"/>
       <c r="Y339" s="30"/>
       <c r="Z339" s="30"/>
       <c r="AA339" s="30"/>
     </row>
-    <row r="340" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="340" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A340" s="1" t="s">
         <v>946</v>
       </c>
@@ -23020,8 +23139,11 @@
       <c r="P340">
         <v>37</v>
       </c>
-    </row>
-    <row r="341" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V340">
+        <v>64.3</v>
+      </c>
+    </row>
+    <row r="341" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A341" s="3" t="s">
         <v>947</v>
       </c>
@@ -23065,7 +23187,9 @@
       <c r="S341" s="3"/>
       <c r="T341" s="3"/>
       <c r="U341" s="3"/>
-      <c r="V341" s="3"/>
+      <c r="V341" s="3">
+        <v>110.4</v>
+      </c>
       <c r="W341" s="3"/>
       <c r="X341" s="3"/>
       <c r="Y341" s="3"/>
@@ -23347,7 +23471,9 @@
       <c r="S347" s="3"/>
       <c r="T347" s="3"/>
       <c r="U347" s="3"/>
-      <c r="V347" s="3"/>
+      <c r="V347" s="3">
+        <v>85.3</v>
+      </c>
       <c r="W347" s="3"/>
       <c r="X347" s="3"/>
       <c r="Y347" s="3"/>
@@ -23391,6 +23517,9 @@
       <c r="P348">
         <v>37</v>
       </c>
+      <c r="V348">
+        <v>91.9</v>
+      </c>
     </row>
     <row r="349" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A349" s="3" t="s">
@@ -23436,7 +23565,9 @@
       <c r="S349" s="3"/>
       <c r="T349" s="3"/>
       <c r="U349" s="3"/>
-      <c r="V349" s="3"/>
+      <c r="V349" s="3">
+        <v>75.900000000000006</v>
+      </c>
       <c r="W349" s="3"/>
       <c r="X349" s="3"/>
       <c r="Y349" s="3"/>
@@ -23483,6 +23614,9 @@
       <c r="S350" s="11" t="s">
         <v>1387</v>
       </c>
+      <c r="V350">
+        <v>71.8</v>
+      </c>
     </row>
     <row r="351" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A351" s="3" t="s">
@@ -23528,14 +23662,16 @@
       <c r="S351" s="3"/>
       <c r="T351" s="3"/>
       <c r="U351" s="3"/>
-      <c r="V351" s="3"/>
+      <c r="V351" s="3">
+        <v>91.7</v>
+      </c>
       <c r="W351" s="3"/>
       <c r="X351" s="3"/>
       <c r="Y351" s="3"/>
       <c r="Z351" s="3"/>
       <c r="AA351" s="3"/>
     </row>
-    <row r="352" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="352" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A352" s="1" t="s">
         <v>969</v>
       </c>
@@ -23572,8 +23708,11 @@
       <c r="P352">
         <v>37</v>
       </c>
-    </row>
-    <row r="353" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V352">
+        <v>84.1</v>
+      </c>
+    </row>
+    <row r="353" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A353" s="3" t="s">
         <v>971</v>
       </c>
@@ -23616,14 +23755,16 @@
       <c r="S353" s="3"/>
       <c r="T353" s="3"/>
       <c r="U353" s="3"/>
-      <c r="V353" s="3"/>
+      <c r="V353" s="3">
+        <v>82.8</v>
+      </c>
       <c r="W353" s="3"/>
       <c r="X353" s="3"/>
       <c r="Y353" s="3"/>
       <c r="Z353" s="3"/>
       <c r="AA353" s="3"/>
     </row>
-    <row r="354" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="354" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A354" s="1" t="s">
         <v>972</v>
       </c>
@@ -23660,8 +23801,11 @@
       <c r="P354">
         <v>37</v>
       </c>
-    </row>
-    <row r="355" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V354">
+        <v>82.9</v>
+      </c>
+    </row>
+    <row r="355" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A355" s="3" t="s">
         <v>974</v>
       </c>
@@ -23714,7 +23858,7 @@
       <c r="Z355" s="3"/>
       <c r="AA355" s="3"/>
     </row>
-    <row r="356" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="356" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A356" s="1" t="s">
         <v>976</v>
       </c>
@@ -23760,7 +23904,9 @@
       <c r="S356" s="12"/>
       <c r="T356" s="30"/>
       <c r="U356" s="30"/>
-      <c r="V356" s="30"/>
+      <c r="V356" s="30">
+        <v>87</v>
+      </c>
       <c r="W356" s="30"/>
       <c r="X356" s="30"/>
       <c r="Y356" s="30"/>
@@ -33794,6 +33940,9 @@
       <c r="S542" s="12" t="s">
         <v>1391</v>
       </c>
+      <c r="X542">
+        <v>328</v>
+      </c>
     </row>
     <row r="543" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A543" s="3" t="s">
@@ -33839,9 +33988,13 @@
       <c r="S543" s="3"/>
       <c r="T543" s="3"/>
       <c r="U543" s="3"/>
-      <c r="V543" s="3"/>
+      <c r="V543" s="3">
+        <v>31.7</v>
+      </c>
       <c r="W543" s="3"/>
-      <c r="X543" s="3"/>
+      <c r="X543">
+        <v>328</v>
+      </c>
       <c r="Y543" s="3"/>
       <c r="Z543" s="3"/>
       <c r="AA543" s="3"/>
@@ -33885,6 +34038,9 @@
       </c>
       <c r="S544" s="12" t="s">
         <v>1391</v>
+      </c>
+      <c r="X544">
+        <v>328</v>
       </c>
     </row>
     <row r="545" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -33931,9 +34087,13 @@
       <c r="S545" s="3"/>
       <c r="T545" s="3"/>
       <c r="U545" s="3"/>
-      <c r="V545" s="3"/>
+      <c r="V545" s="3">
+        <v>26.7</v>
+      </c>
       <c r="W545" s="3"/>
-      <c r="X545" s="3"/>
+      <c r="X545">
+        <v>328</v>
+      </c>
       <c r="Y545" s="3"/>
       <c r="Z545" s="3"/>
       <c r="AA545" s="3"/>
@@ -33974,6 +34134,12 @@
       </c>
       <c r="P546">
         <v>37</v>
+      </c>
+      <c r="V546">
+        <v>23.8</v>
+      </c>
+      <c r="X546">
+        <v>328</v>
       </c>
     </row>
     <row r="547" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -34020,9 +34186,13 @@
       <c r="S547" s="3"/>
       <c r="T547" s="3"/>
       <c r="U547" s="3"/>
-      <c r="V547" s="3"/>
+      <c r="V547" s="3">
+        <v>28.5</v>
+      </c>
       <c r="W547" s="3"/>
-      <c r="X547" s="3"/>
+      <c r="X547">
+        <v>328</v>
+      </c>
       <c r="Y547" s="3"/>
       <c r="Z547" s="3"/>
       <c r="AA547" s="3"/>
@@ -34063,6 +34233,12 @@
       </c>
       <c r="P548">
         <v>37</v>
+      </c>
+      <c r="V548">
+        <v>28.2</v>
+      </c>
+      <c r="X548">
+        <v>328</v>
       </c>
     </row>
     <row r="549" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -34109,9 +34285,13 @@
       <c r="S549" s="3"/>
       <c r="T549" s="3"/>
       <c r="U549" s="3"/>
-      <c r="V549" s="3"/>
+      <c r="V549" s="3">
+        <v>26.7</v>
+      </c>
       <c r="W549" s="3"/>
-      <c r="X549" s="3"/>
+      <c r="X549">
+        <v>328</v>
+      </c>
       <c r="Y549" s="3"/>
       <c r="Z549" s="3"/>
       <c r="AA549" s="3"/>
@@ -34152,6 +34332,12 @@
       </c>
       <c r="P550">
         <v>37</v>
+      </c>
+      <c r="V550">
+        <v>24.6</v>
+      </c>
+      <c r="X550">
+        <v>328</v>
       </c>
     </row>
     <row r="551" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -34198,9 +34384,13 @@
       <c r="S551" s="3"/>
       <c r="T551" s="3"/>
       <c r="U551" s="3"/>
-      <c r="V551" s="3"/>
+      <c r="V551" s="3">
+        <v>29.7</v>
+      </c>
       <c r="W551" s="3"/>
-      <c r="X551" s="3"/>
+      <c r="X551">
+        <v>328</v>
+      </c>
       <c r="Y551" s="3"/>
       <c r="Z551" s="3"/>
       <c r="AA551" s="3"/>
@@ -34244,6 +34434,9 @@
       </c>
       <c r="S552" s="17" t="s">
         <v>1391</v>
+      </c>
+      <c r="X552">
+        <v>328</v>
       </c>
     </row>
     <row r="553" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -34290,9 +34483,13 @@
       <c r="S553" s="3"/>
       <c r="T553" s="3"/>
       <c r="U553" s="3"/>
-      <c r="V553" s="3"/>
+      <c r="V553" s="3">
+        <v>24.7</v>
+      </c>
       <c r="W553" s="3"/>
-      <c r="X553" s="3"/>
+      <c r="X553">
+        <v>328</v>
+      </c>
       <c r="Y553" s="3"/>
       <c r="Z553" s="3"/>
       <c r="AA553" s="3"/>
@@ -34336,6 +34533,9 @@
       </c>
       <c r="S554" s="17" t="s">
         <v>1391</v>
+      </c>
+      <c r="X554">
+        <v>328</v>
       </c>
     </row>
     <row r="555" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -34382,9 +34582,13 @@
       <c r="S555" s="3"/>
       <c r="T555" s="3"/>
       <c r="U555" s="3"/>
-      <c r="V555" s="3"/>
+      <c r="V555" s="3">
+        <v>30.1</v>
+      </c>
       <c r="W555" s="3"/>
-      <c r="X555" s="3"/>
+      <c r="X555">
+        <v>328</v>
+      </c>
       <c r="Y555" s="3"/>
       <c r="Z555" s="3"/>
       <c r="AA555" s="3"/>
@@ -34425,6 +34629,12 @@
       </c>
       <c r="P556">
         <v>57</v>
+      </c>
+      <c r="V556">
+        <v>28.2</v>
+      </c>
+      <c r="X556">
+        <v>328</v>
       </c>
     </row>
     <row r="557" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -34471,9 +34681,13 @@
       <c r="S557" s="3"/>
       <c r="T557" s="3"/>
       <c r="U557" s="3"/>
-      <c r="V557" s="3"/>
+      <c r="V557" s="3">
+        <v>24.1</v>
+      </c>
       <c r="W557" s="3"/>
-      <c r="X557" s="3"/>
+      <c r="X557">
+        <v>328</v>
+      </c>
       <c r="Y557" s="3"/>
       <c r="Z557" s="3"/>
       <c r="AA557" s="3"/>
@@ -34517,6 +34731,9 @@
       </c>
       <c r="S558" s="12" t="s">
         <v>1391</v>
+      </c>
+      <c r="X558">
+        <v>328</v>
       </c>
     </row>
     <row r="559" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -34567,7 +34784,9 @@
       <c r="U559" s="3"/>
       <c r="V559" s="3"/>
       <c r="W559" s="3"/>
-      <c r="X559" s="3"/>
+      <c r="X559">
+        <v>328</v>
+      </c>
       <c r="Y559" s="3"/>
       <c r="Z559" s="3"/>
       <c r="AA559" s="3"/>
@@ -34611,6 +34830,9 @@
       </c>
       <c r="S560" s="12" t="s">
         <v>1391</v>
+      </c>
+      <c r="X560">
+        <v>328</v>
       </c>
     </row>
     <row r="561" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -34657,9 +34879,13 @@
       <c r="S561" s="3"/>
       <c r="T561" s="3"/>
       <c r="U561" s="3"/>
-      <c r="V561" s="3"/>
+      <c r="V561" s="3">
+        <v>21.4</v>
+      </c>
       <c r="W561" s="3"/>
-      <c r="X561" s="3"/>
+      <c r="X561">
+        <v>328</v>
+      </c>
       <c r="Y561" s="3"/>
       <c r="Z561" s="3"/>
       <c r="AA561" s="3"/>
@@ -34700,6 +34926,12 @@
       </c>
       <c r="P562">
         <v>37</v>
+      </c>
+      <c r="V562">
+        <v>33.200000000000003</v>
+      </c>
+      <c r="X562">
+        <v>328</v>
       </c>
     </row>
     <row r="563" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -34746,9 +34978,13 @@
       <c r="S563" s="3"/>
       <c r="T563" s="3"/>
       <c r="U563" s="3"/>
-      <c r="V563" s="3"/>
+      <c r="V563" s="3">
+        <v>31.2</v>
+      </c>
       <c r="W563" s="3"/>
-      <c r="X563" s="3"/>
+      <c r="X563">
+        <v>328</v>
+      </c>
       <c r="Y563" s="3"/>
       <c r="Z563" s="3"/>
       <c r="AA563" s="3"/>
@@ -34789,6 +35025,12 @@
       </c>
       <c r="P564">
         <v>37</v>
+      </c>
+      <c r="V564">
+        <v>36.9</v>
+      </c>
+      <c r="X564">
+        <v>328</v>
       </c>
     </row>
     <row r="565" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -34835,9 +35077,13 @@
       <c r="S565" s="3"/>
       <c r="T565" s="3"/>
       <c r="U565" s="3"/>
-      <c r="V565" s="3"/>
+      <c r="V565" s="3">
+        <v>29.4</v>
+      </c>
       <c r="W565" s="3"/>
-      <c r="X565" s="3"/>
+      <c r="X565">
+        <v>328</v>
+      </c>
       <c r="Y565" s="3"/>
       <c r="Z565" s="3"/>
       <c r="AA565" s="3"/>
@@ -34878,6 +35124,12 @@
       </c>
       <c r="P566">
         <v>37</v>
+      </c>
+      <c r="V566">
+        <v>19.600000000000001</v>
+      </c>
+      <c r="X566">
+        <v>328</v>
       </c>
     </row>
     <row r="567" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -34924,9 +35176,13 @@
       <c r="S567" s="3"/>
       <c r="T567" s="3"/>
       <c r="U567" s="3"/>
-      <c r="V567" s="3"/>
+      <c r="V567" s="3">
+        <v>33.6</v>
+      </c>
       <c r="W567" s="3"/>
-      <c r="X567" s="3"/>
+      <c r="X567">
+        <v>328</v>
+      </c>
       <c r="Y567" s="3"/>
       <c r="Z567" s="3"/>
       <c r="AA567" s="3"/>
@@ -34967,6 +35223,12 @@
       </c>
       <c r="P568">
         <v>57</v>
+      </c>
+      <c r="V568">
+        <v>27.7</v>
+      </c>
+      <c r="X568">
+        <v>328</v>
       </c>
     </row>
     <row r="569" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -35013,9 +35275,13 @@
       <c r="S569" s="3"/>
       <c r="T569" s="3"/>
       <c r="U569" s="3"/>
-      <c r="V569" s="3"/>
+      <c r="V569" s="3">
+        <v>30.2</v>
+      </c>
       <c r="W569" s="3"/>
-      <c r="X569" s="3"/>
+      <c r="X569">
+        <v>328</v>
+      </c>
       <c r="Y569" s="3"/>
       <c r="Z569" s="3"/>
       <c r="AA569" s="3"/>
@@ -35056,6 +35322,12 @@
       </c>
       <c r="P570">
         <v>57</v>
+      </c>
+      <c r="V570">
+        <v>34.299999999999997</v>
+      </c>
+      <c r="X570">
+        <v>328</v>
       </c>
     </row>
     <row r="571" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -35106,7 +35378,9 @@
       <c r="U571" s="3"/>
       <c r="V571" s="3"/>
       <c r="W571" s="3"/>
-      <c r="X571" s="3"/>
+      <c r="X571">
+        <v>328</v>
+      </c>
       <c r="Y571" s="3"/>
       <c r="Z571" s="3"/>
       <c r="AA571" s="3"/>
@@ -35147,6 +35421,12 @@
       </c>
       <c r="P572">
         <v>37</v>
+      </c>
+      <c r="V572">
+        <v>28.2</v>
+      </c>
+      <c r="X572">
+        <v>328</v>
       </c>
     </row>
     <row r="573" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -35191,9 +35471,13 @@
       <c r="S573" s="3"/>
       <c r="T573" s="3"/>
       <c r="U573" s="3"/>
-      <c r="V573" s="3"/>
+      <c r="V573" s="3">
+        <v>30</v>
+      </c>
       <c r="W573" s="3"/>
-      <c r="X573" s="3"/>
+      <c r="X573">
+        <v>328</v>
+      </c>
       <c r="Y573" s="3"/>
       <c r="Z573" s="3"/>
       <c r="AA573" s="3"/>
@@ -35237,6 +35521,9 @@
       </c>
       <c r="S574" s="12" t="s">
         <v>1391</v>
+      </c>
+      <c r="X574">
+        <v>328</v>
       </c>
     </row>
     <row r="575" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -35287,7 +35574,9 @@
       <c r="U575" s="3"/>
       <c r="V575" s="3"/>
       <c r="W575" s="3"/>
-      <c r="X575" s="3"/>
+      <c r="X575">
+        <v>328</v>
+      </c>
       <c r="Y575" s="3"/>
       <c r="Z575" s="3"/>
       <c r="AA575" s="3"/>
@@ -35331,6 +35620,9 @@
       </c>
       <c r="S576" s="12" t="s">
         <v>1391</v>
+      </c>
+      <c r="X576">
+        <v>328</v>
       </c>
     </row>
     <row r="577" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -35377,9 +35669,13 @@
       <c r="S577" s="3"/>
       <c r="T577" s="3"/>
       <c r="U577" s="3"/>
-      <c r="V577" s="3"/>
+      <c r="V577" s="3">
+        <v>24.6</v>
+      </c>
       <c r="W577" s="3"/>
-      <c r="X577" s="3"/>
+      <c r="X577">
+        <v>328</v>
+      </c>
       <c r="Y577" s="3"/>
       <c r="Z577" s="3"/>
       <c r="AA577" s="3"/>
@@ -35423,6 +35719,9 @@
       </c>
       <c r="S578" s="17" t="s">
         <v>1391</v>
+      </c>
+      <c r="X578">
+        <v>328</v>
       </c>
     </row>
     <row r="579" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -35469,9 +35768,13 @@
       <c r="S579" s="3"/>
       <c r="T579" s="3"/>
       <c r="U579" s="3"/>
-      <c r="V579" s="3"/>
+      <c r="V579" s="3">
+        <v>30.8</v>
+      </c>
       <c r="W579" s="3"/>
-      <c r="X579" s="3"/>
+      <c r="X579">
+        <v>328</v>
+      </c>
       <c r="Y579" s="3"/>
       <c r="Z579" s="3"/>
       <c r="AA579" s="3"/>
@@ -35512,6 +35815,12 @@
       </c>
       <c r="P580">
         <v>37</v>
+      </c>
+      <c r="V580">
+        <v>28.4</v>
+      </c>
+      <c r="X580">
+        <v>328</v>
       </c>
     </row>
     <row r="581" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -35558,9 +35867,13 @@
       <c r="S581" s="3"/>
       <c r="T581" s="3"/>
       <c r="U581" s="3"/>
-      <c r="V581" s="3"/>
+      <c r="V581" s="3">
+        <v>29.3</v>
+      </c>
       <c r="W581" s="3"/>
-      <c r="X581" s="3"/>
+      <c r="X581">
+        <v>328</v>
+      </c>
       <c r="Y581" s="3"/>
       <c r="Z581" s="3"/>
       <c r="AA581" s="3"/>
@@ -35601,6 +35914,12 @@
       </c>
       <c r="P582">
         <v>57</v>
+      </c>
+      <c r="V582">
+        <v>28.4</v>
+      </c>
+      <c r="X582">
+        <v>328</v>
       </c>
     </row>
     <row r="583" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -35651,7 +35970,9 @@
       <c r="U583" s="3"/>
       <c r="V583" s="3"/>
       <c r="W583" s="3"/>
-      <c r="X583" s="3"/>
+      <c r="X583">
+        <v>328</v>
+      </c>
       <c r="Y583" s="3"/>
       <c r="Z583" s="3"/>
       <c r="AA583" s="3"/>
@@ -35692,6 +36013,12 @@
       </c>
       <c r="P584">
         <v>57</v>
+      </c>
+      <c r="V584">
+        <v>23.4</v>
+      </c>
+      <c r="X584">
+        <v>328</v>
       </c>
     </row>
     <row r="585" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -35738,9 +36065,13 @@
       <c r="S585" s="3"/>
       <c r="T585" s="3"/>
       <c r="U585" s="3"/>
-      <c r="V585" s="3"/>
+      <c r="V585" s="3">
+        <v>33.4</v>
+      </c>
       <c r="W585" s="3"/>
-      <c r="X585" s="3"/>
+      <c r="X585">
+        <v>328</v>
+      </c>
       <c r="Y585" s="3"/>
       <c r="Z585" s="3"/>
       <c r="AA585" s="3"/>
@@ -35781,6 +36112,12 @@
       </c>
       <c r="P586">
         <v>57</v>
+      </c>
+      <c r="V586">
+        <v>34.5</v>
+      </c>
+      <c r="X586">
+        <v>328</v>
       </c>
     </row>
     <row r="587" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -35827,9 +36164,13 @@
       <c r="S587" s="3"/>
       <c r="T587" s="3"/>
       <c r="U587" s="3"/>
-      <c r="V587" s="3"/>
+      <c r="V587" s="3">
+        <v>34.4</v>
+      </c>
       <c r="W587" s="3"/>
-      <c r="X587" s="3"/>
+      <c r="X587">
+        <v>328</v>
+      </c>
       <c r="Y587" s="3"/>
       <c r="Z587" s="3"/>
       <c r="AA587" s="3"/>
@@ -35873,6 +36214,9 @@
       </c>
       <c r="S588" s="12" t="s">
         <v>1391</v>
+      </c>
+      <c r="X588">
+        <v>328</v>
       </c>
     </row>
     <row r="589" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -35923,7 +36267,9 @@
       <c r="U589" s="3"/>
       <c r="V589" s="3"/>
       <c r="W589" s="3"/>
-      <c r="X589" s="3"/>
+      <c r="X589">
+        <v>328</v>
+      </c>
       <c r="Y589" s="3"/>
       <c r="Z589" s="3"/>
       <c r="AA589" s="3"/>
@@ -35967,6 +36313,9 @@
       </c>
       <c r="S590" s="12" t="s">
         <v>1391</v>
+      </c>
+      <c r="X590">
+        <v>328</v>
       </c>
     </row>
     <row r="591" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -36013,9 +36362,13 @@
       <c r="S591" s="3"/>
       <c r="T591" s="3"/>
       <c r="U591" s="3"/>
-      <c r="V591" s="3"/>
+      <c r="V591" s="3">
+        <v>24.1</v>
+      </c>
       <c r="W591" s="3"/>
-      <c r="X591" s="3"/>
+      <c r="X591">
+        <v>328</v>
+      </c>
       <c r="Y591" s="3"/>
       <c r="Z591" s="3"/>
       <c r="AA591" s="3"/>
@@ -36056,6 +36409,12 @@
       </c>
       <c r="P592">
         <v>37</v>
+      </c>
+      <c r="V592">
+        <v>28.4</v>
+      </c>
+      <c r="X592">
+        <v>328</v>
       </c>
     </row>
     <row r="593" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -36102,9 +36461,13 @@
       <c r="S593" s="3"/>
       <c r="T593" s="3"/>
       <c r="U593" s="3"/>
-      <c r="V593" s="3"/>
+      <c r="V593" s="3">
+        <v>33.200000000000003</v>
+      </c>
       <c r="W593" s="3"/>
-      <c r="X593" s="3"/>
+      <c r="X593">
+        <v>328</v>
+      </c>
       <c r="Y593" s="3"/>
       <c r="Z593" s="3"/>
       <c r="AA593" s="3"/>
@@ -36149,6 +36512,9 @@
       <c r="S594" s="17" t="s">
         <v>1391</v>
       </c>
+      <c r="X594">
+        <v>328</v>
+      </c>
     </row>
     <row r="595" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A595" s="3" t="s">
@@ -36198,9 +36564,13 @@
       </c>
       <c r="T595" s="11"/>
       <c r="U595" s="11"/>
-      <c r="V595" s="11"/>
+      <c r="V595" s="11">
+        <v>33.6</v>
+      </c>
       <c r="W595" s="11"/>
-      <c r="X595" s="11"/>
+      <c r="X595">
+        <v>328</v>
+      </c>
       <c r="Y595" s="11"/>
       <c r="Z595" s="11"/>
       <c r="AA595" s="11"/>
@@ -36244,6 +36614,9 @@
       </c>
       <c r="S596" s="17" t="s">
         <v>1391</v>
+      </c>
+      <c r="X596">
+        <v>328</v>
       </c>
     </row>
     <row r="597" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -36294,7 +36667,9 @@
       <c r="U597" s="3"/>
       <c r="V597" s="3"/>
       <c r="W597" s="3"/>
-      <c r="X597" s="3"/>
+      <c r="X597">
+        <v>328</v>
+      </c>
       <c r="Y597" s="3"/>
       <c r="Z597" s="3"/>
       <c r="AA597" s="3"/>
@@ -36335,6 +36710,12 @@
       </c>
       <c r="P598">
         <v>57</v>
+      </c>
+      <c r="V598">
+        <v>29.1</v>
+      </c>
+      <c r="X598">
+        <v>328</v>
       </c>
     </row>
     <row r="599" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -36381,9 +36762,13 @@
       <c r="S599" s="3"/>
       <c r="T599" s="3"/>
       <c r="U599" s="3"/>
-      <c r="V599" s="3"/>
+      <c r="V599" s="3">
+        <v>35.799999999999997</v>
+      </c>
       <c r="W599" s="3"/>
-      <c r="X599" s="3"/>
+      <c r="X599">
+        <v>328</v>
+      </c>
       <c r="Y599" s="3"/>
       <c r="Z599" s="3"/>
       <c r="AA599" s="3"/>
@@ -36424,6 +36809,12 @@
       </c>
       <c r="P600">
         <v>57</v>
+      </c>
+      <c r="V600">
+        <v>27.5</v>
+      </c>
+      <c r="X600">
+        <v>328</v>
       </c>
     </row>
     <row r="601" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -36470,9 +36861,13 @@
       <c r="S601" s="3"/>
       <c r="T601" s="3"/>
       <c r="U601" s="3"/>
-      <c r="V601" s="3"/>
+      <c r="V601" s="3">
+        <v>37</v>
+      </c>
       <c r="W601" s="3"/>
-      <c r="X601" s="3"/>
+      <c r="X601">
+        <v>328</v>
+      </c>
       <c r="Y601" s="3"/>
       <c r="Z601" s="3"/>
       <c r="AA601" s="3"/>
@@ -36516,6 +36911,9 @@
       </c>
       <c r="S602" s="12" t="s">
         <v>1391</v>
+      </c>
+      <c r="X602">
+        <v>328</v>
       </c>
     </row>
     <row r="603" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -36562,9 +36960,13 @@
       <c r="S603" s="3"/>
       <c r="T603" s="3"/>
       <c r="U603" s="3"/>
-      <c r="V603" s="3"/>
+      <c r="V603" s="3">
+        <v>24.9</v>
+      </c>
       <c r="W603" s="3"/>
-      <c r="X603" s="3"/>
+      <c r="X603">
+        <v>328</v>
+      </c>
       <c r="Y603" s="3"/>
       <c r="Z603" s="3"/>
       <c r="AA603" s="3"/>
@@ -36605,6 +37007,12 @@
       </c>
       <c r="P604">
         <v>37</v>
+      </c>
+      <c r="V604">
+        <v>37.299999999999997</v>
+      </c>
+      <c r="X604">
+        <v>328</v>
       </c>
     </row>
     <row r="605" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -36651,9 +37059,13 @@
       <c r="S605" s="3"/>
       <c r="T605" s="3"/>
       <c r="U605" s="3"/>
-      <c r="V605" s="3"/>
+      <c r="V605" s="3">
+        <v>25.8</v>
+      </c>
       <c r="W605" s="3"/>
-      <c r="X605" s="3"/>
+      <c r="X605">
+        <v>328</v>
+      </c>
       <c r="Y605" s="3"/>
       <c r="Z605" s="3"/>
       <c r="AA605" s="3"/>
@@ -36694,6 +37106,12 @@
       </c>
       <c r="P606">
         <v>37</v>
+      </c>
+      <c r="V606">
+        <v>33.6</v>
+      </c>
+      <c r="X606">
+        <v>328</v>
       </c>
     </row>
     <row r="607" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -36740,9 +37158,13 @@
       <c r="S607" s="3"/>
       <c r="T607" s="3"/>
       <c r="U607" s="3"/>
-      <c r="V607" s="3"/>
+      <c r="V607" s="3">
+        <v>25.4</v>
+      </c>
       <c r="W607" s="3"/>
-      <c r="X607" s="3"/>
+      <c r="X607">
+        <v>328</v>
+      </c>
       <c r="Y607" s="3"/>
       <c r="Z607" s="3"/>
       <c r="AA607" s="3"/>
@@ -36783,6 +37205,12 @@
       </c>
       <c r="P608">
         <v>37</v>
+      </c>
+      <c r="V608">
+        <v>30.7</v>
+      </c>
+      <c r="X608">
+        <v>328</v>
       </c>
     </row>
     <row r="609" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -36829,9 +37257,13 @@
       <c r="S609" s="3"/>
       <c r="T609" s="3"/>
       <c r="U609" s="3"/>
-      <c r="V609" s="3"/>
+      <c r="V609" s="3">
+        <v>33.9</v>
+      </c>
       <c r="W609" s="3"/>
-      <c r="X609" s="3"/>
+      <c r="X609">
+        <v>328</v>
+      </c>
       <c r="Y609" s="3"/>
       <c r="Z609" s="3"/>
       <c r="AA609" s="3"/>
@@ -36872,6 +37304,12 @@
       </c>
       <c r="P610">
         <v>37</v>
+      </c>
+      <c r="V610">
+        <v>24.4</v>
+      </c>
+      <c r="X610">
+        <v>328</v>
       </c>
     </row>
     <row r="611" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -36922,7 +37360,9 @@
       <c r="U611" s="3"/>
       <c r="V611" s="3"/>
       <c r="W611" s="3"/>
-      <c r="X611" s="3"/>
+      <c r="X611">
+        <v>328</v>
+      </c>
       <c r="Y611" s="3"/>
       <c r="Z611" s="3"/>
       <c r="AA611" s="3"/>
@@ -36963,6 +37403,12 @@
       </c>
       <c r="P612">
         <v>57</v>
+      </c>
+      <c r="V612">
+        <v>27.4</v>
+      </c>
+      <c r="X612">
+        <v>328</v>
       </c>
     </row>
     <row r="613" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -37009,9 +37455,13 @@
       <c r="S613" s="3"/>
       <c r="T613" s="3"/>
       <c r="U613" s="3"/>
-      <c r="V613" s="3"/>
+      <c r="V613" s="3">
+        <v>31.6</v>
+      </c>
       <c r="W613" s="3"/>
-      <c r="X613" s="3"/>
+      <c r="X613">
+        <v>328</v>
+      </c>
       <c r="Y613" s="3"/>
       <c r="Z613" s="3"/>
       <c r="AA613" s="3"/>
@@ -37052,6 +37502,12 @@
       </c>
       <c r="P614">
         <v>57</v>
+      </c>
+      <c r="V614">
+        <v>29.4</v>
+      </c>
+      <c r="X614">
+        <v>328</v>
       </c>
     </row>
     <row r="615" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -37098,9 +37554,13 @@
       <c r="S615" s="3"/>
       <c r="T615" s="3"/>
       <c r="U615" s="3"/>
-      <c r="V615" s="3"/>
+      <c r="V615" s="3">
+        <v>32.9</v>
+      </c>
       <c r="W615" s="3"/>
-      <c r="X615" s="3"/>
+      <c r="X615">
+        <v>328</v>
+      </c>
       <c r="Y615" s="3"/>
       <c r="Z615" s="3"/>
       <c r="AA615" s="3"/>
@@ -37144,6 +37604,9 @@
       </c>
       <c r="S616" s="17" t="s">
         <v>1391</v>
+      </c>
+      <c r="X616">
+        <v>328</v>
       </c>
     </row>
     <row r="617" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -37190,9 +37653,13 @@
       <c r="S617" s="3"/>
       <c r="T617" s="3"/>
       <c r="U617" s="3"/>
-      <c r="V617" s="3"/>
+      <c r="V617" s="3">
+        <v>28.1</v>
+      </c>
       <c r="W617" s="3"/>
-      <c r="X617" s="3"/>
+      <c r="X617">
+        <v>328</v>
+      </c>
       <c r="Y617" s="3"/>
       <c r="Z617" s="3"/>
       <c r="AA617" s="3"/>
@@ -37233,6 +37700,12 @@
       </c>
       <c r="P618">
         <v>37</v>
+      </c>
+      <c r="V618">
+        <v>25.4</v>
+      </c>
+      <c r="X618">
+        <v>328</v>
       </c>
     </row>
     <row r="619" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -37279,9 +37752,13 @@
       <c r="S619" s="3"/>
       <c r="T619" s="3"/>
       <c r="U619" s="3"/>
-      <c r="V619" s="3"/>
+      <c r="V619" s="3">
+        <v>29.3</v>
+      </c>
       <c r="W619" s="3"/>
-      <c r="X619" s="3"/>
+      <c r="X619">
+        <v>328</v>
+      </c>
       <c r="Y619" s="3"/>
       <c r="Z619" s="3"/>
       <c r="AA619" s="3"/>
@@ -37325,6 +37802,9 @@
       </c>
       <c r="S620" s="12" t="s">
         <v>1391</v>
+      </c>
+      <c r="X620">
+        <v>328</v>
       </c>
     </row>
     <row r="621" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -37371,9 +37851,13 @@
       <c r="S621" s="3"/>
       <c r="T621" s="3"/>
       <c r="U621" s="3"/>
-      <c r="V621" s="3"/>
+      <c r="V621" s="3">
+        <v>26.4</v>
+      </c>
       <c r="W621" s="3"/>
-      <c r="X621" s="3"/>
+      <c r="X621">
+        <v>328</v>
+      </c>
       <c r="Y621" s="3"/>
       <c r="Z621" s="3"/>
       <c r="AA621" s="3"/>
@@ -37414,6 +37898,12 @@
       </c>
       <c r="P622">
         <v>37</v>
+      </c>
+      <c r="V622">
+        <v>31.1</v>
+      </c>
+      <c r="X622">
+        <v>328</v>
       </c>
     </row>
     <row r="623" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -37460,9 +37950,13 @@
       <c r="S623" s="3"/>
       <c r="T623" s="3"/>
       <c r="U623" s="3"/>
-      <c r="V623" s="3"/>
+      <c r="V623" s="3">
+        <v>27.9</v>
+      </c>
       <c r="W623" s="3"/>
-      <c r="X623" s="3"/>
+      <c r="X623">
+        <v>328</v>
+      </c>
       <c r="Y623" s="3"/>
       <c r="Z623" s="3"/>
       <c r="AA623" s="3"/>
@@ -37503,6 +37997,12 @@
       </c>
       <c r="P624">
         <v>37</v>
+      </c>
+      <c r="V624">
+        <v>24.9</v>
+      </c>
+      <c r="X624">
+        <v>328</v>
       </c>
     </row>
     <row r="625" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -37549,9 +38049,13 @@
       <c r="S625" s="3"/>
       <c r="T625" s="3"/>
       <c r="U625" s="3"/>
-      <c r="V625" s="3"/>
+      <c r="V625" s="3">
+        <v>30.1</v>
+      </c>
       <c r="W625" s="3"/>
-      <c r="X625" s="3"/>
+      <c r="X625">
+        <v>328</v>
+      </c>
       <c r="Y625" s="3"/>
       <c r="Z625" s="3"/>
       <c r="AA625" s="3"/>
@@ -37592,6 +38096,12 @@
       </c>
       <c r="P626">
         <v>37</v>
+      </c>
+      <c r="V626">
+        <v>25.5</v>
+      </c>
+      <c r="X626">
+        <v>328</v>
       </c>
     </row>
     <row r="627" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -37638,9 +38148,13 @@
       <c r="S627" s="3"/>
       <c r="T627" s="3"/>
       <c r="U627" s="3"/>
-      <c r="V627" s="3"/>
+      <c r="V627" s="3">
+        <v>27.3</v>
+      </c>
       <c r="W627" s="3"/>
-      <c r="X627" s="3"/>
+      <c r="X627">
+        <v>328</v>
+      </c>
       <c r="Y627" s="3"/>
       <c r="Z627" s="3"/>
       <c r="AA627" s="3"/>
@@ -37681,6 +38195,12 @@
       </c>
       <c r="P628">
         <v>57</v>
+      </c>
+      <c r="V628">
+        <v>31.1</v>
+      </c>
+      <c r="X628">
+        <v>328</v>
       </c>
     </row>
     <row r="629" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -37727,9 +38247,13 @@
       <c r="S629" s="3"/>
       <c r="T629" s="3"/>
       <c r="U629" s="3"/>
-      <c r="V629" s="3"/>
+      <c r="V629" s="3">
+        <v>34.9</v>
+      </c>
       <c r="W629" s="3"/>
-      <c r="X629" s="3"/>
+      <c r="X629">
+        <v>328</v>
+      </c>
       <c r="Y629" s="3"/>
       <c r="Z629" s="3"/>
       <c r="AA629" s="3"/>
@@ -37770,6 +38294,12 @@
       </c>
       <c r="P630">
         <v>57</v>
+      </c>
+      <c r="V630">
+        <v>32.4</v>
+      </c>
+      <c r="X630">
+        <v>328</v>
       </c>
     </row>
     <row r="631" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -37816,9 +38346,13 @@
       <c r="S631" s="3"/>
       <c r="T631" s="3"/>
       <c r="U631" s="3"/>
-      <c r="V631" s="3"/>
+      <c r="V631" s="3">
+        <v>32.700000000000003</v>
+      </c>
       <c r="W631" s="3"/>
-      <c r="X631" s="3"/>
+      <c r="X631">
+        <v>328</v>
+      </c>
       <c r="Y631" s="3"/>
       <c r="Z631" s="3"/>
       <c r="AA631" s="3"/>
@@ -39336,7 +39870,7 @@
       <c r="K820" s="6"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="21" type="noConversion"/>
+  <phoneticPr fontId="22" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
diameter measurements Segi B2
</commit_message>
<xml_diff>
--- a/data/treeMeasurements/TreeMeasurements.xlsx
+++ b/data/treeMeasurements/TreeMeasurements.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11122"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christophe_rouleau-desrochers/github/fuelinex/data/treeMeasurements/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7C7BA4B-2DA5-1B4C-8837-B4E69E3A0E03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30694F0D-8950-4D43-9109-FDD968B7501B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4752" uniqueCount="1462">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4753" uniqueCount="1462">
   <si>
     <t>tree_ID</t>
   </si>
@@ -4431,11 +4431,18 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -4632,47 +4639,48 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="17" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="19" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="18" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="21" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="17" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="20" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="18" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="19" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -5331,7 +5339,7 @@
     </filterColumn>
     <filterColumn colId="3">
       <filters>
-        <filter val="populus"/>
+        <filter val="sequoiadendron"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -5568,9 +5576,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AA820"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A311" zoomScale="167" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="K1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="V292" sqref="V292"/>
+    <sheetView tabSelected="1" zoomScale="167" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="S1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="U578" sqref="U578"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5585,22 +5593,21 @@
     <col min="8" max="8" width="0.83203125" customWidth="1"/>
     <col min="9" max="9" width="0.33203125" customWidth="1"/>
     <col min="10" max="10" width="20.83203125" customWidth="1"/>
-    <col min="11" max="11" width="17.5" customWidth="1"/>
-    <col min="12" max="12" width="20.5" style="18" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="2.6640625" customWidth="1"/>
+    <col min="11" max="11" width="18.33203125" customWidth="1"/>
+    <col min="12" max="12" width="20.5" style="18" customWidth="1"/>
+    <col min="13" max="13" width="25.33203125" customWidth="1"/>
     <col min="14" max="14" width="18.5" customWidth="1"/>
     <col min="15" max="15" width="21.83203125" customWidth="1"/>
     <col min="16" max="16" width="0.5" hidden="1" customWidth="1"/>
     <col min="17" max="17" width="10.33203125" hidden="1" customWidth="1"/>
     <col min="18" max="18" width="0.1640625" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="17.1640625" customWidth="1"/>
-    <col min="20" max="20" width="0.33203125" customWidth="1"/>
-    <col min="21" max="21" width="1.33203125" customWidth="1"/>
-    <col min="22" max="22" width="12.5" customWidth="1"/>
+    <col min="19" max="20" width="14.6640625" customWidth="1"/>
+    <col min="21" max="21" width="22" customWidth="1"/>
+    <col min="22" max="22" width="14.6640625" customWidth="1"/>
     <col min="23" max="23" width="19.83203125" customWidth="1"/>
     <col min="24" max="24" width="23.1640625" customWidth="1"/>
     <col min="25" max="25" width="22.5" customWidth="1"/>
-    <col min="26" max="26" width="17.83203125" customWidth="1"/>
+    <col min="26" max="26" width="23.33203125" customWidth="1"/>
     <col min="27" max="27" width="25.83203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -20091,7 +20098,7 @@
         <v>71.7</v>
       </c>
     </row>
-    <row r="277" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A277" s="3" t="s">
         <v>850</v>
       </c>
@@ -20144,7 +20151,7 @@
       <c r="Z277" s="3"/>
       <c r="AA277" s="3"/>
     </row>
-    <row r="278" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A278" s="1" t="s">
         <v>853</v>
       </c>
@@ -20185,7 +20192,7 @@
         <v>1386</v>
       </c>
     </row>
-    <row r="279" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A279" s="3" t="s">
         <v>854</v>
       </c>
@@ -20244,7 +20251,7 @@
       <c r="Z279" s="3"/>
       <c r="AA279" s="3"/>
     </row>
-    <row r="280" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A280" s="1" t="s">
         <v>855</v>
       </c>
@@ -20285,7 +20292,7 @@
         <v>80.400000000000006</v>
       </c>
     </row>
-    <row r="281" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A281" s="3" t="s">
         <v>856</v>
       </c>
@@ -20820,7 +20827,7 @@
       <c r="Z291" s="3"/>
       <c r="AA291" s="3"/>
     </row>
-    <row r="292" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A292" s="1" t="s">
         <v>874</v>
       </c>
@@ -20861,7 +20868,7 @@
         <v>1391</v>
       </c>
     </row>
-    <row r="293" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A293" s="3" t="s">
         <v>875</v>
       </c>
@@ -20914,7 +20921,7 @@
       <c r="Z293" s="3"/>
       <c r="AA293" s="3"/>
     </row>
-    <row r="294" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A294" s="1" t="s">
         <v>878</v>
       </c>
@@ -20955,7 +20962,7 @@
         <v>1391</v>
       </c>
     </row>
-    <row r="295" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A295" s="3" t="s">
         <v>880</v>
       </c>
@@ -21008,7 +21015,7 @@
       <c r="Z295" s="3"/>
       <c r="AA295" s="3"/>
     </row>
-    <row r="296" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A296" s="1" t="s">
         <v>882</v>
       </c>
@@ -21511,7 +21518,7 @@
         <v>90.7</v>
       </c>
     </row>
-    <row r="307" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="307" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A307" s="3" t="s">
         <v>899</v>
       </c>
@@ -21564,7 +21571,7 @@
       <c r="Z307" s="3"/>
       <c r="AA307" s="3"/>
     </row>
-    <row r="308" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A308" s="1" t="s">
         <v>901</v>
       </c>
@@ -21605,7 +21612,7 @@
         <v>70.2</v>
       </c>
     </row>
-    <row r="309" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="309" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A309" s="3" t="s">
         <v>902</v>
       </c>
@@ -21658,7 +21665,7 @@
       <c r="Z309" s="3"/>
       <c r="AA309" s="3"/>
     </row>
-    <row r="310" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="310" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A310" s="1" t="s">
         <v>903</v>
       </c>
@@ -21699,7 +21706,7 @@
         <v>85.4</v>
       </c>
     </row>
-    <row r="311" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A311" s="3" t="s">
         <v>904</v>
       </c>
@@ -22223,7 +22230,7 @@
       <c r="Z321" s="3"/>
       <c r="AA321" s="3"/>
     </row>
-    <row r="322" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A322" s="1" t="s">
         <v>922</v>
       </c>
@@ -22264,7 +22271,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="323" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="323" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A323" s="3" t="s">
         <v>923</v>
       </c>
@@ -22317,7 +22324,7 @@
       <c r="Z323" s="3"/>
       <c r="AA323" s="3"/>
     </row>
-    <row r="324" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="324" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A324" s="1" t="s">
         <v>924</v>
       </c>
@@ -22358,7 +22365,7 @@
         <v>58.8</v>
       </c>
     </row>
-    <row r="325" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="325" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A325" s="3" t="s">
         <v>925</v>
       </c>
@@ -22411,7 +22418,7 @@
       <c r="Z325" s="3"/>
       <c r="AA325" s="3"/>
     </row>
-    <row r="326" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="326" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A326" s="1" t="s">
         <v>926</v>
       </c>
@@ -22945,7 +22952,7 @@
         <v>87.7</v>
       </c>
     </row>
-    <row r="337" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="337" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A337" s="3" t="s">
         <v>941</v>
       </c>
@@ -23004,7 +23011,7 @@
       <c r="Z337" s="30"/>
       <c r="AA337" s="30"/>
     </row>
-    <row r="338" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="338" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A338" s="1" t="s">
         <v>943</v>
       </c>
@@ -23045,7 +23052,7 @@
         <v>71.7</v>
       </c>
     </row>
-    <row r="339" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="339" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A339" s="3" t="s">
         <v>945</v>
       </c>
@@ -23102,7 +23109,7 @@
       <c r="Z339" s="30"/>
       <c r="AA339" s="30"/>
     </row>
-    <row r="340" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="340" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A340" s="1" t="s">
         <v>946</v>
       </c>
@@ -23143,7 +23150,7 @@
         <v>64.3</v>
       </c>
     </row>
-    <row r="341" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="341" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A341" s="3" t="s">
         <v>947</v>
       </c>
@@ -23671,7 +23678,7 @@
       <c r="Z351" s="3"/>
       <c r="AA351" s="3"/>
     </row>
-    <row r="352" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="352" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A352" s="1" t="s">
         <v>969</v>
       </c>
@@ -23712,7 +23719,7 @@
         <v>84.1</v>
       </c>
     </row>
-    <row r="353" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="353" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A353" s="3" t="s">
         <v>971</v>
       </c>
@@ -23764,7 +23771,7 @@
       <c r="Z353" s="3"/>
       <c r="AA353" s="3"/>
     </row>
-    <row r="354" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="354" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A354" s="1" t="s">
         <v>972</v>
       </c>
@@ -23805,7 +23812,7 @@
         <v>82.9</v>
       </c>
     </row>
-    <row r="355" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="355" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A355" s="3" t="s">
         <v>974</v>
       </c>
@@ -23858,7 +23865,7 @@
       <c r="Z355" s="3"/>
       <c r="AA355" s="3"/>
     </row>
-    <row r="356" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="356" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A356" s="1" t="s">
         <v>976</v>
       </c>
@@ -34142,7 +34149,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="547" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="547" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A547" s="3" t="s">
         <v>1269</v>
       </c>
@@ -34184,7 +34191,9 @@
       <c r="Q547" s="3"/>
       <c r="R547" s="3"/>
       <c r="S547" s="3"/>
-      <c r="T547" s="3"/>
+      <c r="T547" s="15">
+        <v>11.57</v>
+      </c>
       <c r="U547" s="3"/>
       <c r="V547" s="3">
         <v>28.5</v>
@@ -34194,10 +34203,10 @@
         <v>328</v>
       </c>
       <c r="Y547" s="3"/>
-      <c r="Z547" s="3"/>
+      <c r="Z547" s="15"/>
       <c r="AA547" s="3"/>
     </row>
-    <row r="548" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="548" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A548" s="1" t="s">
         <v>1270</v>
       </c>
@@ -34234,14 +34243,18 @@
       <c r="P548">
         <v>37</v>
       </c>
+      <c r="T548">
+        <v>11.9</v>
+      </c>
       <c r="V548">
         <v>28.2</v>
       </c>
       <c r="X548">
         <v>328</v>
       </c>
-    </row>
-    <row r="549" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Z548" s="15"/>
+    </row>
+    <row r="549" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A549" s="3" t="s">
         <v>1271</v>
       </c>
@@ -34283,7 +34296,9 @@
       <c r="Q549" s="3"/>
       <c r="R549" s="3"/>
       <c r="S549" s="3"/>
-      <c r="T549" s="3"/>
+      <c r="T549" s="3">
+        <v>9.75</v>
+      </c>
       <c r="U549" s="3"/>
       <c r="V549" s="3">
         <v>26.7</v>
@@ -34293,10 +34308,10 @@
         <v>328</v>
       </c>
       <c r="Y549" s="3"/>
-      <c r="Z549" s="3"/>
+      <c r="Z549" s="15"/>
       <c r="AA549" s="3"/>
     </row>
-    <row r="550" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="550" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A550" s="1" t="s">
         <v>1272</v>
       </c>
@@ -34333,14 +34348,18 @@
       <c r="P550">
         <v>37</v>
       </c>
+      <c r="T550" s="15">
+        <v>9.94</v>
+      </c>
       <c r="V550">
         <v>24.6</v>
       </c>
       <c r="X550">
         <v>328</v>
       </c>
-    </row>
-    <row r="551" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Z550" s="15"/>
+    </row>
+    <row r="551" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A551" s="3" t="s">
         <v>1274</v>
       </c>
@@ -34382,7 +34401,9 @@
       <c r="Q551" s="3"/>
       <c r="R551" s="3"/>
       <c r="S551" s="3"/>
-      <c r="T551" s="3"/>
+      <c r="T551" s="3">
+        <v>10.029999999999999</v>
+      </c>
       <c r="U551" s="3"/>
       <c r="V551" s="3">
         <v>29.7</v>
@@ -34392,7 +34413,7 @@
         <v>328</v>
       </c>
       <c r="Y551" s="3"/>
-      <c r="Z551" s="3"/>
+      <c r="Z551" s="15"/>
       <c r="AA551" s="3"/>
     </row>
     <row r="552" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -34438,6 +34459,7 @@
       <c r="X552">
         <v>328</v>
       </c>
+      <c r="Z552" s="15"/>
     </row>
     <row r="553" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A553" s="3" t="s">
@@ -34491,7 +34513,7 @@
         <v>328</v>
       </c>
       <c r="Y553" s="3"/>
-      <c r="Z553" s="3"/>
+      <c r="Z553" s="15"/>
       <c r="AA553" s="3"/>
     </row>
     <row r="554" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -34537,6 +34559,7 @@
       <c r="X554">
         <v>328</v>
       </c>
+      <c r="Z554" s="15"/>
     </row>
     <row r="555" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A555" s="3" t="s">
@@ -34590,7 +34613,7 @@
         <v>328</v>
       </c>
       <c r="Y555" s="3"/>
-      <c r="Z555" s="3"/>
+      <c r="Z555" s="15"/>
       <c r="AA555" s="3"/>
     </row>
     <row r="556" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -34636,6 +34659,7 @@
       <c r="X556">
         <v>328</v>
       </c>
+      <c r="Z556" s="15"/>
     </row>
     <row r="557" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A557" s="3" t="s">
@@ -34689,7 +34713,7 @@
         <v>328</v>
       </c>
       <c r="Y557" s="3"/>
-      <c r="Z557" s="3"/>
+      <c r="Z557" s="15"/>
       <c r="AA557" s="3"/>
     </row>
     <row r="558" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -34735,6 +34759,7 @@
       <c r="X558">
         <v>328</v>
       </c>
+      <c r="Z558" s="15"/>
     </row>
     <row r="559" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A559" s="3" t="s">
@@ -34788,7 +34813,7 @@
         <v>328</v>
       </c>
       <c r="Y559" s="3"/>
-      <c r="Z559" s="3"/>
+      <c r="Z559" s="15"/>
       <c r="AA559" s="3"/>
     </row>
     <row r="560" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -34834,6 +34859,7 @@
       <c r="X560">
         <v>328</v>
       </c>
+      <c r="Z560" s="15"/>
     </row>
     <row r="561" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A561" s="3" t="s">
@@ -34887,10 +34913,10 @@
         <v>328</v>
       </c>
       <c r="Y561" s="3"/>
-      <c r="Z561" s="3"/>
+      <c r="Z561" s="15"/>
       <c r="AA561" s="3"/>
     </row>
-    <row r="562" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="562" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A562" s="1" t="s">
         <v>1290</v>
       </c>
@@ -34927,14 +34953,18 @@
       <c r="P562">
         <v>37</v>
       </c>
+      <c r="T562">
+        <v>15.19</v>
+      </c>
       <c r="V562">
         <v>33.200000000000003</v>
       </c>
       <c r="X562">
         <v>328</v>
       </c>
-    </row>
-    <row r="563" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Z562" s="15"/>
+    </row>
+    <row r="563" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A563" s="3" t="s">
         <v>1293</v>
       </c>
@@ -34976,7 +35006,9 @@
       <c r="Q563" s="3"/>
       <c r="R563" s="3"/>
       <c r="S563" s="3"/>
-      <c r="T563" s="3"/>
+      <c r="T563" s="3">
+        <v>10.78</v>
+      </c>
       <c r="U563" s="3"/>
       <c r="V563" s="3">
         <v>31.2</v>
@@ -34986,10 +35018,10 @@
         <v>328</v>
       </c>
       <c r="Y563" s="3"/>
-      <c r="Z563" s="3"/>
+      <c r="Z563" s="15"/>
       <c r="AA563" s="3"/>
     </row>
-    <row r="564" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="564" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A564" s="1" t="s">
         <v>1295</v>
       </c>
@@ -35026,14 +35058,18 @@
       <c r="P564">
         <v>37</v>
       </c>
+      <c r="T564">
+        <v>12.45</v>
+      </c>
       <c r="V564">
         <v>36.9</v>
       </c>
       <c r="X564">
         <v>328</v>
       </c>
-    </row>
-    <row r="565" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Z564" s="15"/>
+    </row>
+    <row r="565" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A565" s="3" t="s">
         <v>1297</v>
       </c>
@@ -35075,7 +35111,9 @@
       <c r="Q565" s="3"/>
       <c r="R565" s="3"/>
       <c r="S565" s="3"/>
-      <c r="T565" s="3"/>
+      <c r="T565" s="3">
+        <v>11.31</v>
+      </c>
       <c r="U565" s="3"/>
       <c r="V565" s="3">
         <v>29.4</v>
@@ -35085,10 +35123,10 @@
         <v>328</v>
       </c>
       <c r="Y565" s="3"/>
-      <c r="Z565" s="3"/>
+      <c r="Z565" s="15"/>
       <c r="AA565" s="3"/>
     </row>
-    <row r="566" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="566" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A566" s="1" t="s">
         <v>1298</v>
       </c>
@@ -35125,12 +35163,16 @@
       <c r="P566">
         <v>37</v>
       </c>
+      <c r="T566">
+        <v>6.84</v>
+      </c>
       <c r="V566">
         <v>19.600000000000001</v>
       </c>
       <c r="X566">
         <v>328</v>
       </c>
+      <c r="Z566" s="15"/>
     </row>
     <row r="567" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A567" s="3" t="s">
@@ -35184,7 +35226,7 @@
         <v>328</v>
       </c>
       <c r="Y567" s="3"/>
-      <c r="Z567" s="3"/>
+      <c r="Z567" s="15"/>
       <c r="AA567" s="3"/>
     </row>
     <row r="568" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -35230,6 +35272,7 @@
       <c r="X568">
         <v>328</v>
       </c>
+      <c r="Z568" s="15"/>
     </row>
     <row r="569" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A569" s="3" t="s">
@@ -35283,7 +35326,7 @@
         <v>328</v>
       </c>
       <c r="Y569" s="3"/>
-      <c r="Z569" s="3"/>
+      <c r="Z569" s="15"/>
       <c r="AA569" s="3"/>
     </row>
     <row r="570" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -35329,6 +35372,7 @@
       <c r="X570">
         <v>328</v>
       </c>
+      <c r="Z570" s="15"/>
     </row>
     <row r="571" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A571" s="3" t="s">
@@ -35382,7 +35426,7 @@
         <v>328</v>
       </c>
       <c r="Y571" s="3"/>
-      <c r="Z571" s="3"/>
+      <c r="Z571" s="15"/>
       <c r="AA571" s="3"/>
     </row>
     <row r="572" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -35428,6 +35472,7 @@
       <c r="X572">
         <v>328</v>
       </c>
+      <c r="Z572" s="15"/>
     </row>
     <row r="573" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A573" s="3" t="s">
@@ -35479,7 +35524,7 @@
         <v>328</v>
       </c>
       <c r="Y573" s="3"/>
-      <c r="Z573" s="3"/>
+      <c r="Z573" s="15"/>
       <c r="AA573" s="3"/>
     </row>
     <row r="574" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -35525,6 +35570,7 @@
       <c r="X574">
         <v>328</v>
       </c>
+      <c r="Z574" s="15"/>
     </row>
     <row r="575" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A575" s="3" t="s">
@@ -35578,7 +35624,7 @@
         <v>328</v>
       </c>
       <c r="Y575" s="3"/>
-      <c r="Z575" s="3"/>
+      <c r="Z575" s="15"/>
       <c r="AA575" s="3"/>
     </row>
     <row r="576" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -35624,8 +35670,9 @@
       <c r="X576">
         <v>328</v>
       </c>
-    </row>
-    <row r="577" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Z576" s="15"/>
+    </row>
+    <row r="577" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A577" s="3" t="s">
         <v>1313</v>
       </c>
@@ -35667,7 +35714,9 @@
       <c r="Q577" s="3"/>
       <c r="R577" s="3"/>
       <c r="S577" s="3"/>
-      <c r="T577" s="3"/>
+      <c r="T577" s="3">
+        <v>12.04</v>
+      </c>
       <c r="U577" s="3"/>
       <c r="V577" s="3">
         <v>24.6</v>
@@ -35677,10 +35726,10 @@
         <v>328</v>
       </c>
       <c r="Y577" s="3"/>
-      <c r="Z577" s="3"/>
+      <c r="Z577" s="15"/>
       <c r="AA577" s="3"/>
     </row>
-    <row r="578" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="578" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A578" s="1" t="s">
         <v>1315</v>
       </c>
@@ -35720,11 +35769,15 @@
       <c r="S578" s="17" t="s">
         <v>1391</v>
       </c>
+      <c r="T578" s="47" t="s">
+        <v>1386</v>
+      </c>
       <c r="X578">
         <v>328</v>
       </c>
-    </row>
-    <row r="579" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Z578" s="15"/>
+    </row>
+    <row r="579" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A579" s="3" t="s">
         <v>1316</v>
       </c>
@@ -35766,7 +35819,9 @@
       <c r="Q579" s="3"/>
       <c r="R579" s="3"/>
       <c r="S579" s="3"/>
-      <c r="T579" s="3"/>
+      <c r="T579" s="3">
+        <v>11.66</v>
+      </c>
       <c r="U579" s="3"/>
       <c r="V579" s="3">
         <v>30.8</v>
@@ -35776,10 +35831,10 @@
         <v>328</v>
       </c>
       <c r="Y579" s="3"/>
-      <c r="Z579" s="3"/>
+      <c r="Z579" s="15"/>
       <c r="AA579" s="3"/>
     </row>
-    <row r="580" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="580" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A580" s="1" t="s">
         <v>1317</v>
       </c>
@@ -35816,14 +35871,18 @@
       <c r="P580">
         <v>37</v>
       </c>
+      <c r="T580">
+        <v>9.86</v>
+      </c>
       <c r="V580">
         <v>28.4</v>
       </c>
       <c r="X580">
         <v>328</v>
       </c>
-    </row>
-    <row r="581" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Z580" s="15"/>
+    </row>
+    <row r="581" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A581" s="3" t="s">
         <v>1318</v>
       </c>
@@ -35865,7 +35924,9 @@
       <c r="Q581" s="3"/>
       <c r="R581" s="3"/>
       <c r="S581" s="3"/>
-      <c r="T581" s="3"/>
+      <c r="T581" s="3">
+        <v>9.9</v>
+      </c>
       <c r="U581" s="3"/>
       <c r="V581" s="3">
         <v>29.3</v>
@@ -35875,7 +35936,7 @@
         <v>328</v>
       </c>
       <c r="Y581" s="3"/>
-      <c r="Z581" s="3"/>
+      <c r="Z581" s="15"/>
       <c r="AA581" s="3"/>
     </row>
     <row r="582" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -35921,6 +35982,7 @@
       <c r="X582">
         <v>328</v>
       </c>
+      <c r="Z582" s="15"/>
     </row>
     <row r="583" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A583" s="3" t="s">
@@ -35974,7 +36036,7 @@
         <v>328</v>
       </c>
       <c r="Y583" s="3"/>
-      <c r="Z583" s="3"/>
+      <c r="Z583" s="15"/>
       <c r="AA583" s="3"/>
     </row>
     <row r="584" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -36020,6 +36082,7 @@
       <c r="X584">
         <v>328</v>
       </c>
+      <c r="Z584" s="15"/>
     </row>
     <row r="585" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A585" s="3" t="s">
@@ -36073,7 +36136,7 @@
         <v>328</v>
       </c>
       <c r="Y585" s="3"/>
-      <c r="Z585" s="3"/>
+      <c r="Z585" s="15"/>
       <c r="AA585" s="3"/>
     </row>
     <row r="586" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -36119,6 +36182,7 @@
       <c r="X586">
         <v>328</v>
       </c>
+      <c r="Z586" s="15"/>
     </row>
     <row r="587" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A587" s="3" t="s">
@@ -36172,7 +36236,7 @@
         <v>328</v>
       </c>
       <c r="Y587" s="3"/>
-      <c r="Z587" s="3"/>
+      <c r="Z587" s="15"/>
       <c r="AA587" s="3"/>
     </row>
     <row r="588" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -36218,6 +36282,7 @@
       <c r="X588">
         <v>328</v>
       </c>
+      <c r="Z588" s="15"/>
     </row>
     <row r="589" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A589" s="3" t="s">
@@ -36271,7 +36336,7 @@
         <v>328</v>
       </c>
       <c r="Y589" s="3"/>
-      <c r="Z589" s="3"/>
+      <c r="Z589" s="15"/>
       <c r="AA589" s="3"/>
     </row>
     <row r="590" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -36317,6 +36382,7 @@
       <c r="X590">
         <v>328</v>
       </c>
+      <c r="Z590" s="15"/>
     </row>
     <row r="591" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A591" s="3" t="s">
@@ -36370,10 +36436,10 @@
         <v>328</v>
       </c>
       <c r="Y591" s="3"/>
-      <c r="Z591" s="3"/>
+      <c r="Z591" s="15"/>
       <c r="AA591" s="3"/>
     </row>
-    <row r="592" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="592" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A592" s="1" t="s">
         <v>1332</v>
       </c>
@@ -36410,14 +36476,18 @@
       <c r="P592">
         <v>37</v>
       </c>
+      <c r="T592">
+        <v>11.84</v>
+      </c>
       <c r="V592">
         <v>28.4</v>
       </c>
       <c r="X592">
         <v>328</v>
       </c>
-    </row>
-    <row r="593" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Z592" s="15"/>
+    </row>
+    <row r="593" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A593" s="3" t="s">
         <v>1333</v>
       </c>
@@ -36459,7 +36529,9 @@
       <c r="Q593" s="3"/>
       <c r="R593" s="3"/>
       <c r="S593" s="3"/>
-      <c r="T593" s="3"/>
+      <c r="T593" s="3">
+        <v>11.69</v>
+      </c>
       <c r="U593" s="3"/>
       <c r="V593" s="3">
         <v>33.200000000000003</v>
@@ -36469,10 +36541,10 @@
         <v>328</v>
       </c>
       <c r="Y593" s="3"/>
-      <c r="Z593" s="3"/>
+      <c r="Z593" s="15"/>
       <c r="AA593" s="3"/>
     </row>
-    <row r="594" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="594" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A594" s="1" t="s">
         <v>1335</v>
       </c>
@@ -36515,8 +36587,9 @@
       <c r="X594">
         <v>328</v>
       </c>
-    </row>
-    <row r="595" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Z594" s="15"/>
+    </row>
+    <row r="595" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A595" s="3" t="s">
         <v>1336</v>
       </c>
@@ -36562,7 +36635,9 @@
       <c r="S595" s="11" t="s">
         <v>1405</v>
       </c>
-      <c r="T595" s="11"/>
+      <c r="T595" s="11">
+        <v>10.94</v>
+      </c>
       <c r="U595" s="11"/>
       <c r="V595" s="11">
         <v>33.6</v>
@@ -36572,10 +36647,10 @@
         <v>328</v>
       </c>
       <c r="Y595" s="11"/>
-      <c r="Z595" s="11"/>
+      <c r="Z595" s="15"/>
       <c r="AA595" s="11"/>
     </row>
-    <row r="596" spans="1:27" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="596" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A596" s="1" t="s">
         <v>1337</v>
       </c>
@@ -36618,6 +36693,7 @@
       <c r="X596">
         <v>328</v>
       </c>
+      <c r="Z596" s="15"/>
     </row>
     <row r="597" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A597" s="3" t="s">
@@ -36671,7 +36747,7 @@
         <v>328</v>
       </c>
       <c r="Y597" s="3"/>
-      <c r="Z597" s="3"/>
+      <c r="Z597" s="15"/>
       <c r="AA597" s="3"/>
     </row>
     <row r="598" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -36717,6 +36793,7 @@
       <c r="X598">
         <v>328</v>
       </c>
+      <c r="Z598" s="15"/>
     </row>
     <row r="599" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A599" s="3" t="s">
@@ -36770,7 +36847,7 @@
         <v>328</v>
       </c>
       <c r="Y599" s="3"/>
-      <c r="Z599" s="3"/>
+      <c r="Z599" s="15"/>
       <c r="AA599" s="3"/>
     </row>
     <row r="600" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -36816,6 +36893,7 @@
       <c r="X600">
         <v>328</v>
       </c>
+      <c r="Z600" s="15"/>
     </row>
     <row r="601" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A601" s="3" t="s">
@@ -36869,7 +36947,7 @@
         <v>328</v>
       </c>
       <c r="Y601" s="3"/>
-      <c r="Z601" s="3"/>
+      <c r="Z601" s="15"/>
       <c r="AA601" s="3"/>
     </row>
     <row r="602" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -36915,6 +36993,7 @@
       <c r="X602">
         <v>328</v>
       </c>
+      <c r="Z602" s="15"/>
     </row>
     <row r="603" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A603" s="3" t="s">
@@ -36968,7 +37047,7 @@
         <v>328</v>
       </c>
       <c r="Y603" s="3"/>
-      <c r="Z603" s="3"/>
+      <c r="Z603" s="15"/>
       <c r="AA603" s="3"/>
     </row>
     <row r="604" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -37014,6 +37093,7 @@
       <c r="X604">
         <v>328</v>
       </c>
+      <c r="Z604" s="15"/>
     </row>
     <row r="605" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A605" s="3" t="s">
@@ -37067,7 +37147,7 @@
         <v>328</v>
       </c>
       <c r="Y605" s="3"/>
-      <c r="Z605" s="3"/>
+      <c r="Z605" s="15"/>
       <c r="AA605" s="3"/>
     </row>
     <row r="606" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -37113,8 +37193,9 @@
       <c r="X606">
         <v>328</v>
       </c>
-    </row>
-    <row r="607" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Z606" s="15"/>
+    </row>
+    <row r="607" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A607" s="3" t="s">
         <v>1353</v>
       </c>
@@ -37156,7 +37237,9 @@
       <c r="Q607" s="3"/>
       <c r="R607" s="3"/>
       <c r="S607" s="3"/>
-      <c r="T607" s="3"/>
+      <c r="T607" s="3">
+        <v>8.4499999999999993</v>
+      </c>
       <c r="U607" s="3"/>
       <c r="V607" s="3">
         <v>25.4</v>
@@ -37166,10 +37249,10 @@
         <v>328</v>
       </c>
       <c r="Y607" s="3"/>
-      <c r="Z607" s="3"/>
+      <c r="Z607" s="15"/>
       <c r="AA607" s="3"/>
     </row>
-    <row r="608" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="608" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A608" s="1" t="s">
         <v>1354</v>
       </c>
@@ -37206,14 +37289,18 @@
       <c r="P608">
         <v>37</v>
       </c>
+      <c r="T608">
+        <v>10.199999999999999</v>
+      </c>
       <c r="V608">
         <v>30.7</v>
       </c>
       <c r="X608">
         <v>328</v>
       </c>
-    </row>
-    <row r="609" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Z608" s="15"/>
+    </row>
+    <row r="609" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A609" s="3" t="s">
         <v>1355</v>
       </c>
@@ -37255,7 +37342,9 @@
       <c r="Q609" s="3"/>
       <c r="R609" s="3"/>
       <c r="S609" s="3"/>
-      <c r="T609" s="3"/>
+      <c r="T609" s="3">
+        <v>12.55</v>
+      </c>
       <c r="U609" s="3"/>
       <c r="V609" s="3">
         <v>33.9</v>
@@ -37265,10 +37354,10 @@
         <v>328</v>
       </c>
       <c r="Y609" s="3"/>
-      <c r="Z609" s="3"/>
+      <c r="Z609" s="15"/>
       <c r="AA609" s="3"/>
     </row>
-    <row r="610" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="610" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A610" s="1" t="s">
         <v>1356</v>
       </c>
@@ -37305,14 +37394,18 @@
       <c r="P610">
         <v>37</v>
       </c>
+      <c r="T610">
+        <v>8.26</v>
+      </c>
       <c r="V610">
         <v>24.4</v>
       </c>
       <c r="X610">
         <v>328</v>
       </c>
-    </row>
-    <row r="611" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Z610" s="15"/>
+    </row>
+    <row r="611" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A611" s="3" t="s">
         <v>1357</v>
       </c>
@@ -37364,7 +37457,7 @@
         <v>328</v>
       </c>
       <c r="Y611" s="3"/>
-      <c r="Z611" s="3"/>
+      <c r="Z611" s="15"/>
       <c r="AA611" s="3"/>
     </row>
     <row r="612" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -37410,6 +37503,7 @@
       <c r="X612">
         <v>328</v>
       </c>
+      <c r="Z612" s="15"/>
     </row>
     <row r="613" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A613" s="3" t="s">
@@ -37463,7 +37557,7 @@
         <v>328</v>
       </c>
       <c r="Y613" s="3"/>
-      <c r="Z613" s="3"/>
+      <c r="Z613" s="15"/>
       <c r="AA613" s="3"/>
     </row>
     <row r="614" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -37509,6 +37603,7 @@
       <c r="X614">
         <v>328</v>
       </c>
+      <c r="Z614" s="15"/>
     </row>
     <row r="615" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A615" s="3" t="s">
@@ -37562,7 +37657,7 @@
         <v>328</v>
       </c>
       <c r="Y615" s="3"/>
-      <c r="Z615" s="3"/>
+      <c r="Z615" s="15"/>
       <c r="AA615" s="3"/>
     </row>
     <row r="616" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -37608,6 +37703,7 @@
       <c r="X616">
         <v>328</v>
       </c>
+      <c r="Z616" s="15"/>
     </row>
     <row r="617" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A617" s="3" t="s">
@@ -37661,7 +37757,7 @@
         <v>328</v>
       </c>
       <c r="Y617" s="3"/>
-      <c r="Z617" s="3"/>
+      <c r="Z617" s="15"/>
       <c r="AA617" s="3"/>
     </row>
     <row r="618" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -37707,6 +37803,7 @@
       <c r="X618">
         <v>328</v>
       </c>
+      <c r="Z618" s="15"/>
     </row>
     <row r="619" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A619" s="3" t="s">
@@ -37760,7 +37857,7 @@
         <v>328</v>
       </c>
       <c r="Y619" s="3"/>
-      <c r="Z619" s="3"/>
+      <c r="Z619" s="15"/>
       <c r="AA619" s="3"/>
     </row>
     <row r="620" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -37806,6 +37903,7 @@
       <c r="X620">
         <v>328</v>
       </c>
+      <c r="Z620" s="15"/>
     </row>
     <row r="621" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A621" s="3" t="s">
@@ -37859,10 +37957,10 @@
         <v>328</v>
       </c>
       <c r="Y621" s="3"/>
-      <c r="Z621" s="3"/>
+      <c r="Z621" s="15"/>
       <c r="AA621" s="3"/>
     </row>
-    <row r="622" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="622" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A622" s="1" t="s">
         <v>1372</v>
       </c>
@@ -37899,14 +37997,18 @@
       <c r="P622">
         <v>37</v>
       </c>
+      <c r="T622">
+        <v>11.67</v>
+      </c>
       <c r="V622">
         <v>31.1</v>
       </c>
       <c r="X622">
         <v>328</v>
       </c>
-    </row>
-    <row r="623" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Z622" s="15"/>
+    </row>
+    <row r="623" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A623" s="3" t="s">
         <v>1373</v>
       </c>
@@ -37948,7 +38050,9 @@
       <c r="Q623" s="3"/>
       <c r="R623" s="3"/>
       <c r="S623" s="3"/>
-      <c r="T623" s="3"/>
+      <c r="T623" s="3">
+        <v>9.3800000000000008</v>
+      </c>
       <c r="U623" s="3"/>
       <c r="V623" s="3">
         <v>27.9</v>
@@ -37958,10 +38062,10 @@
         <v>328</v>
       </c>
       <c r="Y623" s="3"/>
-      <c r="Z623" s="3"/>
+      <c r="Z623" s="15"/>
       <c r="AA623" s="3"/>
     </row>
-    <row r="624" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="624" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A624" s="1" t="s">
         <v>1374</v>
       </c>
@@ -37998,14 +38102,18 @@
       <c r="P624">
         <v>37</v>
       </c>
+      <c r="T624">
+        <v>9.8699999999999992</v>
+      </c>
       <c r="V624">
         <v>24.9</v>
       </c>
       <c r="X624">
         <v>328</v>
       </c>
-    </row>
-    <row r="625" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Z624" s="15"/>
+    </row>
+    <row r="625" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A625" s="3" t="s">
         <v>1375</v>
       </c>
@@ -38047,7 +38155,9 @@
       <c r="Q625" s="3"/>
       <c r="R625" s="3"/>
       <c r="S625" s="3"/>
-      <c r="T625" s="3"/>
+      <c r="T625" s="3">
+        <v>11.64</v>
+      </c>
       <c r="U625" s="3"/>
       <c r="V625" s="3">
         <v>30.1</v>
@@ -38057,10 +38167,10 @@
         <v>328</v>
       </c>
       <c r="Y625" s="3"/>
-      <c r="Z625" s="3"/>
+      <c r="Z625" s="15"/>
       <c r="AA625" s="3"/>
     </row>
-    <row r="626" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="626" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A626" s="1" t="s">
         <v>1377</v>
       </c>
@@ -38097,12 +38207,16 @@
       <c r="P626">
         <v>37</v>
       </c>
+      <c r="T626">
+        <v>10.79</v>
+      </c>
       <c r="V626">
         <v>25.5</v>
       </c>
       <c r="X626">
         <v>328</v>
       </c>
+      <c r="Z626" s="15"/>
     </row>
     <row r="627" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A627" s="3" t="s">
@@ -39870,7 +39984,7 @@
       <c r="K820" s="6"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="22" type="noConversion"/>
+  <phoneticPr fontId="23" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
tree measurements segi and poba
</commit_message>
<xml_diff>
--- a/data/treeMeasurements/TreeMeasurements.xlsx
+++ b/data/treeMeasurements/TreeMeasurements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christophe_rouleau-desrochers/github/fuelinex/data/treeMeasurements/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30694F0D-8950-4D43-9109-FDD968B7501B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13C44731-F9C3-AB42-97F7-A86469471232}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4753" uniqueCount="1462">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4783" uniqueCount="1465">
   <si>
     <t>tree_ID</t>
   </si>
@@ -4422,6 +4422,15 @@
   </si>
   <si>
     <t>apical shoot died; lateral shoot measured</t>
+  </si>
+  <si>
+    <t>apical meristem snapped off but it shouldn't be much taller than that height; look up the shoot elongation measurements</t>
+  </si>
+  <si>
+    <t>branch sprouted on red mark so diameter measurement might not be accurate</t>
+  </si>
+  <si>
+    <t>the second shoot mentioned last year died</t>
   </si>
 </sst>
 </file>
@@ -4431,11 +4440,18 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -4639,47 +4655,48 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="20" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="19" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="22" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="18" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="21" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="19" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="20" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -5334,7 +5351,7 @@
   <autoFilter ref="A1:AA631" xr:uid="{3F288811-81FB-F847-9587-99D03002EDFF}">
     <filterColumn colId="1">
       <filters>
-        <filter val="2"/>
+        <filter val="1"/>
       </filters>
     </filterColumn>
     <filterColumn colId="3">
@@ -5577,8 +5594,8 @@
   <dimension ref="A1:AA820"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="167" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="S1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="U578" sqref="U578"/>
+      <pane xSplit="1" topLeftCell="M1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="U617" sqref="U617"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5593,10 +5610,10 @@
     <col min="8" max="8" width="0.83203125" customWidth="1"/>
     <col min="9" max="9" width="0.33203125" customWidth="1"/>
     <col min="10" max="10" width="20.83203125" customWidth="1"/>
-    <col min="11" max="11" width="18.33203125" customWidth="1"/>
-    <col min="12" max="12" width="20.5" style="18" customWidth="1"/>
-    <col min="13" max="13" width="25.33203125" customWidth="1"/>
-    <col min="14" max="14" width="18.5" customWidth="1"/>
+    <col min="11" max="11" width="28.83203125" customWidth="1"/>
+    <col min="12" max="12" width="18.83203125" style="18" customWidth="1"/>
+    <col min="13" max="13" width="22.1640625" customWidth="1"/>
+    <col min="14" max="14" width="3.1640625" customWidth="1"/>
     <col min="15" max="15" width="21.83203125" customWidth="1"/>
     <col min="16" max="16" width="0.5" hidden="1" customWidth="1"/>
     <col min="17" max="17" width="10.33203125" hidden="1" customWidth="1"/>
@@ -19901,6 +19918,9 @@
       <c r="S272" s="11" t="s">
         <v>1387</v>
       </c>
+      <c r="T272">
+        <v>6.7</v>
+      </c>
       <c r="V272">
         <v>72.2</v>
       </c>
@@ -19947,7 +19967,9 @@
       <c r="Q273" s="3"/>
       <c r="R273" s="3"/>
       <c r="S273" s="3"/>
-      <c r="T273" s="3"/>
+      <c r="T273" s="3">
+        <v>7.17</v>
+      </c>
       <c r="U273" s="3"/>
       <c r="V273" s="3">
         <v>88.9</v>
@@ -19995,6 +20017,9 @@
       <c r="P274">
         <v>37</v>
       </c>
+      <c r="T274">
+        <v>6.64</v>
+      </c>
       <c r="V274">
         <v>70.2</v>
       </c>
@@ -20043,7 +20068,9 @@
       <c r="S275" s="11" t="s">
         <v>1387</v>
       </c>
-      <c r="T275" s="3"/>
+      <c r="T275" s="3">
+        <v>7.39</v>
+      </c>
       <c r="U275" s="3"/>
       <c r="V275" s="3">
         <v>82.9</v>
@@ -20094,6 +20121,9 @@
       <c r="S276" s="11" t="s">
         <v>1387</v>
       </c>
+      <c r="T276">
+        <v>7.27</v>
+      </c>
       <c r="V276">
         <v>71.7</v>
       </c>
@@ -20140,7 +20170,9 @@
       <c r="Q277" s="3"/>
       <c r="R277" s="3"/>
       <c r="S277" s="3"/>
-      <c r="T277" s="3"/>
+      <c r="T277" s="3">
+        <v>5.62</v>
+      </c>
       <c r="U277" s="3"/>
       <c r="V277" s="3" t="s">
         <v>1386</v>
@@ -20188,6 +20220,9 @@
       <c r="P278">
         <v>37</v>
       </c>
+      <c r="T278">
+        <v>7.04</v>
+      </c>
       <c r="V278" s="46" t="s">
         <v>1386</v>
       </c>
@@ -20240,7 +20275,9 @@
       <c r="S279" s="12" t="s">
         <v>1388</v>
       </c>
-      <c r="T279" s="3"/>
+      <c r="T279" s="3">
+        <v>8.25</v>
+      </c>
       <c r="U279" s="3"/>
       <c r="V279" s="3">
         <v>94.2</v>
@@ -20288,6 +20325,9 @@
       <c r="P280">
         <v>37</v>
       </c>
+      <c r="T280">
+        <v>6.67</v>
+      </c>
       <c r="V280">
         <v>80.400000000000006</v>
       </c>
@@ -20334,7 +20374,9 @@
       <c r="Q281" s="3"/>
       <c r="R281" s="3"/>
       <c r="S281" s="3"/>
-      <c r="T281" s="3"/>
+      <c r="T281" s="3">
+        <v>7.85</v>
+      </c>
       <c r="U281" s="3"/>
       <c r="V281" s="3">
         <v>97.9</v>
@@ -20388,17 +20430,23 @@
       <c r="R282" s="30" t="s">
         <v>1407</v>
       </c>
-      <c r="S282" s="17" t="s">
+      <c r="S282" s="48" t="s">
         <v>1415</v>
       </c>
-      <c r="T282" s="30"/>
+      <c r="T282" s="30">
+        <v>5.26</v>
+      </c>
       <c r="U282" s="30"/>
-      <c r="V282" s="30"/>
+      <c r="V282" s="30">
+        <v>77.8</v>
+      </c>
       <c r="W282" s="30"/>
       <c r="X282" s="30"/>
       <c r="Y282" s="30"/>
       <c r="Z282" s="30"/>
-      <c r="AA282" s="30"/>
+      <c r="AA282" s="48" t="s">
+        <v>1464</v>
+      </c>
     </row>
     <row r="283" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A283" s="3" t="s">
@@ -20444,9 +20492,13 @@
       <c r="S283" s="3" t="s">
         <v>1391</v>
       </c>
-      <c r="T283" s="3"/>
+      <c r="T283" s="48" t="s">
+        <v>1386</v>
+      </c>
       <c r="U283" s="3"/>
-      <c r="V283" s="3"/>
+      <c r="V283" s="3" t="s">
+        <v>1386</v>
+      </c>
       <c r="W283" s="3"/>
       <c r="X283" s="3"/>
       <c r="Y283" s="3"/>
@@ -20490,6 +20542,12 @@
       <c r="P284">
         <v>57</v>
       </c>
+      <c r="T284" s="15">
+        <v>7.08</v>
+      </c>
+      <c r="V284">
+        <v>69</v>
+      </c>
     </row>
     <row r="285" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A285" s="3" t="s">
@@ -20533,9 +20591,13 @@
       <c r="Q285" s="3"/>
       <c r="R285" s="3"/>
       <c r="S285" s="3"/>
-      <c r="T285" s="3"/>
+      <c r="T285" s="3">
+        <v>5.96</v>
+      </c>
       <c r="U285" s="3"/>
-      <c r="V285" s="3"/>
+      <c r="V285" s="3">
+        <v>60.2</v>
+      </c>
       <c r="W285" s="3"/>
       <c r="X285" s="3"/>
       <c r="Y285" s="3"/>
@@ -20579,6 +20641,12 @@
       <c r="P286">
         <v>57</v>
       </c>
+      <c r="T286">
+        <v>7.4</v>
+      </c>
+      <c r="V286">
+        <v>117.4</v>
+      </c>
     </row>
     <row r="287" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A287" s="3" t="s">
@@ -20622,7 +20690,9 @@
       <c r="Q287" s="3"/>
       <c r="R287" s="3"/>
       <c r="S287" s="3"/>
-      <c r="T287" s="3"/>
+      <c r="T287" s="3">
+        <v>7.56</v>
+      </c>
       <c r="U287" s="3"/>
       <c r="V287" s="3">
         <v>101.6</v>
@@ -20670,6 +20740,9 @@
       <c r="P288">
         <v>37</v>
       </c>
+      <c r="T288">
+        <v>7.72</v>
+      </c>
       <c r="V288">
         <v>66.5</v>
       </c>
@@ -20716,7 +20789,9 @@
       <c r="Q289" s="3"/>
       <c r="R289" s="3"/>
       <c r="S289" s="3"/>
-      <c r="T289" s="3"/>
+      <c r="T289" s="3">
+        <v>7.38</v>
+      </c>
       <c r="U289" s="3"/>
       <c r="V289" s="3">
         <v>90.5</v>
@@ -20764,6 +20839,9 @@
       <c r="P290">
         <v>37</v>
       </c>
+      <c r="T290">
+        <v>7.99</v>
+      </c>
       <c r="V290">
         <v>83.6</v>
       </c>
@@ -20816,7 +20894,9 @@
       <c r="S291" s="12" t="s">
         <v>1388</v>
       </c>
-      <c r="T291" s="3"/>
+      <c r="T291" s="3">
+        <v>6.38</v>
+      </c>
       <c r="U291" s="3"/>
       <c r="V291" s="3">
         <v>80.7</v>
@@ -20867,6 +20947,12 @@
       <c r="S292" s="12" t="s">
         <v>1391</v>
       </c>
+      <c r="T292" s="48" t="s">
+        <v>1386</v>
+      </c>
+      <c r="V292" s="48" t="s">
+        <v>1386</v>
+      </c>
     </row>
     <row r="293" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A293" s="3" t="s">
@@ -20910,7 +20996,9 @@
       <c r="Q293" s="3"/>
       <c r="R293" s="3"/>
       <c r="S293" s="3"/>
-      <c r="T293" s="3"/>
+      <c r="T293" s="3">
+        <v>8.73</v>
+      </c>
       <c r="U293" s="3"/>
       <c r="V293" s="3">
         <v>101.7</v>
@@ -20961,6 +21049,12 @@
       <c r="S294" s="12" t="s">
         <v>1391</v>
       </c>
+      <c r="T294" s="48" t="s">
+        <v>1386</v>
+      </c>
+      <c r="V294" s="48" t="s">
+        <v>1386</v>
+      </c>
     </row>
     <row r="295" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A295" s="3" t="s">
@@ -21004,7 +21098,9 @@
       <c r="Q295" s="3"/>
       <c r="R295" s="3"/>
       <c r="S295" s="3"/>
-      <c r="T295" s="3"/>
+      <c r="T295" s="3">
+        <v>7.22</v>
+      </c>
       <c r="U295" s="3"/>
       <c r="V295" s="3">
         <v>122.5</v>
@@ -21052,6 +21148,9 @@
       <c r="P296">
         <v>37</v>
       </c>
+      <c r="T296">
+        <v>7.8</v>
+      </c>
       <c r="V296">
         <v>114.9</v>
       </c>
@@ -21098,9 +21197,13 @@
       <c r="Q297" s="3"/>
       <c r="R297" s="3"/>
       <c r="S297" s="3"/>
-      <c r="T297" s="3"/>
+      <c r="T297" s="3">
+        <v>6.89</v>
+      </c>
       <c r="U297" s="3"/>
-      <c r="V297" s="3"/>
+      <c r="V297" s="3">
+        <v>72.599999999999994</v>
+      </c>
       <c r="W297" s="3"/>
       <c r="X297" s="3"/>
       <c r="Y297" s="3"/>
@@ -21144,6 +21247,12 @@
       <c r="P298">
         <v>57</v>
       </c>
+      <c r="T298">
+        <v>8.86</v>
+      </c>
+      <c r="V298">
+        <v>125.1</v>
+      </c>
     </row>
     <row r="299" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A299" s="3" t="s">
@@ -21187,14 +21296,20 @@
       <c r="Q299" s="3"/>
       <c r="R299" s="3"/>
       <c r="S299" s="3"/>
-      <c r="T299" s="3"/>
+      <c r="T299" s="3">
+        <v>7.37</v>
+      </c>
       <c r="U299" s="3"/>
-      <c r="V299" s="3"/>
+      <c r="V299" s="3">
+        <v>75.8</v>
+      </c>
       <c r="W299" s="3"/>
       <c r="X299" s="3"/>
       <c r="Y299" s="3"/>
       <c r="Z299" s="3"/>
-      <c r="AA299" s="3"/>
+      <c r="AA299" s="3" t="s">
+        <v>1463</v>
+      </c>
     </row>
     <row r="300" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A300" s="1" t="s">
@@ -21233,6 +21348,12 @@
       <c r="P300">
         <v>57</v>
       </c>
+      <c r="T300">
+        <v>7.85</v>
+      </c>
+      <c r="V300">
+        <v>68.8</v>
+      </c>
     </row>
     <row r="301" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A301" s="3" t="s">
@@ -21280,9 +21401,13 @@
       <c r="S301" s="3" t="s">
         <v>1421</v>
       </c>
-      <c r="T301" s="3"/>
+      <c r="T301" s="3">
+        <v>7.66</v>
+      </c>
       <c r="U301" s="3"/>
-      <c r="V301" s="3"/>
+      <c r="V301" s="3">
+        <v>46.3</v>
+      </c>
       <c r="W301" s="3"/>
       <c r="X301" s="3"/>
       <c r="Y301" s="3"/>
@@ -21326,6 +21451,9 @@
       <c r="P302">
         <v>37</v>
       </c>
+      <c r="T302">
+        <v>6.87</v>
+      </c>
       <c r="V302">
         <v>51.5</v>
       </c>
@@ -21372,7 +21500,9 @@
       <c r="Q303" s="3"/>
       <c r="R303" s="3"/>
       <c r="S303" s="3"/>
-      <c r="T303" s="3"/>
+      <c r="T303" s="3">
+        <v>7.09</v>
+      </c>
       <c r="U303" s="3"/>
       <c r="V303" s="3">
         <v>87.6</v>
@@ -21420,6 +21550,9 @@
       <c r="P304">
         <v>37</v>
       </c>
+      <c r="T304">
+        <v>6.19</v>
+      </c>
       <c r="V304">
         <v>78.099999999999994</v>
       </c>
@@ -21466,7 +21599,9 @@
       <c r="Q305" s="3"/>
       <c r="R305" s="3"/>
       <c r="S305" s="3"/>
-      <c r="T305" s="3"/>
+      <c r="T305" s="3">
+        <v>7.89</v>
+      </c>
       <c r="U305" s="3"/>
       <c r="V305" s="3">
         <v>82.3</v>
@@ -21514,6 +21649,9 @@
       <c r="P306">
         <v>37</v>
       </c>
+      <c r="T306">
+        <v>7.62</v>
+      </c>
       <c r="V306">
         <v>90.7</v>
       </c>
@@ -21560,7 +21698,9 @@
       <c r="Q307" s="3"/>
       <c r="R307" s="3"/>
       <c r="S307" s="3"/>
-      <c r="T307" s="3"/>
+      <c r="T307" s="3">
+        <v>7.01</v>
+      </c>
       <c r="U307" s="3"/>
       <c r="V307" s="3">
         <v>88.2</v>
@@ -21608,6 +21748,9 @@
       <c r="P308">
         <v>37</v>
       </c>
+      <c r="T308">
+        <v>7.9</v>
+      </c>
       <c r="V308">
         <v>70.2</v>
       </c>
@@ -21654,7 +21797,9 @@
       <c r="Q309" s="3"/>
       <c r="R309" s="3"/>
       <c r="S309" s="3"/>
-      <c r="T309" s="3"/>
+      <c r="T309" s="3">
+        <v>6.92</v>
+      </c>
       <c r="U309" s="3"/>
       <c r="V309" s="3">
         <v>63.5</v>
@@ -21702,6 +21847,9 @@
       <c r="P310">
         <v>37</v>
       </c>
+      <c r="T310">
+        <v>7.17</v>
+      </c>
       <c r="V310">
         <v>85.4</v>
       </c>
@@ -21748,7 +21896,9 @@
       <c r="Q311" s="3"/>
       <c r="R311" s="3"/>
       <c r="S311" s="3"/>
-      <c r="T311" s="3"/>
+      <c r="T311" s="3">
+        <v>7.32</v>
+      </c>
       <c r="U311" s="3"/>
       <c r="V311" s="3">
         <v>106.9</v>
@@ -21796,6 +21946,12 @@
       <c r="P312">
         <v>57</v>
       </c>
+      <c r="T312">
+        <v>8.2899999999999991</v>
+      </c>
+      <c r="V312">
+        <v>96.4</v>
+      </c>
     </row>
     <row r="313" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A313" s="3" t="s">
@@ -21839,9 +21995,13 @@
       <c r="Q313" s="3"/>
       <c r="R313" s="3"/>
       <c r="S313" s="3"/>
-      <c r="T313" s="3"/>
+      <c r="T313" s="3">
+        <v>8.85</v>
+      </c>
       <c r="U313" s="3"/>
-      <c r="V313" s="3"/>
+      <c r="V313" s="3">
+        <v>106.3</v>
+      </c>
       <c r="W313" s="3"/>
       <c r="X313" s="3"/>
       <c r="Y313" s="3"/>
@@ -21885,6 +22045,12 @@
       <c r="P314">
         <v>57</v>
       </c>
+      <c r="T314">
+        <v>6.65</v>
+      </c>
+      <c r="V314">
+        <v>104</v>
+      </c>
     </row>
     <row r="315" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A315" s="3" t="s">
@@ -21928,9 +22094,13 @@
       <c r="Q315" s="3"/>
       <c r="R315" s="3"/>
       <c r="S315" s="3"/>
-      <c r="T315" s="3"/>
+      <c r="T315" s="3">
+        <v>9.08</v>
+      </c>
       <c r="U315" s="3"/>
-      <c r="V315" s="3"/>
+      <c r="V315" s="3">
+        <v>108.9</v>
+      </c>
       <c r="W315" s="3"/>
       <c r="X315" s="3"/>
       <c r="Y315" s="3"/>
@@ -21974,6 +22144,15 @@
       <c r="P316">
         <v>57</v>
       </c>
+      <c r="T316">
+        <v>7.79</v>
+      </c>
+      <c r="V316">
+        <v>91.9</v>
+      </c>
+      <c r="AA316" s="48" t="s">
+        <v>1462</v>
+      </c>
     </row>
     <row r="317" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A317" s="3" t="s">
@@ -22017,7 +22196,9 @@
       <c r="Q317" s="3"/>
       <c r="R317" s="3"/>
       <c r="S317" s="3"/>
-      <c r="T317" s="3"/>
+      <c r="T317" s="3">
+        <v>8.4600000000000009</v>
+      </c>
       <c r="U317" s="3"/>
       <c r="V317" s="3">
         <v>97.5</v>
@@ -22065,6 +22246,9 @@
       <c r="P318">
         <v>37</v>
       </c>
+      <c r="T318">
+        <v>8.8699999999999992</v>
+      </c>
       <c r="V318">
         <v>86.6</v>
       </c>
@@ -22111,7 +22295,9 @@
       <c r="Q319" s="3"/>
       <c r="R319" s="3"/>
       <c r="S319" s="3"/>
-      <c r="T319" s="3"/>
+      <c r="T319" s="3">
+        <v>7.61</v>
+      </c>
       <c r="U319" s="3"/>
       <c r="V319" s="3">
         <v>62</v>
@@ -22166,7 +22352,9 @@
         <v>1427</v>
       </c>
       <c r="S320" s="12"/>
-      <c r="T320" s="30"/>
+      <c r="T320" s="30">
+        <v>9.3800000000000008</v>
+      </c>
       <c r="U320" s="30"/>
       <c r="V320" s="30">
         <v>61.9</v>
@@ -22219,7 +22407,9 @@
       <c r="Q321" s="3"/>
       <c r="R321" s="3"/>
       <c r="S321" s="3"/>
-      <c r="T321" s="3"/>
+      <c r="T321" s="3">
+        <v>9.27</v>
+      </c>
       <c r="U321" s="3"/>
       <c r="V321" s="3">
         <v>83.8</v>
@@ -22267,6 +22457,9 @@
       <c r="P322">
         <v>37</v>
       </c>
+      <c r="T322">
+        <v>9.2799999999999994</v>
+      </c>
       <c r="V322">
         <v>78</v>
       </c>
@@ -22313,7 +22506,9 @@
       <c r="Q323" s="3"/>
       <c r="R323" s="3"/>
       <c r="S323" s="3"/>
-      <c r="T323" s="3"/>
+      <c r="T323" s="3">
+        <v>8.41</v>
+      </c>
       <c r="U323" s="3"/>
       <c r="V323" s="3">
         <v>76.900000000000006</v>
@@ -22361,6 +22556,9 @@
       <c r="P324">
         <v>37</v>
       </c>
+      <c r="T324">
+        <v>6.35</v>
+      </c>
       <c r="V324">
         <v>58.8</v>
       </c>
@@ -22407,7 +22605,9 @@
       <c r="Q325" s="3"/>
       <c r="R325" s="3"/>
       <c r="S325" s="3"/>
-      <c r="T325" s="3"/>
+      <c r="T325" s="3">
+        <v>7.99</v>
+      </c>
       <c r="U325" s="3"/>
       <c r="V325" s="3">
         <v>102.3</v>
@@ -22455,6 +22655,9 @@
       <c r="P326">
         <v>37</v>
       </c>
+      <c r="T326">
+        <v>8.33</v>
+      </c>
       <c r="V326">
         <v>91</v>
       </c>
@@ -22501,9 +22704,13 @@
       <c r="Q327" s="3"/>
       <c r="R327" s="3"/>
       <c r="S327" s="3"/>
-      <c r="T327" s="3"/>
+      <c r="T327" s="3">
+        <v>7.2</v>
+      </c>
       <c r="U327" s="3"/>
-      <c r="V327" s="3"/>
+      <c r="V327" s="3">
+        <v>83.3</v>
+      </c>
       <c r="W327" s="3"/>
       <c r="X327" s="3"/>
       <c r="Y327" s="3"/>
@@ -22550,6 +22757,12 @@
       <c r="S328" s="19" t="s">
         <v>1409</v>
       </c>
+      <c r="T328">
+        <v>7.71</v>
+      </c>
+      <c r="V328">
+        <v>62</v>
+      </c>
     </row>
     <row r="329" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A329" s="3" t="s">
@@ -22593,9 +22806,13 @@
       <c r="Q329" s="3"/>
       <c r="R329" s="3"/>
       <c r="S329" s="3"/>
-      <c r="T329" s="3"/>
+      <c r="T329" s="3">
+        <v>8.4499999999999993</v>
+      </c>
       <c r="U329" s="3"/>
-      <c r="V329" s="3"/>
+      <c r="V329" s="3">
+        <v>84.2</v>
+      </c>
       <c r="W329" s="3"/>
       <c r="X329" s="3"/>
       <c r="Y329" s="3"/>
@@ -22639,6 +22856,12 @@
       <c r="P330">
         <v>57</v>
       </c>
+      <c r="T330">
+        <v>8.4600000000000009</v>
+      </c>
+      <c r="V330">
+        <v>91.4</v>
+      </c>
     </row>
     <row r="331" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A331" s="3" t="s">
@@ -22682,9 +22905,13 @@
       <c r="Q331" s="3"/>
       <c r="R331" s="3"/>
       <c r="S331" s="3"/>
-      <c r="T331" s="3"/>
+      <c r="T331" s="3">
+        <v>7.02</v>
+      </c>
       <c r="U331" s="3"/>
-      <c r="V331" s="3"/>
+      <c r="V331" s="3">
+        <v>68.3</v>
+      </c>
       <c r="W331" s="3"/>
       <c r="X331" s="3"/>
       <c r="Y331" s="3"/>
@@ -22735,7 +22962,9 @@
         <v>1427</v>
       </c>
       <c r="S332" s="12"/>
-      <c r="T332" s="30"/>
+      <c r="T332" s="30">
+        <v>8.1999999999999993</v>
+      </c>
       <c r="U332" s="30"/>
       <c r="V332" s="30">
         <v>85.2</v>
@@ -22792,7 +23021,9 @@
         <v>1427</v>
       </c>
       <c r="S333" s="12"/>
-      <c r="T333" s="30"/>
+      <c r="T333" s="30">
+        <v>7.26</v>
+      </c>
       <c r="U333" s="30"/>
       <c r="V333" s="30">
         <v>99.6</v>
@@ -22847,7 +23078,9 @@
         <v>1427</v>
       </c>
       <c r="S334" s="12"/>
-      <c r="T334" s="30"/>
+      <c r="T334" s="30">
+        <v>6.75</v>
+      </c>
       <c r="U334" s="30"/>
       <c r="V334" s="30">
         <v>95.4</v>
@@ -22900,7 +23133,9 @@
       <c r="Q335" s="3"/>
       <c r="R335" s="3"/>
       <c r="S335" s="3"/>
-      <c r="T335" s="3"/>
+      <c r="T335" s="3">
+        <v>9.31</v>
+      </c>
       <c r="U335" s="3"/>
       <c r="V335" s="3">
         <v>74.400000000000006</v>
@@ -22948,6 +23183,9 @@
       <c r="P336">
         <v>37</v>
       </c>
+      <c r="T336">
+        <v>7.61</v>
+      </c>
       <c r="V336">
         <v>87.7</v>
       </c>
@@ -23000,7 +23238,9 @@
       <c r="S337" s="12" t="s">
         <v>1388</v>
       </c>
-      <c r="T337" s="30"/>
+      <c r="T337" s="30">
+        <v>8.2200000000000006</v>
+      </c>
       <c r="U337" s="30"/>
       <c r="V337" s="30">
         <v>94.5</v>
@@ -23048,6 +23288,9 @@
       <c r="P338">
         <v>37</v>
       </c>
+      <c r="T338">
+        <v>8.8800000000000008</v>
+      </c>
       <c r="V338">
         <v>71.7</v>
       </c>
@@ -23098,7 +23341,9 @@
         <v>1427</v>
       </c>
       <c r="S339" s="12"/>
-      <c r="T339" s="30"/>
+      <c r="T339" s="30">
+        <v>6.92</v>
+      </c>
       <c r="U339" s="30"/>
       <c r="V339" s="30">
         <v>63.9</v>
@@ -23146,6 +23391,9 @@
       <c r="P340">
         <v>37</v>
       </c>
+      <c r="T340">
+        <v>6.76</v>
+      </c>
       <c r="V340">
         <v>64.3</v>
       </c>
@@ -23192,7 +23440,9 @@
       <c r="Q341" s="3"/>
       <c r="R341" s="3"/>
       <c r="S341" s="3"/>
-      <c r="T341" s="3"/>
+      <c r="T341" s="3">
+        <v>9.11</v>
+      </c>
       <c r="U341" s="3"/>
       <c r="V341" s="3">
         <v>110.4</v>
@@ -23240,6 +23490,12 @@
       <c r="P342">
         <v>57</v>
       </c>
+      <c r="T342">
+        <v>7.78</v>
+      </c>
+      <c r="V342">
+        <v>87.4</v>
+      </c>
     </row>
     <row r="343" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A343" s="3" t="s">
@@ -23283,9 +23539,13 @@
       <c r="Q343" s="3"/>
       <c r="R343" s="3"/>
       <c r="S343" s="3"/>
-      <c r="T343" s="3"/>
+      <c r="T343" s="3">
+        <v>8.7100000000000009</v>
+      </c>
       <c r="U343" s="3"/>
-      <c r="V343" s="3"/>
+      <c r="V343" s="3">
+        <v>86.4</v>
+      </c>
       <c r="W343" s="3"/>
       <c r="X343" s="3"/>
       <c r="Y343" s="3"/>
@@ -23329,6 +23589,12 @@
       <c r="P344">
         <v>57</v>
       </c>
+      <c r="T344">
+        <v>8.42</v>
+      </c>
+      <c r="V344">
+        <v>106.6</v>
+      </c>
     </row>
     <row r="345" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A345" s="3" t="s">
@@ -23372,9 +23638,13 @@
       <c r="Q345" s="3"/>
       <c r="R345" s="3"/>
       <c r="S345" s="19"/>
-      <c r="T345" s="3"/>
+      <c r="T345" s="3">
+        <v>7.05</v>
+      </c>
       <c r="U345" s="3"/>
-      <c r="V345" s="3"/>
+      <c r="V345" s="3">
+        <v>100.7</v>
+      </c>
       <c r="W345" s="3"/>
       <c r="X345" s="3"/>
       <c r="Y345" s="3"/>
@@ -23425,9 +23695,13 @@
         <v>1427</v>
       </c>
       <c r="S346" s="17"/>
-      <c r="T346" s="30"/>
+      <c r="T346" s="30">
+        <v>8.24</v>
+      </c>
       <c r="U346" s="30"/>
-      <c r="V346" s="30"/>
+      <c r="V346" s="30">
+        <v>101.7</v>
+      </c>
       <c r="W346" s="30"/>
       <c r="X346" s="30"/>
       <c r="Y346" s="30"/>
@@ -23476,7 +23750,9 @@
       <c r="Q347" s="3"/>
       <c r="R347" s="3"/>
       <c r="S347" s="3"/>
-      <c r="T347" s="3"/>
+      <c r="T347" s="3">
+        <v>9.3000000000000007</v>
+      </c>
       <c r="U347" s="3"/>
       <c r="V347" s="3">
         <v>85.3</v>
@@ -23524,6 +23800,9 @@
       <c r="P348">
         <v>37</v>
       </c>
+      <c r="T348">
+        <v>8.59</v>
+      </c>
       <c r="V348">
         <v>91.9</v>
       </c>
@@ -23570,7 +23849,9 @@
       <c r="Q349" s="3"/>
       <c r="R349" s="3"/>
       <c r="S349" s="3"/>
-      <c r="T349" s="3"/>
+      <c r="T349" s="3">
+        <v>7.68</v>
+      </c>
       <c r="U349" s="3"/>
       <c r="V349" s="3">
         <v>75.900000000000006</v>
@@ -23621,6 +23902,9 @@
       <c r="S350" s="11" t="s">
         <v>1387</v>
       </c>
+      <c r="T350">
+        <v>6.1</v>
+      </c>
       <c r="V350">
         <v>71.8</v>
       </c>
@@ -23667,7 +23951,9 @@
       <c r="Q351" s="3"/>
       <c r="R351" s="3"/>
       <c r="S351" s="3"/>
-      <c r="T351" s="3"/>
+      <c r="T351" s="3">
+        <v>8.1199999999999992</v>
+      </c>
       <c r="U351" s="3"/>
       <c r="V351" s="3">
         <v>91.7</v>
@@ -23715,6 +24001,9 @@
       <c r="P352">
         <v>37</v>
       </c>
+      <c r="T352">
+        <v>8.7200000000000006</v>
+      </c>
       <c r="V352">
         <v>84.1</v>
       </c>
@@ -23760,7 +24049,9 @@
       <c r="Q353" s="3"/>
       <c r="R353" s="3"/>
       <c r="S353" s="3"/>
-      <c r="T353" s="3"/>
+      <c r="T353" s="3">
+        <v>7.53</v>
+      </c>
       <c r="U353" s="3"/>
       <c r="V353" s="3">
         <v>82.8</v>
@@ -23808,6 +24099,9 @@
       <c r="P354">
         <v>37</v>
       </c>
+      <c r="T354">
+        <v>7.43</v>
+      </c>
       <c r="V354">
         <v>82.9</v>
       </c>
@@ -23856,9 +24150,13 @@
       <c r="S355" s="11" t="s">
         <v>1391</v>
       </c>
-      <c r="T355" s="3"/>
+      <c r="T355" s="3" t="s">
+        <v>1386</v>
+      </c>
       <c r="U355" s="3"/>
-      <c r="V355" s="3"/>
+      <c r="V355" s="3" t="s">
+        <v>1386</v>
+      </c>
       <c r="W355" s="3"/>
       <c r="X355" s="3"/>
       <c r="Y355" s="3"/>
@@ -23909,7 +24207,9 @@
         <v>1427</v>
       </c>
       <c r="S356" s="12"/>
-      <c r="T356" s="30"/>
+      <c r="T356" s="30">
+        <v>8</v>
+      </c>
       <c r="U356" s="30"/>
       <c r="V356" s="30">
         <v>87</v>
@@ -23962,9 +24262,13 @@
       <c r="Q357" s="3"/>
       <c r="R357" s="3"/>
       <c r="S357" s="3"/>
-      <c r="T357" s="3"/>
+      <c r="T357" s="3">
+        <v>8.5299999999999994</v>
+      </c>
       <c r="U357" s="3"/>
-      <c r="V357" s="3"/>
+      <c r="V357" s="3">
+        <v>51.8</v>
+      </c>
       <c r="W357" s="3"/>
       <c r="X357" s="3"/>
       <c r="Y357" s="3"/>
@@ -24008,6 +24312,12 @@
       <c r="P358">
         <v>57</v>
       </c>
+      <c r="T358">
+        <v>8.4700000000000006</v>
+      </c>
+      <c r="V358">
+        <v>83</v>
+      </c>
     </row>
     <row r="359" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A359" s="3" t="s">
@@ -24051,9 +24361,13 @@
       <c r="Q359" s="3"/>
       <c r="R359" s="3"/>
       <c r="S359" s="3"/>
-      <c r="T359" s="3"/>
+      <c r="T359" s="3">
+        <v>8.6</v>
+      </c>
       <c r="U359" s="3"/>
-      <c r="V359" s="3"/>
+      <c r="V359" s="3">
+        <v>60.9</v>
+      </c>
       <c r="W359" s="3"/>
       <c r="X359" s="3"/>
       <c r="Y359" s="3"/>
@@ -24097,6 +24411,12 @@
       <c r="P360">
         <v>57</v>
       </c>
+      <c r="T360">
+        <v>8.82</v>
+      </c>
+      <c r="V360">
+        <v>119.4</v>
+      </c>
     </row>
     <row r="361" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A361" s="3" t="s">
@@ -24140,9 +24460,13 @@
       <c r="Q361" s="3"/>
       <c r="R361" s="3"/>
       <c r="S361" s="3"/>
-      <c r="T361" s="3"/>
+      <c r="T361" s="3">
+        <v>8.3000000000000007</v>
+      </c>
       <c r="U361" s="3"/>
-      <c r="V361" s="3"/>
+      <c r="V361" s="3">
+        <v>122.3</v>
+      </c>
       <c r="W361" s="3"/>
       <c r="X361" s="3"/>
       <c r="Y361" s="3"/>
@@ -33907,7 +34231,7 @@
       <c r="Z541" s="3"/>
       <c r="AA541" s="3"/>
     </row>
-    <row r="542" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="542" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A542" s="1" t="s">
         <v>1261</v>
       </c>
@@ -33947,11 +34271,14 @@
       <c r="S542" s="12" t="s">
         <v>1391</v>
       </c>
+      <c r="T542" s="48" t="s">
+        <v>1386</v>
+      </c>
       <c r="X542">
         <v>328</v>
       </c>
     </row>
-    <row r="543" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="543" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A543" s="3" t="s">
         <v>1264</v>
       </c>
@@ -33993,7 +34320,9 @@
       <c r="Q543" s="3"/>
       <c r="R543" s="3"/>
       <c r="S543" s="3"/>
-      <c r="T543" s="3"/>
+      <c r="T543" s="3">
+        <v>11.22</v>
+      </c>
       <c r="U543" s="3"/>
       <c r="V543" s="3">
         <v>31.7</v>
@@ -34006,7 +34335,7 @@
       <c r="Z543" s="3"/>
       <c r="AA543" s="3"/>
     </row>
-    <row r="544" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="544" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A544" s="1" t="s">
         <v>1265</v>
       </c>
@@ -34046,11 +34375,14 @@
       <c r="S544" s="12" t="s">
         <v>1391</v>
       </c>
+      <c r="T544" s="48" t="s">
+        <v>1386</v>
+      </c>
       <c r="X544">
         <v>328</v>
       </c>
     </row>
-    <row r="545" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="545" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A545" s="3" t="s">
         <v>1266</v>
       </c>
@@ -34092,7 +34424,9 @@
       <c r="Q545" s="3"/>
       <c r="R545" s="3"/>
       <c r="S545" s="3"/>
-      <c r="T545" s="3"/>
+      <c r="T545" s="3">
+        <v>9.26</v>
+      </c>
       <c r="U545" s="3"/>
       <c r="V545" s="3">
         <v>26.7</v>
@@ -34105,7 +34439,7 @@
       <c r="Z545" s="3"/>
       <c r="AA545" s="3"/>
     </row>
-    <row r="546" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="546" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A546" s="1" t="s">
         <v>1267</v>
       </c>
@@ -34142,6 +34476,9 @@
       <c r="P546">
         <v>37</v>
       </c>
+      <c r="T546">
+        <v>9.0399999999999991</v>
+      </c>
       <c r="V546">
         <v>23.8</v>
       </c>
@@ -34149,7 +34486,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="547" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="547" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A547" s="3" t="s">
         <v>1269</v>
       </c>
@@ -34206,7 +34543,7 @@
       <c r="Z547" s="15"/>
       <c r="AA547" s="3"/>
     </row>
-    <row r="548" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="548" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A548" s="1" t="s">
         <v>1270</v>
       </c>
@@ -34254,7 +34591,7 @@
       </c>
       <c r="Z548" s="15"/>
     </row>
-    <row r="549" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="549" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A549" s="3" t="s">
         <v>1271</v>
       </c>
@@ -34311,7 +34648,7 @@
       <c r="Z549" s="15"/>
       <c r="AA549" s="3"/>
     </row>
-    <row r="550" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="550" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A550" s="1" t="s">
         <v>1272</v>
       </c>
@@ -34359,7 +34696,7 @@
       </c>
       <c r="Z550" s="15"/>
     </row>
-    <row r="551" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="551" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A551" s="3" t="s">
         <v>1274</v>
       </c>
@@ -34456,6 +34793,9 @@
       <c r="S552" s="17" t="s">
         <v>1391</v>
       </c>
+      <c r="T552" s="48" t="s">
+        <v>1386</v>
+      </c>
       <c r="X552">
         <v>328</v>
       </c>
@@ -34503,7 +34843,9 @@
       <c r="Q553" s="3"/>
       <c r="R553" s="3"/>
       <c r="S553" s="3"/>
-      <c r="T553" s="3"/>
+      <c r="T553" s="3">
+        <v>9.35</v>
+      </c>
       <c r="U553" s="3"/>
       <c r="V553" s="3">
         <v>24.7</v>
@@ -34556,6 +34898,9 @@
       <c r="S554" s="17" t="s">
         <v>1391</v>
       </c>
+      <c r="T554" s="48" t="s">
+        <v>1386</v>
+      </c>
       <c r="X554">
         <v>328</v>
       </c>
@@ -34603,7 +34948,9 @@
       <c r="Q555" s="3"/>
       <c r="R555" s="3"/>
       <c r="S555" s="3"/>
-      <c r="T555" s="3"/>
+      <c r="T555" s="3">
+        <v>7.21</v>
+      </c>
       <c r="U555" s="3"/>
       <c r="V555" s="3">
         <v>30.1</v>
@@ -34653,6 +35000,9 @@
       <c r="P556">
         <v>57</v>
       </c>
+      <c r="T556">
+        <v>9.6199999999999992</v>
+      </c>
       <c r="V556">
         <v>28.2</v>
       </c>
@@ -34661,7 +35011,7 @@
       </c>
       <c r="Z556" s="15"/>
     </row>
-    <row r="557" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="557" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A557" s="3" t="s">
         <v>1283</v>
       </c>
@@ -34703,7 +35053,9 @@
       <c r="Q557" s="3"/>
       <c r="R557" s="3"/>
       <c r="S557" s="3"/>
-      <c r="T557" s="3"/>
+      <c r="T557" s="3">
+        <v>9.16</v>
+      </c>
       <c r="U557" s="3"/>
       <c r="V557" s="3">
         <v>24.1</v>
@@ -34716,7 +35068,7 @@
       <c r="Z557" s="15"/>
       <c r="AA557" s="3"/>
     </row>
-    <row r="558" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="558" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A558" s="1" t="s">
         <v>1284</v>
       </c>
@@ -34756,12 +35108,15 @@
       <c r="S558" s="12" t="s">
         <v>1391</v>
       </c>
+      <c r="T558" s="48" t="s">
+        <v>1386</v>
+      </c>
       <c r="X558">
         <v>328</v>
       </c>
       <c r="Z558" s="15"/>
     </row>
-    <row r="559" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="559" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A559" s="3" t="s">
         <v>1286</v>
       </c>
@@ -34805,7 +35160,9 @@
       <c r="S559" s="11" t="s">
         <v>1391</v>
       </c>
-      <c r="T559" s="3"/>
+      <c r="T559" s="3" t="s">
+        <v>1386</v>
+      </c>
       <c r="U559" s="3"/>
       <c r="V559" s="3"/>
       <c r="W559" s="3"/>
@@ -34816,7 +35173,7 @@
       <c r="Z559" s="15"/>
       <c r="AA559" s="3"/>
     </row>
-    <row r="560" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="560" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A560" s="1" t="s">
         <v>1287</v>
       </c>
@@ -34856,12 +35213,15 @@
       <c r="S560" s="12" t="s">
         <v>1391</v>
       </c>
+      <c r="T560" s="48" t="s">
+        <v>1386</v>
+      </c>
       <c r="X560">
         <v>328</v>
       </c>
       <c r="Z560" s="15"/>
     </row>
-    <row r="561" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="561" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A561" s="3" t="s">
         <v>1288</v>
       </c>
@@ -34903,7 +35263,9 @@
       <c r="Q561" s="3"/>
       <c r="R561" s="3"/>
       <c r="S561" s="3"/>
-      <c r="T561" s="3"/>
+      <c r="T561" s="3">
+        <v>6.42</v>
+      </c>
       <c r="U561" s="3"/>
       <c r="V561" s="3">
         <v>21.4</v>
@@ -34916,7 +35278,7 @@
       <c r="Z561" s="15"/>
       <c r="AA561" s="3"/>
     </row>
-    <row r="562" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="562" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A562" s="1" t="s">
         <v>1290</v>
       </c>
@@ -34964,7 +35326,7 @@
       </c>
       <c r="Z562" s="15"/>
     </row>
-    <row r="563" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="563" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A563" s="3" t="s">
         <v>1293</v>
       </c>
@@ -35021,7 +35383,7 @@
       <c r="Z563" s="15"/>
       <c r="AA563" s="3"/>
     </row>
-    <row r="564" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="564" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A564" s="1" t="s">
         <v>1295</v>
       </c>
@@ -35069,7 +35431,7 @@
       </c>
       <c r="Z564" s="15"/>
     </row>
-    <row r="565" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="565" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A565" s="3" t="s">
         <v>1297</v>
       </c>
@@ -35126,7 +35488,7 @@
       <c r="Z565" s="15"/>
       <c r="AA565" s="3"/>
     </row>
-    <row r="566" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="566" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A566" s="1" t="s">
         <v>1298</v>
       </c>
@@ -35216,7 +35578,9 @@
       <c r="Q567" s="3"/>
       <c r="R567" s="3"/>
       <c r="S567" s="3"/>
-      <c r="T567" s="3"/>
+      <c r="T567" s="3">
+        <v>8.9</v>
+      </c>
       <c r="U567" s="3"/>
       <c r="V567" s="3">
         <v>33.6</v>
@@ -35266,6 +35630,9 @@
       <c r="P568">
         <v>57</v>
       </c>
+      <c r="T568">
+        <v>10.42</v>
+      </c>
       <c r="V568">
         <v>27.7</v>
       </c>
@@ -35316,7 +35683,9 @@
       <c r="Q569" s="3"/>
       <c r="R569" s="3"/>
       <c r="S569" s="3"/>
-      <c r="T569" s="3"/>
+      <c r="T569" s="3">
+        <v>13.02</v>
+      </c>
       <c r="U569" s="3"/>
       <c r="V569" s="3">
         <v>30.2</v>
@@ -35365,6 +35734,9 @@
       </c>
       <c r="P570">
         <v>57</v>
+      </c>
+      <c r="T570">
+        <v>10.76</v>
       </c>
       <c r="V570">
         <v>34.299999999999997</v>
@@ -35418,7 +35790,9 @@
       <c r="S571" s="11" t="s">
         <v>1391</v>
       </c>
-      <c r="T571" s="3"/>
+      <c r="T571" s="3" t="s">
+        <v>1386</v>
+      </c>
       <c r="U571" s="3"/>
       <c r="V571" s="3"/>
       <c r="W571" s="3"/>
@@ -35429,7 +35803,7 @@
       <c r="Z571" s="15"/>
       <c r="AA571" s="3"/>
     </row>
-    <row r="572" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="572" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A572" s="1" t="s">
         <v>1306</v>
       </c>
@@ -35466,6 +35840,9 @@
       <c r="P572">
         <v>37</v>
       </c>
+      <c r="T572">
+        <v>10.18</v>
+      </c>
       <c r="V572">
         <v>28.2</v>
       </c>
@@ -35474,7 +35851,7 @@
       </c>
       <c r="Z572" s="15"/>
     </row>
-    <row r="573" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="573" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A573" s="3" t="s">
         <v>1308</v>
       </c>
@@ -35514,7 +35891,9 @@
       <c r="Q573" s="3"/>
       <c r="R573" s="3"/>
       <c r="S573" s="3"/>
-      <c r="T573" s="3"/>
+      <c r="T573" s="3">
+        <v>11.89</v>
+      </c>
       <c r="U573" s="3"/>
       <c r="V573" s="3">
         <v>30</v>
@@ -35527,7 +35906,7 @@
       <c r="Z573" s="15"/>
       <c r="AA573" s="3"/>
     </row>
-    <row r="574" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="574" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A574" s="1" t="s">
         <v>1310</v>
       </c>
@@ -35567,12 +35946,15 @@
       <c r="S574" s="12" t="s">
         <v>1391</v>
       </c>
+      <c r="T574" s="48" t="s">
+        <v>1386</v>
+      </c>
       <c r="X574">
         <v>328</v>
       </c>
       <c r="Z574" s="15"/>
     </row>
-    <row r="575" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="575" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A575" s="3" t="s">
         <v>1311</v>
       </c>
@@ -35616,7 +35998,9 @@
       <c r="S575" s="11" t="s">
         <v>1391</v>
       </c>
-      <c r="T575" s="3"/>
+      <c r="T575" s="3" t="s">
+        <v>1386</v>
+      </c>
       <c r="U575" s="3"/>
       <c r="V575" s="3"/>
       <c r="W575" s="3"/>
@@ -35627,7 +36011,7 @@
       <c r="Z575" s="15"/>
       <c r="AA575" s="3"/>
     </row>
-    <row r="576" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="576" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A576" s="1" t="s">
         <v>1312</v>
       </c>
@@ -35667,12 +36051,15 @@
       <c r="S576" s="12" t="s">
         <v>1391</v>
       </c>
+      <c r="T576" s="48" t="s">
+        <v>1386</v>
+      </c>
       <c r="X576">
         <v>328</v>
       </c>
       <c r="Z576" s="15"/>
     </row>
-    <row r="577" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="577" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A577" s="3" t="s">
         <v>1313</v>
       </c>
@@ -35729,7 +36116,7 @@
       <c r="Z577" s="15"/>
       <c r="AA577" s="3"/>
     </row>
-    <row r="578" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="578" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A578" s="1" t="s">
         <v>1315</v>
       </c>
@@ -35777,7 +36164,7 @@
       </c>
       <c r="Z578" s="15"/>
     </row>
-    <row r="579" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="579" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A579" s="3" t="s">
         <v>1316</v>
       </c>
@@ -35834,7 +36221,7 @@
       <c r="Z579" s="15"/>
       <c r="AA579" s="3"/>
     </row>
-    <row r="580" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="580" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A580" s="1" t="s">
         <v>1317</v>
       </c>
@@ -35882,7 +36269,7 @@
       </c>
       <c r="Z580" s="15"/>
     </row>
-    <row r="581" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="581" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A581" s="3" t="s">
         <v>1318</v>
       </c>
@@ -35976,6 +36363,9 @@
       <c r="P582">
         <v>57</v>
       </c>
+      <c r="T582">
+        <v>12.36</v>
+      </c>
       <c r="V582">
         <v>28.4</v>
       </c>
@@ -36028,7 +36418,9 @@
       <c r="S583" s="11" t="s">
         <v>1391</v>
       </c>
-      <c r="T583" s="3"/>
+      <c r="T583" s="3" t="s">
+        <v>1386</v>
+      </c>
       <c r="U583" s="3"/>
       <c r="V583" s="3"/>
       <c r="W583" s="3"/>
@@ -36076,6 +36468,9 @@
       <c r="P584">
         <v>57</v>
       </c>
+      <c r="T584">
+        <v>10.199999999999999</v>
+      </c>
       <c r="V584">
         <v>23.4</v>
       </c>
@@ -36126,7 +36521,9 @@
       <c r="Q585" s="3"/>
       <c r="R585" s="3"/>
       <c r="S585" s="3"/>
-      <c r="T585" s="3"/>
+      <c r="T585" s="3">
+        <v>14.38</v>
+      </c>
       <c r="U585" s="3"/>
       <c r="V585" s="3">
         <v>33.4</v>
@@ -36176,6 +36573,9 @@
       <c r="P586">
         <v>57</v>
       </c>
+      <c r="T586">
+        <v>13.34</v>
+      </c>
       <c r="V586">
         <v>34.5</v>
       </c>
@@ -36184,7 +36584,7 @@
       </c>
       <c r="Z586" s="15"/>
     </row>
-    <row r="587" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="587" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A587" s="3" t="s">
         <v>1327</v>
       </c>
@@ -36226,7 +36626,9 @@
       <c r="Q587" s="3"/>
       <c r="R587" s="3"/>
       <c r="S587" s="3"/>
-      <c r="T587" s="3"/>
+      <c r="T587" s="3">
+        <v>9.81</v>
+      </c>
       <c r="U587" s="3"/>
       <c r="V587" s="3">
         <v>34.4</v>
@@ -36239,7 +36641,7 @@
       <c r="Z587" s="15"/>
       <c r="AA587" s="3"/>
     </row>
-    <row r="588" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="588" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A588" s="1" t="s">
         <v>1328</v>
       </c>
@@ -36279,12 +36681,15 @@
       <c r="S588" s="12" t="s">
         <v>1391</v>
       </c>
+      <c r="T588" s="48" t="s">
+        <v>1386</v>
+      </c>
       <c r="X588">
         <v>328</v>
       </c>
       <c r="Z588" s="15"/>
     </row>
-    <row r="589" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="589" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A589" s="3" t="s">
         <v>1329</v>
       </c>
@@ -36328,7 +36733,9 @@
       <c r="S589" s="11" t="s">
         <v>1391</v>
       </c>
-      <c r="T589" s="3"/>
+      <c r="T589" s="3" t="s">
+        <v>1386</v>
+      </c>
       <c r="U589" s="3"/>
       <c r="V589" s="3"/>
       <c r="W589" s="3"/>
@@ -36339,7 +36746,7 @@
       <c r="Z589" s="15"/>
       <c r="AA589" s="3"/>
     </row>
-    <row r="590" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="590" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A590" s="1" t="s">
         <v>1330</v>
       </c>
@@ -36379,12 +36786,15 @@
       <c r="S590" s="12" t="s">
         <v>1391</v>
       </c>
+      <c r="T590" s="48" t="s">
+        <v>1386</v>
+      </c>
       <c r="X590">
         <v>328</v>
       </c>
       <c r="Z590" s="15"/>
     </row>
-    <row r="591" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="591" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A591" s="3" t="s">
         <v>1331</v>
       </c>
@@ -36426,7 +36836,9 @@
       <c r="Q591" s="3"/>
       <c r="R591" s="3"/>
       <c r="S591" s="3"/>
-      <c r="T591" s="3"/>
+      <c r="T591" s="3">
+        <v>7.49</v>
+      </c>
       <c r="U591" s="3"/>
       <c r="V591" s="3">
         <v>24.1</v>
@@ -36439,7 +36851,7 @@
       <c r="Z591" s="15"/>
       <c r="AA591" s="3"/>
     </row>
-    <row r="592" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="592" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A592" s="1" t="s">
         <v>1332</v>
       </c>
@@ -36487,7 +36899,7 @@
       </c>
       <c r="Z592" s="15"/>
     </row>
-    <row r="593" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="593" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A593" s="3" t="s">
         <v>1333</v>
       </c>
@@ -36544,7 +36956,7 @@
       <c r="Z593" s="15"/>
       <c r="AA593" s="3"/>
     </row>
-    <row r="594" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="594" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A594" s="1" t="s">
         <v>1335</v>
       </c>
@@ -36589,7 +37001,7 @@
       </c>
       <c r="Z594" s="15"/>
     </row>
-    <row r="595" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="595" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A595" s="3" t="s">
         <v>1336</v>
       </c>
@@ -36650,7 +37062,7 @@
       <c r="Z595" s="15"/>
       <c r="AA595" s="11"/>
     </row>
-    <row r="596" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+    <row r="596" spans="1:27" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A596" s="1" t="s">
         <v>1337</v>
       </c>
@@ -36739,7 +37151,9 @@
       <c r="S597" s="11" t="s">
         <v>1391</v>
       </c>
-      <c r="T597" s="3"/>
+      <c r="T597" s="3" t="s">
+        <v>1386</v>
+      </c>
       <c r="U597" s="3"/>
       <c r="V597" s="3"/>
       <c r="W597" s="3"/>
@@ -36787,6 +37201,9 @@
       <c r="P598">
         <v>57</v>
       </c>
+      <c r="T598">
+        <v>10.54</v>
+      </c>
       <c r="V598">
         <v>29.1</v>
       </c>
@@ -36837,7 +37254,9 @@
       <c r="Q599" s="3"/>
       <c r="R599" s="3"/>
       <c r="S599" s="3"/>
-      <c r="T599" s="3"/>
+      <c r="T599" s="3">
+        <v>11.48</v>
+      </c>
       <c r="U599" s="3"/>
       <c r="V599" s="3">
         <v>35.799999999999997</v>
@@ -36879,13 +37298,16 @@
       </c>
       <c r="K600" s="6"/>
       <c r="L600">
-        <v>40</v>
+        <v>4</v>
       </c>
       <c r="N600">
         <v>17.399999999999999</v>
       </c>
       <c r="P600">
         <v>57</v>
+      </c>
+      <c r="T600">
+        <v>7.74</v>
       </c>
       <c r="V600">
         <v>27.5</v>
@@ -36937,7 +37359,9 @@
       <c r="Q601" s="3"/>
       <c r="R601" s="3"/>
       <c r="S601" s="3"/>
-      <c r="T601" s="3"/>
+      <c r="T601" s="3">
+        <v>10.57</v>
+      </c>
       <c r="U601" s="3"/>
       <c r="V601" s="3">
         <v>37</v>
@@ -36950,7 +37374,7 @@
       <c r="Z601" s="15"/>
       <c r="AA601" s="3"/>
     </row>
-    <row r="602" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="602" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A602" s="1" t="s">
         <v>1347</v>
       </c>
@@ -36990,12 +37414,15 @@
       <c r="S602" s="12" t="s">
         <v>1391</v>
       </c>
+      <c r="T602" s="48" t="s">
+        <v>1386</v>
+      </c>
       <c r="X602">
         <v>328</v>
       </c>
       <c r="Z602" s="15"/>
     </row>
-    <row r="603" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="603" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A603" s="3" t="s">
         <v>1348</v>
       </c>
@@ -37037,7 +37464,9 @@
       <c r="Q603" s="3"/>
       <c r="R603" s="3"/>
       <c r="S603" s="3"/>
-      <c r="T603" s="3"/>
+      <c r="T603" s="3">
+        <v>9.23</v>
+      </c>
       <c r="U603" s="3"/>
       <c r="V603" s="3">
         <v>24.9</v>
@@ -37050,7 +37479,7 @@
       <c r="Z603" s="15"/>
       <c r="AA603" s="3"/>
     </row>
-    <row r="604" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="604" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A604" s="1" t="s">
         <v>1349</v>
       </c>
@@ -37087,6 +37516,9 @@
       <c r="P604">
         <v>37</v>
       </c>
+      <c r="T604">
+        <v>12.23</v>
+      </c>
       <c r="V604">
         <v>37.299999999999997</v>
       </c>
@@ -37095,7 +37527,7 @@
       </c>
       <c r="Z604" s="15"/>
     </row>
-    <row r="605" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="605" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A605" s="3" t="s">
         <v>1350</v>
       </c>
@@ -37137,7 +37569,9 @@
       <c r="Q605" s="3"/>
       <c r="R605" s="3"/>
       <c r="S605" s="3"/>
-      <c r="T605" s="3"/>
+      <c r="T605" s="3">
+        <v>9.77</v>
+      </c>
       <c r="U605" s="3"/>
       <c r="V605" s="3">
         <v>25.8</v>
@@ -37150,7 +37584,7 @@
       <c r="Z605" s="15"/>
       <c r="AA605" s="3"/>
     </row>
-    <row r="606" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="606" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A606" s="1" t="s">
         <v>1352</v>
       </c>
@@ -37187,6 +37621,9 @@
       <c r="P606">
         <v>37</v>
       </c>
+      <c r="T606">
+        <v>10.8</v>
+      </c>
       <c r="V606">
         <v>33.6</v>
       </c>
@@ -37195,7 +37632,7 @@
       </c>
       <c r="Z606" s="15"/>
     </row>
-    <row r="607" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="607" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A607" s="3" t="s">
         <v>1353</v>
       </c>
@@ -37252,7 +37689,7 @@
       <c r="Z607" s="15"/>
       <c r="AA607" s="3"/>
     </row>
-    <row r="608" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="608" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A608" s="1" t="s">
         <v>1354</v>
       </c>
@@ -37300,7 +37737,7 @@
       </c>
       <c r="Z608" s="15"/>
     </row>
-    <row r="609" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="609" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A609" s="3" t="s">
         <v>1355</v>
       </c>
@@ -37357,7 +37794,7 @@
       <c r="Z609" s="15"/>
       <c r="AA609" s="3"/>
     </row>
-    <row r="610" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="610" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A610" s="1" t="s">
         <v>1356</v>
       </c>
@@ -37405,7 +37842,7 @@
       </c>
       <c r="Z610" s="15"/>
     </row>
-    <row r="611" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="611" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A611" s="3" t="s">
         <v>1357</v>
       </c>
@@ -37497,6 +37934,9 @@
       <c r="P612">
         <v>57</v>
       </c>
+      <c r="T612">
+        <v>10.83</v>
+      </c>
       <c r="V612">
         <v>27.4</v>
       </c>
@@ -37547,7 +37987,9 @@
       <c r="Q613" s="3"/>
       <c r="R613" s="3"/>
       <c r="S613" s="3"/>
-      <c r="T613" s="3"/>
+      <c r="T613" s="3">
+        <v>9.92</v>
+      </c>
       <c r="U613" s="3"/>
       <c r="V613" s="3">
         <v>31.6</v>
@@ -37597,6 +38039,9 @@
       <c r="P614">
         <v>57</v>
       </c>
+      <c r="T614">
+        <v>11.45</v>
+      </c>
       <c r="V614">
         <v>29.4</v>
       </c>
@@ -37647,7 +38092,9 @@
       <c r="Q615" s="3"/>
       <c r="R615" s="3"/>
       <c r="S615" s="3"/>
-      <c r="T615" s="3"/>
+      <c r="T615" s="3">
+        <v>10.35</v>
+      </c>
       <c r="U615" s="3"/>
       <c r="V615" s="3">
         <v>32.9</v>
@@ -37700,12 +38147,15 @@
       <c r="S616" s="17" t="s">
         <v>1391</v>
       </c>
+      <c r="T616" s="48" t="s">
+        <v>1386</v>
+      </c>
       <c r="X616">
         <v>328</v>
       </c>
       <c r="Z616" s="15"/>
     </row>
-    <row r="617" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="617" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A617" s="3" t="s">
         <v>1366</v>
       </c>
@@ -37747,7 +38197,9 @@
       <c r="Q617" s="3"/>
       <c r="R617" s="3"/>
       <c r="S617" s="3"/>
-      <c r="T617" s="3"/>
+      <c r="T617" s="3">
+        <v>9.5399999999999991</v>
+      </c>
       <c r="U617" s="3"/>
       <c r="V617" s="3">
         <v>28.1</v>
@@ -37760,7 +38212,7 @@
       <c r="Z617" s="15"/>
       <c r="AA617" s="3"/>
     </row>
-    <row r="618" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="618" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A618" s="1" t="s">
         <v>1368</v>
       </c>
@@ -37797,6 +38249,9 @@
       <c r="P618">
         <v>37</v>
       </c>
+      <c r="T618">
+        <v>5.85</v>
+      </c>
       <c r="V618">
         <v>25.4</v>
       </c>
@@ -37805,7 +38260,7 @@
       </c>
       <c r="Z618" s="15"/>
     </row>
-    <row r="619" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="619" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A619" s="3" t="s">
         <v>1369</v>
       </c>
@@ -37847,7 +38302,9 @@
       <c r="Q619" s="3"/>
       <c r="R619" s="3"/>
       <c r="S619" s="3"/>
-      <c r="T619" s="3"/>
+      <c r="T619" s="3">
+        <v>9.51</v>
+      </c>
       <c r="U619" s="3"/>
       <c r="V619" s="3">
         <v>29.3</v>
@@ -37860,7 +38317,7 @@
       <c r="Z619" s="15"/>
       <c r="AA619" s="3"/>
     </row>
-    <row r="620" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="620" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A620" s="1" t="s">
         <v>1370</v>
       </c>
@@ -37900,12 +38357,15 @@
       <c r="S620" s="12" t="s">
         <v>1391</v>
       </c>
+      <c r="T620" s="48" t="s">
+        <v>1386</v>
+      </c>
       <c r="X620">
         <v>328</v>
       </c>
       <c r="Z620" s="15"/>
     </row>
-    <row r="621" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="621" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A621" s="3" t="s">
         <v>1371</v>
       </c>
@@ -37947,7 +38407,9 @@
       <c r="Q621" s="3"/>
       <c r="R621" s="3"/>
       <c r="S621" s="3"/>
-      <c r="T621" s="3"/>
+      <c r="T621" s="3">
+        <v>8.4</v>
+      </c>
       <c r="U621" s="3"/>
       <c r="V621" s="3">
         <v>26.4</v>
@@ -37960,7 +38422,7 @@
       <c r="Z621" s="15"/>
       <c r="AA621" s="3"/>
     </row>
-    <row r="622" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="622" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A622" s="1" t="s">
         <v>1372</v>
       </c>
@@ -38008,7 +38470,7 @@
       </c>
       <c r="Z622" s="15"/>
     </row>
-    <row r="623" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="623" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A623" s="3" t="s">
         <v>1373</v>
       </c>
@@ -38065,7 +38527,7 @@
       <c r="Z623" s="15"/>
       <c r="AA623" s="3"/>
     </row>
-    <row r="624" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="624" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A624" s="1" t="s">
         <v>1374</v>
       </c>
@@ -38113,7 +38575,7 @@
       </c>
       <c r="Z624" s="15"/>
     </row>
-    <row r="625" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="625" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A625" s="3" t="s">
         <v>1375</v>
       </c>
@@ -38170,7 +38632,7 @@
       <c r="Z625" s="15"/>
       <c r="AA625" s="3"/>
     </row>
-    <row r="626" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="626" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A626" s="1" t="s">
         <v>1377</v>
       </c>
@@ -38260,7 +38722,9 @@
       <c r="Q627" s="3"/>
       <c r="R627" s="3"/>
       <c r="S627" s="3"/>
-      <c r="T627" s="3"/>
+      <c r="T627" s="3">
+        <v>9.86</v>
+      </c>
       <c r="U627" s="3"/>
       <c r="V627" s="3">
         <v>27.3</v>
@@ -38310,6 +38774,9 @@
       <c r="P628">
         <v>57</v>
       </c>
+      <c r="T628">
+        <v>11.52</v>
+      </c>
       <c r="V628">
         <v>31.1</v>
       </c>
@@ -38359,7 +38826,9 @@
       <c r="Q629" s="3"/>
       <c r="R629" s="3"/>
       <c r="S629" s="3"/>
-      <c r="T629" s="3"/>
+      <c r="T629" s="3">
+        <v>11.64</v>
+      </c>
       <c r="U629" s="3"/>
       <c r="V629" s="3">
         <v>34.9</v>
@@ -38409,6 +38878,9 @@
       <c r="P630">
         <v>57</v>
       </c>
+      <c r="T630">
+        <v>13.24</v>
+      </c>
       <c r="V630">
         <v>32.4</v>
       </c>
@@ -38458,7 +38930,9 @@
       <c r="Q631" s="3"/>
       <c r="R631" s="3"/>
       <c r="S631" s="3"/>
-      <c r="T631" s="3"/>
+      <c r="T631" s="3">
+        <v>9.9499999999999993</v>
+      </c>
       <c r="U631" s="3"/>
       <c r="V631" s="3">
         <v>32.700000000000003</v>
@@ -39984,7 +40458,7 @@
       <c r="K820" s="6"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="23" type="noConversion"/>
+  <phoneticPr fontId="24" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
tree measurements csv  updates
</commit_message>
<xml_diff>
--- a/data/treeMeasurements/TreeMeasurements.xlsx
+++ b/data/treeMeasurements/TreeMeasurements.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11122"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christophe_rouleau-desrochers/github/fuelinex/data/treeMeasurements/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13C44731-F9C3-AB42-97F7-A86469471232}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0809BE55-2DC8-DE49-904D-C1C2604678FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4655,7 +4655,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -4705,6 +4705,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5349,14 +5351,9 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{3F288811-81FB-F847-9587-99D03002EDFF}" name="Table4" displayName="Table4" ref="A1:AA631" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
   <autoFilter ref="A1:AA631" xr:uid="{3F288811-81FB-F847-9587-99D03002EDFF}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="1"/>
-      </filters>
-    </filterColumn>
     <filterColumn colId="3">
       <filters>
-        <filter val="sequoiadendron"/>
+        <filter val="populus"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -5594,8 +5591,8 @@
   <dimension ref="A1:AA820"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="167" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="M1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="U617" sqref="U617"/>
+      <pane xSplit="1" topLeftCell="O1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="V355" sqref="V355"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5613,7 +5610,7 @@
     <col min="11" max="11" width="28.83203125" customWidth="1"/>
     <col min="12" max="12" width="18.83203125" style="18" customWidth="1"/>
     <col min="13" max="13" width="22.1640625" customWidth="1"/>
-    <col min="14" max="14" width="3.1640625" customWidth="1"/>
+    <col min="14" max="14" width="10.6640625" customWidth="1"/>
     <col min="15" max="15" width="21.83203125" customWidth="1"/>
     <col min="16" max="16" width="0.5" hidden="1" customWidth="1"/>
     <col min="17" max="17" width="10.33203125" hidden="1" customWidth="1"/>
@@ -19878,7 +19875,7 @@
       <c r="Z271" s="3"/>
       <c r="AA271" s="3"/>
     </row>
-    <row r="272" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A272" s="1" t="s">
         <v>838</v>
       </c>
@@ -19925,7 +19922,7 @@
         <v>72.2</v>
       </c>
     </row>
-    <row r="273" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A273" s="3" t="s">
         <v>843</v>
       </c>
@@ -19980,7 +19977,7 @@
       <c r="Z273" s="3"/>
       <c r="AA273" s="3"/>
     </row>
-    <row r="274" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A274" s="1" t="s">
         <v>845</v>
       </c>
@@ -20024,7 +20021,7 @@
         <v>70.2</v>
       </c>
     </row>
-    <row r="275" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A275" s="3" t="s">
         <v>847</v>
       </c>
@@ -20081,7 +20078,7 @@
       <c r="Z275" s="3"/>
       <c r="AA275" s="3"/>
     </row>
-    <row r="276" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A276" s="1" t="s">
         <v>848</v>
       </c>
@@ -20128,8 +20125,8 @@
         <v>71.7</v>
       </c>
     </row>
-    <row r="277" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A277" s="3" t="s">
+    <row r="277" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A277" s="49" t="s">
         <v>850</v>
       </c>
       <c r="B277" s="3">
@@ -20183,8 +20180,8 @@
       <c r="Z277" s="3"/>
       <c r="AA277" s="3"/>
     </row>
-    <row r="278" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A278" s="1" t="s">
+    <row r="278" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A278" s="50" t="s">
         <v>853</v>
       </c>
       <c r="B278" s="1">
@@ -20227,7 +20224,7 @@
         <v>1386</v>
       </c>
     </row>
-    <row r="279" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A279" s="3" t="s">
         <v>854</v>
       </c>
@@ -20288,7 +20285,7 @@
       <c r="Z279" s="3"/>
       <c r="AA279" s="3"/>
     </row>
-    <row r="280" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A280" s="1" t="s">
         <v>855</v>
       </c>
@@ -20332,7 +20329,7 @@
         <v>80.400000000000006</v>
       </c>
     </row>
-    <row r="281" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A281" s="3" t="s">
         <v>856</v>
       </c>
@@ -20387,7 +20384,7 @@
       <c r="Z281" s="3"/>
       <c r="AA281" s="3"/>
     </row>
-    <row r="282" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A282" s="1" t="s">
         <v>857</v>
       </c>
@@ -20448,7 +20445,7 @@
         <v>1464</v>
       </c>
     </row>
-    <row r="283" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A283" s="3" t="s">
         <v>858</v>
       </c>
@@ -20505,7 +20502,7 @@
       <c r="Z283" s="3"/>
       <c r="AA283" s="3"/>
     </row>
-    <row r="284" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A284" s="1" t="s">
         <v>860</v>
       </c>
@@ -20549,7 +20546,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="285" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A285" s="3" t="s">
         <v>862</v>
       </c>
@@ -20604,7 +20601,7 @@
       <c r="Z285" s="3"/>
       <c r="AA285" s="3"/>
     </row>
-    <row r="286" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A286" s="1" t="s">
         <v>864</v>
       </c>
@@ -20648,7 +20645,7 @@
         <v>117.4</v>
       </c>
     </row>
-    <row r="287" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A287" s="3" t="s">
         <v>867</v>
       </c>
@@ -20703,7 +20700,7 @@
       <c r="Z287" s="3"/>
       <c r="AA287" s="3"/>
     </row>
-    <row r="288" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A288" s="1" t="s">
         <v>868</v>
       </c>
@@ -20747,7 +20744,7 @@
         <v>66.5</v>
       </c>
     </row>
-    <row r="289" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A289" s="3" t="s">
         <v>870</v>
       </c>
@@ -20802,7 +20799,7 @@
       <c r="Z289" s="3"/>
       <c r="AA289" s="3"/>
     </row>
-    <row r="290" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A290" s="1" t="s">
         <v>871</v>
       </c>
@@ -20846,7 +20843,7 @@
         <v>83.6</v>
       </c>
     </row>
-    <row r="291" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A291" s="3" t="s">
         <v>873</v>
       </c>
@@ -20907,7 +20904,7 @@
       <c r="Z291" s="3"/>
       <c r="AA291" s="3"/>
     </row>
-    <row r="292" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A292" s="1" t="s">
         <v>874</v>
       </c>
@@ -20954,7 +20951,7 @@
         <v>1386</v>
       </c>
     </row>
-    <row r="293" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A293" s="3" t="s">
         <v>875</v>
       </c>
@@ -21009,7 +21006,7 @@
       <c r="Z293" s="3"/>
       <c r="AA293" s="3"/>
     </row>
-    <row r="294" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A294" s="1" t="s">
         <v>878</v>
       </c>
@@ -21056,7 +21053,7 @@
         <v>1386</v>
       </c>
     </row>
-    <row r="295" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A295" s="3" t="s">
         <v>880</v>
       </c>
@@ -21111,7 +21108,7 @@
       <c r="Z295" s="3"/>
       <c r="AA295" s="3"/>
     </row>
-    <row r="296" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A296" s="1" t="s">
         <v>882</v>
       </c>
@@ -21155,7 +21152,7 @@
         <v>114.9</v>
       </c>
     </row>
-    <row r="297" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A297" s="3" t="s">
         <v>883</v>
       </c>
@@ -21210,7 +21207,7 @@
       <c r="Z297" s="3"/>
       <c r="AA297" s="3"/>
     </row>
-    <row r="298" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A298" s="1" t="s">
         <v>884</v>
       </c>
@@ -21254,7 +21251,7 @@
         <v>125.1</v>
       </c>
     </row>
-    <row r="299" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A299" s="3" t="s">
         <v>885</v>
       </c>
@@ -21311,7 +21308,7 @@
         <v>1463</v>
       </c>
     </row>
-    <row r="300" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A300" s="1" t="s">
         <v>886</v>
       </c>
@@ -21355,7 +21352,7 @@
         <v>68.8</v>
       </c>
     </row>
-    <row r="301" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A301" s="3" t="s">
         <v>888</v>
       </c>
@@ -21414,7 +21411,7 @@
       <c r="Z301" s="3"/>
       <c r="AA301" s="3"/>
     </row>
-    <row r="302" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A302" s="1" t="s">
         <v>890</v>
       </c>
@@ -21458,7 +21455,7 @@
         <v>51.5</v>
       </c>
     </row>
-    <row r="303" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A303" s="3" t="s">
         <v>892</v>
       </c>
@@ -21513,7 +21510,7 @@
       <c r="Z303" s="3"/>
       <c r="AA303" s="3"/>
     </row>
-    <row r="304" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A304" s="1" t="s">
         <v>893</v>
       </c>
@@ -21557,7 +21554,7 @@
         <v>78.099999999999994</v>
       </c>
     </row>
-    <row r="305" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A305" s="3" t="s">
         <v>896</v>
       </c>
@@ -21612,7 +21609,7 @@
       <c r="Z305" s="3"/>
       <c r="AA305" s="3"/>
     </row>
-    <row r="306" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="306" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A306" s="1" t="s">
         <v>898</v>
       </c>
@@ -21656,7 +21653,7 @@
         <v>90.7</v>
       </c>
     </row>
-    <row r="307" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="307" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A307" s="3" t="s">
         <v>899</v>
       </c>
@@ -21711,7 +21708,7 @@
       <c r="Z307" s="3"/>
       <c r="AA307" s="3"/>
     </row>
-    <row r="308" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A308" s="1" t="s">
         <v>901</v>
       </c>
@@ -21755,7 +21752,7 @@
         <v>70.2</v>
       </c>
     </row>
-    <row r="309" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="309" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A309" s="3" t="s">
         <v>902</v>
       </c>
@@ -21810,7 +21807,7 @@
       <c r="Z309" s="3"/>
       <c r="AA309" s="3"/>
     </row>
-    <row r="310" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="310" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A310" s="1" t="s">
         <v>903</v>
       </c>
@@ -21854,7 +21851,7 @@
         <v>85.4</v>
       </c>
     </row>
-    <row r="311" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A311" s="3" t="s">
         <v>904</v>
       </c>
@@ -21909,7 +21906,7 @@
       <c r="Z311" s="3"/>
       <c r="AA311" s="3"/>
     </row>
-    <row r="312" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="312" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A312" s="1" t="s">
         <v>905</v>
       </c>
@@ -21953,7 +21950,7 @@
         <v>96.4</v>
       </c>
     </row>
-    <row r="313" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="313" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A313" s="3" t="s">
         <v>906</v>
       </c>
@@ -22008,7 +22005,7 @@
       <c r="Z313" s="3"/>
       <c r="AA313" s="3"/>
     </row>
-    <row r="314" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="314" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A314" s="1" t="s">
         <v>908</v>
       </c>
@@ -22052,7 +22049,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="315" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="315" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A315" s="3" t="s">
         <v>909</v>
       </c>
@@ -22107,7 +22104,7 @@
       <c r="Z315" s="3"/>
       <c r="AA315" s="3"/>
     </row>
-    <row r="316" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="316" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A316" s="1" t="s">
         <v>912</v>
       </c>
@@ -22154,7 +22151,7 @@
         <v>1462</v>
       </c>
     </row>
-    <row r="317" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="317" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A317" s="3" t="s">
         <v>914</v>
       </c>
@@ -22209,7 +22206,7 @@
       <c r="Z317" s="3"/>
       <c r="AA317" s="3"/>
     </row>
-    <row r="318" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="318" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A318" s="1" t="s">
         <v>915</v>
       </c>
@@ -22253,7 +22250,7 @@
         <v>86.6</v>
       </c>
     </row>
-    <row r="319" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="319" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A319" s="3" t="s">
         <v>917</v>
       </c>
@@ -22308,7 +22305,7 @@
       <c r="Z319" s="3"/>
       <c r="AA319" s="3"/>
     </row>
-    <row r="320" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="320" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A320" s="1" t="s">
         <v>919</v>
       </c>
@@ -22365,7 +22362,7 @@
       <c r="Z320" s="30"/>
       <c r="AA320" s="30"/>
     </row>
-    <row r="321" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="321" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A321" s="3" t="s">
         <v>921</v>
       </c>
@@ -22420,7 +22417,7 @@
       <c r="Z321" s="3"/>
       <c r="AA321" s="3"/>
     </row>
-    <row r="322" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A322" s="1" t="s">
         <v>922</v>
       </c>
@@ -22464,7 +22461,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="323" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="323" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A323" s="3" t="s">
         <v>923</v>
       </c>
@@ -22519,7 +22516,7 @@
       <c r="Z323" s="3"/>
       <c r="AA323" s="3"/>
     </row>
-    <row r="324" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="324" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A324" s="1" t="s">
         <v>924</v>
       </c>
@@ -22563,7 +22560,7 @@
         <v>58.8</v>
       </c>
     </row>
-    <row r="325" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="325" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A325" s="3" t="s">
         <v>925</v>
       </c>
@@ -22618,7 +22615,7 @@
       <c r="Z325" s="3"/>
       <c r="AA325" s="3"/>
     </row>
-    <row r="326" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="326" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A326" s="1" t="s">
         <v>926</v>
       </c>
@@ -22662,7 +22659,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="327" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="327" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A327" s="3" t="s">
         <v>927</v>
       </c>
@@ -22717,7 +22714,7 @@
       <c r="Z327" s="3"/>
       <c r="AA327" s="3"/>
     </row>
-    <row r="328" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="328" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A328" s="1" t="s">
         <v>928</v>
       </c>
@@ -22764,7 +22761,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="329" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="329" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A329" s="3" t="s">
         <v>930</v>
       </c>
@@ -22819,7 +22816,7 @@
       <c r="Z329" s="3"/>
       <c r="AA329" s="3"/>
     </row>
-    <row r="330" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="330" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A330" s="1" t="s">
         <v>931</v>
       </c>
@@ -22863,7 +22860,7 @@
         <v>91.4</v>
       </c>
     </row>
-    <row r="331" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="331" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A331" s="3" t="s">
         <v>932</v>
       </c>
@@ -22918,7 +22915,7 @@
       <c r="Z331" s="3"/>
       <c r="AA331" s="3"/>
     </row>
-    <row r="332" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="332" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A332" s="1" t="s">
         <v>934</v>
       </c>
@@ -22975,7 +22972,7 @@
       <c r="Z332" s="30"/>
       <c r="AA332" s="30"/>
     </row>
-    <row r="333" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="333" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A333" s="3" t="s">
         <v>935</v>
       </c>
@@ -23034,7 +23031,7 @@
       <c r="Z333" s="30"/>
       <c r="AA333" s="30"/>
     </row>
-    <row r="334" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="334" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A334" s="1" t="s">
         <v>937</v>
       </c>
@@ -23091,7 +23088,7 @@
       <c r="Z334" s="30"/>
       <c r="AA334" s="30"/>
     </row>
-    <row r="335" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="335" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A335" s="3" t="s">
         <v>939</v>
       </c>
@@ -23146,7 +23143,7 @@
       <c r="Z335" s="3"/>
       <c r="AA335" s="3"/>
     </row>
-    <row r="336" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="336" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A336" s="1" t="s">
         <v>940</v>
       </c>
@@ -23190,7 +23187,7 @@
         <v>87.7</v>
       </c>
     </row>
-    <row r="337" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="337" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A337" s="3" t="s">
         <v>941</v>
       </c>
@@ -23251,7 +23248,7 @@
       <c r="Z337" s="30"/>
       <c r="AA337" s="30"/>
     </row>
-    <row r="338" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="338" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A338" s="1" t="s">
         <v>943</v>
       </c>
@@ -23295,7 +23292,7 @@
         <v>71.7</v>
       </c>
     </row>
-    <row r="339" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="339" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A339" s="3" t="s">
         <v>945</v>
       </c>
@@ -23354,7 +23351,7 @@
       <c r="Z339" s="30"/>
       <c r="AA339" s="30"/>
     </row>
-    <row r="340" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="340" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A340" s="1" t="s">
         <v>946</v>
       </c>
@@ -23398,7 +23395,7 @@
         <v>64.3</v>
       </c>
     </row>
-    <row r="341" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="341" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A341" s="3" t="s">
         <v>947</v>
       </c>
@@ -23453,7 +23450,7 @@
       <c r="Z341" s="3"/>
       <c r="AA341" s="3"/>
     </row>
-    <row r="342" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="342" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A342" s="1" t="s">
         <v>948</v>
       </c>
@@ -23497,7 +23494,7 @@
         <v>87.4</v>
       </c>
     </row>
-    <row r="343" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="343" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A343" s="3" t="s">
         <v>950</v>
       </c>
@@ -23552,7 +23549,7 @@
       <c r="Z343" s="3"/>
       <c r="AA343" s="3"/>
     </row>
-    <row r="344" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="344" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A344" s="1" t="s">
         <v>952</v>
       </c>
@@ -23596,7 +23593,7 @@
         <v>106.6</v>
       </c>
     </row>
-    <row r="345" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="345" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A345" s="3" t="s">
         <v>954</v>
       </c>
@@ -23651,7 +23648,7 @@
       <c r="Z345" s="3"/>
       <c r="AA345" s="3"/>
     </row>
-    <row r="346" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="346" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A346" s="1" t="s">
         <v>956</v>
       </c>
@@ -23708,7 +23705,7 @@
       <c r="Z346" s="30"/>
       <c r="AA346" s="30"/>
     </row>
-    <row r="347" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="347" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A347" s="3" t="s">
         <v>959</v>
       </c>
@@ -23763,7 +23760,7 @@
       <c r="Z347" s="3"/>
       <c r="AA347" s="3"/>
     </row>
-    <row r="348" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="348" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A348" s="1" t="s">
         <v>962</v>
       </c>
@@ -23807,7 +23804,7 @@
         <v>91.9</v>
       </c>
     </row>
-    <row r="349" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="349" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A349" s="3" t="s">
         <v>964</v>
       </c>
@@ -23862,7 +23859,7 @@
       <c r="Z349" s="3"/>
       <c r="AA349" s="3"/>
     </row>
-    <row r="350" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="350" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A350" s="1" t="s">
         <v>965</v>
       </c>
@@ -23909,7 +23906,7 @@
         <v>71.8</v>
       </c>
     </row>
-    <row r="351" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="351" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A351" s="3" t="s">
         <v>967</v>
       </c>
@@ -23964,7 +23961,7 @@
       <c r="Z351" s="3"/>
       <c r="AA351" s="3"/>
     </row>
-    <row r="352" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="352" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A352" s="1" t="s">
         <v>969</v>
       </c>
@@ -24008,7 +24005,7 @@
         <v>84.1</v>
       </c>
     </row>
-    <row r="353" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="353" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A353" s="3" t="s">
         <v>971</v>
       </c>
@@ -24062,7 +24059,7 @@
       <c r="Z353" s="3"/>
       <c r="AA353" s="3"/>
     </row>
-    <row r="354" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="354" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A354" s="1" t="s">
         <v>972</v>
       </c>
@@ -24106,7 +24103,7 @@
         <v>82.9</v>
       </c>
     </row>
-    <row r="355" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="355" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A355" s="3" t="s">
         <v>974</v>
       </c>
@@ -24163,7 +24160,7 @@
       <c r="Z355" s="3"/>
       <c r="AA355" s="3"/>
     </row>
-    <row r="356" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="356" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A356" s="1" t="s">
         <v>976</v>
       </c>
@@ -24220,7 +24217,7 @@
       <c r="Z356" s="30"/>
       <c r="AA356" s="30"/>
     </row>
-    <row r="357" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="357" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A357" s="3" t="s">
         <v>977</v>
       </c>
@@ -24275,7 +24272,7 @@
       <c r="Z357" s="3"/>
       <c r="AA357" s="3"/>
     </row>
-    <row r="358" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="358" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A358" s="1" t="s">
         <v>979</v>
       </c>
@@ -24319,7 +24316,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="359" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="359" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A359" s="3" t="s">
         <v>980</v>
       </c>
@@ -24374,7 +24371,7 @@
       <c r="Z359" s="3"/>
       <c r="AA359" s="3"/>
     </row>
-    <row r="360" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="360" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A360" s="1" t="s">
         <v>982</v>
       </c>
@@ -24418,7 +24415,7 @@
         <v>119.4</v>
       </c>
     </row>
-    <row r="361" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="361" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A361" s="3" t="s">
         <v>983</v>
       </c>
@@ -34231,7 +34228,7 @@
       <c r="Z541" s="3"/>
       <c r="AA541" s="3"/>
     </row>
-    <row r="542" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="542" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A542" s="1" t="s">
         <v>1261</v>
       </c>
@@ -34278,7 +34275,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="543" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="543" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A543" s="3" t="s">
         <v>1264</v>
       </c>
@@ -34335,7 +34332,7 @@
       <c r="Z543" s="3"/>
       <c r="AA543" s="3"/>
     </row>
-    <row r="544" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="544" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A544" s="1" t="s">
         <v>1265</v>
       </c>
@@ -34382,7 +34379,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="545" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="545" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A545" s="3" t="s">
         <v>1266</v>
       </c>
@@ -34439,7 +34436,7 @@
       <c r="Z545" s="3"/>
       <c r="AA545" s="3"/>
     </row>
-    <row r="546" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="546" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A546" s="1" t="s">
         <v>1267</v>
       </c>
@@ -35011,7 +35008,7 @@
       </c>
       <c r="Z556" s="15"/>
     </row>
-    <row r="557" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="557" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A557" s="3" t="s">
         <v>1283</v>
       </c>
@@ -35068,7 +35065,7 @@
       <c r="Z557" s="15"/>
       <c r="AA557" s="3"/>
     </row>
-    <row r="558" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="558" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A558" s="1" t="s">
         <v>1284</v>
       </c>
@@ -35116,7 +35113,7 @@
       </c>
       <c r="Z558" s="15"/>
     </row>
-    <row r="559" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="559" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A559" s="3" t="s">
         <v>1286</v>
       </c>
@@ -35173,7 +35170,7 @@
       <c r="Z559" s="15"/>
       <c r="AA559" s="3"/>
     </row>
-    <row r="560" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="560" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A560" s="1" t="s">
         <v>1287</v>
       </c>
@@ -35221,7 +35218,7 @@
       </c>
       <c r="Z560" s="15"/>
     </row>
-    <row r="561" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="561" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A561" s="3" t="s">
         <v>1288</v>
       </c>
@@ -35803,7 +35800,7 @@
       <c r="Z571" s="15"/>
       <c r="AA571" s="3"/>
     </row>
-    <row r="572" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="572" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A572" s="1" t="s">
         <v>1306</v>
       </c>
@@ -35851,7 +35848,7 @@
       </c>
       <c r="Z572" s="15"/>
     </row>
-    <row r="573" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="573" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A573" s="3" t="s">
         <v>1308</v>
       </c>
@@ -35906,7 +35903,7 @@
       <c r="Z573" s="15"/>
       <c r="AA573" s="3"/>
     </row>
-    <row r="574" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="574" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A574" s="1" t="s">
         <v>1310</v>
       </c>
@@ -35954,7 +35951,7 @@
       </c>
       <c r="Z574" s="15"/>
     </row>
-    <row r="575" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="575" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A575" s="3" t="s">
         <v>1311</v>
       </c>
@@ -36011,7 +36008,7 @@
       <c r="Z575" s="15"/>
       <c r="AA575" s="3"/>
     </row>
-    <row r="576" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="576" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A576" s="1" t="s">
         <v>1312</v>
       </c>
@@ -36584,7 +36581,7 @@
       </c>
       <c r="Z586" s="15"/>
     </row>
-    <row r="587" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="587" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A587" s="3" t="s">
         <v>1327</v>
       </c>
@@ -36641,7 +36638,7 @@
       <c r="Z587" s="15"/>
       <c r="AA587" s="3"/>
     </row>
-    <row r="588" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="588" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A588" s="1" t="s">
         <v>1328</v>
       </c>
@@ -36689,7 +36686,7 @@
       </c>
       <c r="Z588" s="15"/>
     </row>
-    <row r="589" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="589" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A589" s="3" t="s">
         <v>1329</v>
       </c>
@@ -36746,7 +36743,7 @@
       <c r="Z589" s="15"/>
       <c r="AA589" s="3"/>
     </row>
-    <row r="590" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="590" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A590" s="1" t="s">
         <v>1330</v>
       </c>
@@ -36794,7 +36791,7 @@
       </c>
       <c r="Z590" s="15"/>
     </row>
-    <row r="591" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="591" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A591" s="3" t="s">
         <v>1331</v>
       </c>
@@ -37374,7 +37371,7 @@
       <c r="Z601" s="15"/>
       <c r="AA601" s="3"/>
     </row>
-    <row r="602" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="602" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A602" s="1" t="s">
         <v>1347</v>
       </c>
@@ -37422,7 +37419,7 @@
       </c>
       <c r="Z602" s="15"/>
     </row>
-    <row r="603" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="603" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A603" s="3" t="s">
         <v>1348</v>
       </c>
@@ -37479,7 +37476,7 @@
       <c r="Z603" s="15"/>
       <c r="AA603" s="3"/>
     </row>
-    <row r="604" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="604" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A604" s="1" t="s">
         <v>1349</v>
       </c>
@@ -37527,7 +37524,7 @@
       </c>
       <c r="Z604" s="15"/>
     </row>
-    <row r="605" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="605" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A605" s="3" t="s">
         <v>1350</v>
       </c>
@@ -37584,7 +37581,7 @@
       <c r="Z605" s="15"/>
       <c r="AA605" s="3"/>
     </row>
-    <row r="606" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="606" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A606" s="1" t="s">
         <v>1352</v>
       </c>
@@ -38155,7 +38152,7 @@
       </c>
       <c r="Z616" s="15"/>
     </row>
-    <row r="617" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="617" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A617" s="3" t="s">
         <v>1366</v>
       </c>
@@ -38212,7 +38209,7 @@
       <c r="Z617" s="15"/>
       <c r="AA617" s="3"/>
     </row>
-    <row r="618" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="618" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A618" s="1" t="s">
         <v>1368</v>
       </c>
@@ -38260,7 +38257,7 @@
       </c>
       <c r="Z618" s="15"/>
     </row>
-    <row r="619" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="619" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A619" s="3" t="s">
         <v>1369</v>
       </c>
@@ -38317,7 +38314,7 @@
       <c r="Z619" s="15"/>
       <c r="AA619" s="3"/>
     </row>
-    <row r="620" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="620" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A620" s="1" t="s">
         <v>1370</v>
       </c>
@@ -38365,7 +38362,7 @@
       </c>
       <c r="Z620" s="15"/>
     </row>
-    <row r="621" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="621" spans="1:27" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A621" s="3" t="s">
         <v>1371</v>
       </c>

</xml_diff>

<commit_message>
updated comment for 2 pobas cc b2 height fall 2025
</commit_message>
<xml_diff>
--- a/data/treeMeasurements/TreeMeasurements.xlsx
+++ b/data/treeMeasurements/TreeMeasurements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christophe_rouleau-desrochers/github/fuelinex/data/treeMeasurements/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0809BE55-2DC8-DE49-904D-C1C2604678FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B4B0F82-4245-1648-99CF-5A949B59BCD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34620" yWindow="-1200" windowWidth="29400" windowHeight="18380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4783" uniqueCount="1465">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4785" uniqueCount="1466">
   <si>
     <t>tree_ID</t>
   </si>
@@ -4431,6 +4431,9 @@
   </si>
   <si>
     <t>the second shoot mentioned last year died</t>
+  </si>
+  <si>
+    <t>check shoot elongation if stopped at some point and add the max elongation value to the height of last year</t>
   </si>
 </sst>
 </file>
@@ -4705,8 +4708,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5591,8 +5594,8 @@
   <dimension ref="A1:AA820"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="167" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="O1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="V355" sqref="V355"/>
+      <pane xSplit="1" topLeftCell="Y1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A277" sqref="A277"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -20178,7 +20181,9 @@
       <c r="X277" s="3"/>
       <c r="Y277" s="3"/>
       <c r="Z277" s="3"/>
-      <c r="AA277" s="3"/>
+      <c r="AA277" s="3" t="s">
+        <v>1465</v>
+      </c>
     </row>
     <row r="278" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A278" s="50" t="s">
@@ -20222,6 +20227,9 @@
       </c>
       <c r="V278" s="46" t="s">
         <v>1386</v>
+      </c>
+      <c r="AA278" t="s">
+        <v>1465</v>
       </c>
     </row>
     <row r="279" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>